<commit_message>
Reported issues #51, #52, #53, #54, #55 and #56
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA05044-DDA4-4C95-8748-BFD6E06F1CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBD7DF0-3E8E-44D6-95A7-DCBD0B97443E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27960" windowHeight="18240" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27960" windowHeight="18240" tabRatio="693" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Run 20200811" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="280">
   <si>
     <t>Scenario</t>
   </si>
@@ -1204,6 +1204,9 @@
   </si>
   <si>
     <t>To "Valid Given" belongs helper function CreateValidGiven, this should be renamed to CreateRenamedValidGiven, instead a call to MakeRenamedValidGiven is created (with no comment and no helper function</t>
+  </si>
+  <si>
+    <t>Issue 2</t>
   </si>
 </sst>
 </file>
@@ -1720,12 +1723,15 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
+  <dxfs count="84">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1753,12 +1759,59 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="164" formatCode="0000"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1766,6 +1819,34 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1789,6 +1870,21 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i/>
         <strike val="0"/>
@@ -1808,13 +1904,71 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0000"/>
@@ -1824,6 +1978,41 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1868,6 +2057,203 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1929,386 +2315,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2323,122 +2329,119 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="A1:F19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="75"/>
+    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="73">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="77">
+    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="72">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="76"/>
-    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:F21" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="70">
+    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="62">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="69">
+    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="61">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:G60" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
-  <autoFilter ref="A1:G60" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F60">
-    <sortCondition ref="A2:A60"/>
-    <sortCondition ref="B2:B60"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H60" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A1:H60" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="51">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="61">
+    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="50">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:F3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="39">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K344" totalsRowCount="1" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K344" totalsRowCount="1" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:K343" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K149">
     <sortCondition ref="B3:B149"/>
     <sortCondition ref="I3:I149"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="55" totalsRowDxfId="15">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="54" totalsRowDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="53" totalsRowDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="52" totalsRowDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="11">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="50" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="49" totalsRowDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="48" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="47" totalsRowDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="46" totalsRowDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="45" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="8" totalsRowDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:E7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3119,24 +3122,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E20:E1048576 E1:E17">
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3635,13 +3638,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3655,10 +3658,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E210D12-4685-43CE-97DA-E3A60E5FBE1A}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,7 +3675,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3694,8 +3697,11 @@
       <c r="G1" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>27</v>
       </c>
@@ -3715,7 +3721,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>27</v>
       </c>
@@ -3735,7 +3741,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>27</v>
       </c>
@@ -3755,7 +3761,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>27</v>
       </c>
@@ -3775,7 +3781,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>27</v>
       </c>
@@ -3795,7 +3801,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>27</v>
       </c>
@@ -3815,7 +3821,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>27</v>
       </c>
@@ -3836,8 +3842,11 @@
       <c r="F8" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="89">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>27</v>
       </c>
@@ -3858,8 +3867,11 @@
       <c r="F9" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="89">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>27</v>
       </c>
@@ -3879,7 +3891,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>27</v>
       </c>
@@ -3899,7 +3911,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>27</v>
       </c>
@@ -3919,7 +3931,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>27</v>
       </c>
@@ -3939,7 +3951,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>27</v>
       </c>
@@ -3959,7 +3971,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>27</v>
       </c>
@@ -3979,7 +3991,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>28</v>
       </c>
@@ -3999,7 +4011,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>28</v>
       </c>
@@ -4019,7 +4031,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>28</v>
       </c>
@@ -4040,8 +4052,14 @@
       <c r="F18" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="89">
+        <v>53</v>
+      </c>
+      <c r="H18" s="89">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>28</v>
       </c>
@@ -4061,7 +4079,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>28</v>
       </c>
@@ -4082,8 +4100,14 @@
       <c r="F20" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="89">
+        <v>53</v>
+      </c>
+      <c r="H20" s="89">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>28</v>
       </c>
@@ -4103,7 +4127,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>28</v>
       </c>
@@ -4123,7 +4147,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>28</v>
       </c>
@@ -4143,7 +4167,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>28</v>
       </c>
@@ -4163,7 +4187,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>28</v>
       </c>
@@ -4184,8 +4208,11 @@
       <c r="F25" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="89">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>28</v>
       </c>
@@ -4205,7 +4232,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -4225,7 +4252,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -4246,8 +4273,11 @@
       <c r="F28" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4268,8 +4298,11 @@
       <c r="F29" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4290,8 +4323,11 @@
       <c r="F30" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -4312,8 +4348,11 @@
       <c r="F31" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -4759,6 +4798,9 @@
       <c r="F52" s="2" t="s">
         <v>236</v>
       </c>
+      <c r="G52" s="89">
+        <v>56</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -4800,6 +4842,9 @@
       </c>
       <c r="F54" s="2" t="s">
         <v>244</v>
+      </c>
+      <c r="G54" s="89">
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4943,13 +4988,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4960,11 +5005,24 @@
     <hyperlink ref="G55" r:id="rId4" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/44" xr:uid="{74FACEB3-F86D-4741-BE6E-4FD01661A61C}"/>
     <hyperlink ref="G45" r:id="rId5" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/51" xr:uid="{165016DB-6686-4CB4-978C-5177C03FF3B3}"/>
     <hyperlink ref="G50" r:id="rId6" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/51" xr:uid="{3882B1E2-5655-4B19-9E4B-C13542F60BC0}"/>
+    <hyperlink ref="G8" r:id="rId7" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/52" xr:uid="{5D54C956-00A4-4983-92AB-A74B21732150}"/>
+    <hyperlink ref="G9" r:id="rId8" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/52" xr:uid="{337F053B-11D9-4EBF-BE53-5B87B552EA11}"/>
+    <hyperlink ref="G18" r:id="rId9" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/53" xr:uid="{4A7B03B2-1DE5-4EBE-A93D-9CFFBEF25C5D}"/>
+    <hyperlink ref="G20" r:id="rId10" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/53" xr:uid="{5D17D4C3-1744-4023-B0F5-CBE273A52FC2}"/>
+    <hyperlink ref="G25" r:id="rId11" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/53" xr:uid="{FBF559D7-CF62-44F6-93E0-1C29D885D000}"/>
+    <hyperlink ref="H18" r:id="rId12" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/54" xr:uid="{C38BF5EE-7464-48F0-85D4-D59D8C250A9B}"/>
+    <hyperlink ref="H20" r:id="rId13" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/54" xr:uid="{07C47D43-B01C-449C-94C4-63F323B45E68}"/>
+    <hyperlink ref="G28" r:id="rId14" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{2FFBFEE6-6C93-4A6B-8BE9-38773F862480}"/>
+    <hyperlink ref="G29" r:id="rId15" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{84F77E47-34AF-4356-A3F2-BFFEF83B06F8}"/>
+    <hyperlink ref="G30" r:id="rId16" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{EADA9EEF-8698-4BC4-9A0D-A234BBCAF4E2}"/>
+    <hyperlink ref="G31" r:id="rId17" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{497802EF-D2E8-44D9-B316-96E248D498C2}"/>
+    <hyperlink ref="G52" r:id="rId18" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/56" xr:uid="{BE77F74A-0CD4-44AC-ADC2-9F3DA951450A}"/>
+    <hyperlink ref="G54" r:id="rId19" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/56" xr:uid="{821E4586-1080-416B-9C72-1E56D3FF443A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5062,13 +5120,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5084,7 +5142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
   <dimension ref="A1:K344"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J318" sqref="J318"/>
     </sheetView>
   </sheetViews>
@@ -15074,12 +15132,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15108,13 +15166,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Tested #54 and OK
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CE1259-50C7-49D2-832E-5C5E8B7CC934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C055BF-860C-4C30-A5AD-390503F6EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="693" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="693" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Run 20200811" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="300">
   <si>
     <t>Scenario</t>
   </si>
@@ -1254,6 +1254,41 @@
   <si>
     <t>All tests that reside in the test project are displayed with right feature, ID and scenario</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1) "Valid Given" is not removed from ATDD.TestScriptor page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+(2) ATDD.TestScriptor page does no longer show Scenario</t>
+    </r>
+  </si>
+  <si>
+    <t>Has been solved.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Solved</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
 </sst>
 </file>
 
@@ -1262,7 +1297,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1407,8 +1442,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1456,8 +1498,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1493,13 +1541,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1790,13 +1886,64 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2019,274 +2166,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2321,6 +2200,9 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2332,6 +2214,271 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2461,140 +2608,141 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
   <autoFilter ref="A1:F19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="93"/>
-    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="91">
+    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="95">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="90">
+    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="94">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="89"/>
-    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="93"/>
+    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
   <autoFilter ref="A1:F21" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="83">
+    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="87">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="82">
+    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="86">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="81"/>
-    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="85"/>
+    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H60" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H60" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:H60" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="77"/>
-    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="75">
+    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="81"/>
+    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="79">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="74">
+    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="78">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="A1:F3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="69">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="64">
+    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="68">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="67"/>
+    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G5" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
-  <autoFilter ref="A1:G5" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+  <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="61">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K354" totalsRowCount="1" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K354" totalsRowCount="1" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A1:K353" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K153">
     <sortCondition ref="B7:B153"/>
     <sortCondition ref="I7:I153"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="44" totalsRowDxfId="33">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="54" totalsRowDxfId="53">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="43" totalsRowDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="42" totalsRowDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="41" totalsRowDxfId="30"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="29">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="45">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="39" totalsRowDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="38" totalsRowDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="37" totalsRowDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="36" totalsRowDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="35" totalsRowDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="34" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="34" totalsRowDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0" dataDxfId="59">
-  <autoFilter ref="A1:E7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="32">
+  <autoFilter ref="A1:F7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3274,24 +3422,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E20:E1048576 E1:E17">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3790,13 +3938,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3812,7 +3960,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E210D12-4685-43CE-97DA-E3A60E5FBE1A}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5138,13 +5288,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5270,13 +5420,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5290,10 +5440,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A07736E-642F-4113-870C-47BFB0737DE7}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5307,7 +5457,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -5330,7 +5480,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>28</v>
       </c>
@@ -5353,7 +5503,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>28</v>
       </c>
@@ -5376,7 +5526,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>28</v>
       </c>
@@ -5399,7 +5549,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>28</v>
       </c>
@@ -5422,9 +5572,61 @@
         <v>55</v>
       </c>
     </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="98">
+        <v>28</v>
+      </c>
+      <c r="B6" s="99">
+        <v>30</v>
+      </c>
+      <c r="C6" s="65" t="str">
+        <f>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Given</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Remove Given step 3a</v>
+      </c>
+      <c r="E6" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>295</v>
+      </c>
+      <c r="G6" s="102">
+        <v>54</v>
+      </c>
+      <c r="H6"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="103">
+        <v>28</v>
+      </c>
+      <c r="B7" s="9">
+        <v>32</v>
+      </c>
+      <c r="C7" s="65" t="str">
+        <f>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Given</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Remove Given step 3b</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G7" s="89">
+        <v>54</v>
+      </c>
+      <c r="H7"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5436,14 +5638,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A7">
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -5451,11 +5665,13 @@
     <hyperlink ref="G3" r:id="rId2" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{5442411F-8EDF-4E91-BF6B-AB942DC06AE6}"/>
     <hyperlink ref="G4" r:id="rId3" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{6EDE31A8-2EA5-4AF1-84D1-0445317CA29D}"/>
     <hyperlink ref="G5" r:id="rId4" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/55" xr:uid="{667E6963-BF02-4732-AE57-8AA0636981DA}"/>
+    <hyperlink ref="G6" r:id="rId5" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/54" xr:uid="{C8B5AE43-0E5B-458F-8B5E-67E41BE44DA9}"/>
+    <hyperlink ref="G7" r:id="rId6" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/54" xr:uid="{64D8C3C8-555F-42A7-8E9B-3866C59C5D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5464,7 +5680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
   <dimension ref="A1:K354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B224" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -11954,7 +12170,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A225" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>28</v>
@@ -11980,7 +12196,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="226" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A226" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>28</v>
@@ -12011,7 +12227,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A227" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>28</v>
@@ -12041,7 +12257,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A228" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>28</v>
@@ -12069,7 +12285,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A229" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>29</v>
@@ -12097,7 +12313,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A230" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>29</v>
@@ -12128,7 +12344,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="231" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A231" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>29</v>
@@ -12158,7 +12374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A232" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>29</v>
@@ -12188,7 +12404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>30</v>
@@ -12216,7 +12432,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A234" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>30</v>
@@ -12247,7 +12463,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A235" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>30</v>
@@ -12277,7 +12493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A236" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>30</v>
@@ -12307,7 +12523,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" ht="15" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A237" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>30</v>
@@ -12337,7 +12553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A238" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>30</v>
@@ -12367,7 +12583,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>31</v>
@@ -12395,7 +12611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A240" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>31</v>
@@ -12426,7 +12642,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="241" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A241" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>31</v>
@@ -12456,7 +12672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A242" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>31</v>
@@ -12486,7 +12702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A243" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>32</v>
@@ -12514,7 +12730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="244" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A244" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>32</v>
@@ -12545,7 +12761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="245" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A245" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>32</v>
@@ -12575,7 +12791,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="246" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A246" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>32</v>
@@ -12605,7 +12821,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="247" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A247" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>32</v>
@@ -12635,7 +12851,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A248" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>32</v>
@@ -12665,7 +12881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A249" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12691,7 +12907,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="250" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A250" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12722,7 +12938,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A251" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12750,7 +12966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A252" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12778,7 +12994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="253" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A253" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12806,7 +13022,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A254" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12836,7 +13052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="255" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A255" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12864,7 +13080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="256" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A256" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -12892,7 +13108,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="257" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A257" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -12918,7 +13134,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A258" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -12949,7 +13165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="259" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A259" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -12977,7 +13193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="260" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A260" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -13007,7 +13223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="261" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A261" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -13035,7 +13251,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="262" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A262" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -13063,7 +13279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="263" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A263" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -13091,7 +13307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="264" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A264" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -13119,7 +13335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="265" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A265" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>40</v>
@@ -13147,7 +13363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A266" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -13173,7 +13389,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="267" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A267" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -13204,7 +13420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="268" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A268" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -13232,7 +13448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="269" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A269" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -13262,7 +13478,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="270" spans="1:11" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A270" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -13290,7 +13506,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="271" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -13318,7 +13534,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="272" spans="1:11" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="52">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>0</v>
@@ -15710,12 +15926,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15744,13 +15960,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15764,10 +15980,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB16863-C9D6-47DE-82AF-06BDE2CF5BC1}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15778,7 +15994,7 @@
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -15794,8 +16010,11 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -15809,8 +16028,11 @@
         <v>273</v>
       </c>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -15824,8 +16046,11 @@
       <c r="E3" s="89">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -15839,8 +16064,11 @@
       <c r="E4" s="89">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -15854,8 +16082,11 @@
       <c r="E5" s="89">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -15865,12 +16096,17 @@
       <c r="C6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>296</v>
+      </c>
       <c r="E6" s="89">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -15884,8 +16120,19 @@
       <c r="E7" s="89">
         <v>50</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>299</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Solved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/47" xr:uid="{7ED3BAA5-9FF9-4E61-9BCA-46B887418E89}"/>
     <hyperlink ref="E4" r:id="rId2" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/48" xr:uid="{13CE0C6E-9DA7-4EC3-B5C2-899D1E1DF82F}"/>

</xml_diff>

<commit_message>
#39 Tested and OK
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E68DA0A-9CFC-4E7C-8EE2-7119DE413875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926FD318-4029-4B85-8C6D-BF42C3DA34A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="693" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="309">
   <si>
     <t>Scenario</t>
   </si>
@@ -5845,7 +5845,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="B2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5900,6 +5900,9 @@
         <f>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</f>
         <v>Removing Scenario</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5917,6 +5920,9 @@
         <f>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</f>
         <v>Removing Scenario step 2a</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5934,6 +5940,9 @@
         <f>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</f>
         <v>Removing Scenario step 3a</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5951,6 +5960,9 @@
         <f>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</f>
         <v>Removing Scenario step 2b</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>257</v>
       </c>
@@ -5970,6 +5982,9 @@
         <f>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</f>
         <v>Removing Scenario step 3b</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5986,6 +6001,9 @@
       <c r="D7" s="1" t="str">
         <f>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</f>
         <v>Removing Scenario with initialize</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -6025,7 +6043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
   <dimension ref="A1:K364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B332" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K364" sqref="K364"/>
     </sheetView>
   </sheetViews>
@@ -15514,7 +15532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="330" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A330" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -15539,7 +15557,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="331" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A331" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -15569,7 +15587,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="332" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A332" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -15597,7 +15615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="333" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A333" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -15627,7 +15645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="334" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A334" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -15655,7 +15673,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="335" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A335" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>57</v>
@@ -15682,7 +15700,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="336" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A336" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>57</v>
@@ -15713,7 +15731,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="337" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A337" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>57</v>
@@ -15743,7 +15761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="338" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A338" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>57</v>
@@ -15773,7 +15791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="339" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A339" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -15800,7 +15818,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="340" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A340" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -15831,7 +15849,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="341" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A341" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -15861,7 +15879,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="342" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A342" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -15891,7 +15909,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="343" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A343" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -15921,7 +15939,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="344" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A344" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -15951,7 +15969,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="345" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A345" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>59</v>
@@ -15978,7 +15996,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="346" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A346" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>59</v>
@@ -16009,7 +16027,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="347" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A347" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>59</v>
@@ -16039,7 +16057,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="348" spans="1:11" s="65" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A348" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>59</v>
@@ -16069,7 +16087,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="349" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A349" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -16096,7 +16114,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="350" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A350" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -16127,7 +16145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="351" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A351" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -16157,7 +16175,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="352" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A352" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -16187,7 +16205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="353" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A353" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -16217,7 +16235,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="354" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A354" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -16247,7 +16265,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="355" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A355" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16272,7 +16290,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="356" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A356" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16302,7 +16320,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="357" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A357" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16330,7 +16348,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="358" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A358" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16358,7 +16376,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="359" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A359" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16386,7 +16404,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="360" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A360" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16414,7 +16432,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="361" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A361" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16442,7 +16460,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="362" spans="1:11" s="65" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A362" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16470,7 +16488,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="363" spans="1:11" s="65" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A363" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -16498,7 +16516,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A364" s="61"/>
       <c r="B364" s="1" t="s">
         <v>66</v>
@@ -16506,13 +16524,13 @@
       <c r="C364" s="3"/>
       <c r="E364" s="10">
         <f>Table14[[#Totals],[Scenario '#]]</f>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F364" s="6"/>
       <c r="H364" s="2"/>
       <c r="I364" s="12">
         <f>SUBTOTAL(104,Table14[Scenario '#])</f>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tested #39 and #67 and OK
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2966280A-C253-44F1-8A20-3A736214D4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025DD528-E4B5-4BB0-B1F1-77F7DADCF42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27960" windowHeight="18240" tabRatio="693" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="693" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200811" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="20201013" sheetId="9" r:id="rId7"/>
     <sheet name="20201014" sheetId="10" r:id="rId8"/>
     <sheet name="20201027" sheetId="11" r:id="rId9"/>
-    <sheet name="ATDD Scenarios" sheetId="3" r:id="rId10"/>
-    <sheet name="Questions" sheetId="2" r:id="rId11"/>
+    <sheet name="20201028" sheetId="12" r:id="rId10"/>
+    <sheet name="ATDD Scenarios" sheetId="3" r:id="rId11"/>
+    <sheet name="Questions" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="335">
   <si>
     <t>Scenario</t>
   </si>
@@ -1295,9 +1296,6 @@
     <t>Adding Scenario (to existing test codeunit)</t>
   </si>
   <si>
-    <t>Removing Scenario with initialize</t>
-  </si>
-  <si>
     <t>Test codeunit with one test function with valid Given-When-Then structure and call to Initialize</t>
   </si>
   <si>
@@ -1390,7 +1388,121 @@
     <t>Revert Rename of Then step 2</t>
   </si>
   <si>
-    <t>Duplicate Then control disappears form ATDD.TestScriptor page</t>
+    <t>Intialize helper function is not removed</t>
+  </si>
+  <si>
+    <t>See codeunit 50104 TestObjectWithUIHandlerFLX.al in AL project test-project</t>
+  </si>
+  <si>
+    <t>Removing Scenario with UI Handler</t>
+  </si>
+  <si>
+    <t>Test codeunit with one test function with valid Given-When-Then structure and UI Handler</t>
+  </si>
+  <si>
+    <t>User confirms removal of UI handler</t>
+  </si>
+  <si>
+    <t>UI handler function is removed</t>
+  </si>
+  <si>
+    <t>Removing Scenario with UI Handler 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User does </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> confirm removal of UI handler</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UI handler function is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>removed</t>
+    </r>
+  </si>
+  <si>
+    <t>Removal Mode "No confirmation, but removal"</t>
+  </si>
+  <si>
+    <t>Setting atddTestScriptor.removalMode equals "No confirmation, but removal"</t>
+  </si>
+  <si>
+    <t>Removal Mode "No confirmation &amp; no removal"</t>
+  </si>
+  <si>
+    <t>Setting atddTestScriptor.removalMode equals "No confirmation &amp; no removal"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All Given/When/Then helper functions related to scenario are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>removed from test codeunit</t>
+    </r>
+  </si>
+  <si>
+    <t>Removing Scenario with Initialize</t>
+  </si>
+  <si>
+    <t>Duplicate Then control disappears from ATDD.TestScriptor page</t>
   </si>
 </sst>
 </file>
@@ -2016,7 +2128,7 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="166">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2096,6 +2208,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2489,43 +2631,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2690,6 +2795,76 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2986,223 +3161,244 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="165" dataDxfId="164">
   <autoFilter ref="A1:F19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="150"/>
-    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="149"/>
-    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="148">
+    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="163"/>
+    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="161">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="147">
+    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="160">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="146"/>
-    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="145"/>
+    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="159"/>
+    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="158"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K392" totalsRowCount="1" headerRowDxfId="70" dataDxfId="69">
-  <autoFilter ref="A1:K391" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+  <autoFilter ref="A1:H17" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="66">
+      <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="65">
+      <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="67"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K433" totalsRowCount="1" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:K432" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="68" totalsRowDxfId="50">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="64" totalsRowDxfId="53">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="66" totalsRowDxfId="48"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="65" totalsRowDxfId="47"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="64" totalsRowDxfId="46">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="63" totalsRowDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="62" totalsRowDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="61" totalsRowDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="60" totalsRowDxfId="49">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="63" totalsRowDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="62" totalsRowDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="61" totalsRowDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="60" totalsRowDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="59" totalsRowDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="58" totalsRowDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="59" totalsRowDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="58" totalsRowDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="57" totalsRowDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="56" totalsRowDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="55" totalsRowDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="54" totalsRowDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="57">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="81">
   <autoFilter ref="A1:F7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="157" dataDxfId="156">
   <autoFilter ref="A1:F21" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="142"/>
-    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="140">
+    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="155"/>
+    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="153">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="139">
+    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="152">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="138"/>
-    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="137"/>
+    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="151"/>
+    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H60" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H60" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="A1:H60" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="134"/>
-    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="132">
+    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="147"/>
+    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="146"/>
+    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="145">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="131">
+    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="144">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="130"/>
-    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="129"/>
-    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="128"/>
-    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="143"/>
+    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="142"/>
+    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="141"/>
+    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138">
   <autoFilter ref="A1:F3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="124"/>
-    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="122">
+    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="137"/>
+    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="135">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="121">
+    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="134">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="120"/>
-    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="133"/>
+    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="132"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="116"/>
-    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="129"/>
+    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="127">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="113">
+    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="126">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="112"/>
-    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <autoFilter ref="A1:H7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="107"/>
-    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="105">
+    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="118">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="104">
+    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="117">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="103"/>
-    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="116"/>
+    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="114"/>
+    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H5" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H5" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
   <autoFilter ref="A1:H5" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="97"/>
-    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="95">
+    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="110"/>
+    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="108">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="94">
+    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="107">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="93"/>
-    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="90"/>
+    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="106"/>
+    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="104"/>
+    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
     <sortCondition ref="B1:B7"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="87"/>
-    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="86"/>
-    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="85">
+    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="100"/>
+    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="98">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="84">
+    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="97">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="83"/>
-    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="81"/>
+    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="96"/>
+    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H24" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H24" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A1:H24" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="78"/>
-    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="76">
+    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="91"/>
+    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="89">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="75">
+    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="88">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="74"/>
-    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="87"/>
+    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3882,24 +4078,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E20:E1048576 E1:E17">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3924,11 +4120,432 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147E497E-232A-46AA-9846-A7D1E9C8C98A}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="90.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>39</v>
+      </c>
+      <c r="B2" s="8">
+        <v>56</v>
+      </c>
+      <c r="C2" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8">
+        <v>57</v>
+      </c>
+      <c r="C3" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario step 2a</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>39</v>
+      </c>
+      <c r="B4" s="8">
+        <v>58</v>
+      </c>
+      <c r="C4" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario step 3a</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>39</v>
+      </c>
+      <c r="B5" s="8">
+        <v>59</v>
+      </c>
+      <c r="C5" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario step 2b</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>39</v>
+      </c>
+      <c r="B6" s="8">
+        <v>60</v>
+      </c>
+      <c r="C6" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario step 3b</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>39</v>
+      </c>
+      <c r="B7" s="8">
+        <v>68</v>
+      </c>
+      <c r="C7" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario with Initialize</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>39</v>
+      </c>
+      <c r="B8" s="8">
+        <v>69</v>
+      </c>
+      <c r="C8" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario with UI Handler</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>39</v>
+      </c>
+      <c r="B9" s="8">
+        <v>70</v>
+      </c>
+      <c r="C9" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario with UI Handler 2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>39</v>
+      </c>
+      <c r="B10" s="8">
+        <v>71</v>
+      </c>
+      <c r="C10" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removal Mode "No confirmation, but removal"</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>39</v>
+      </c>
+      <c r="B11" s="8">
+        <v>72</v>
+      </c>
+      <c r="C11" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removal Mode "No confirmation &amp; no removal"</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>30</v>
+      </c>
+      <c r="B12" s="8">
+        <v>16</v>
+      </c>
+      <c r="C12" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Given</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Given" to "Renamed Valid Given"</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="87">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8">
+        <v>17</v>
+      </c>
+      <c r="C13" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Given</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Given" to "Renamed Valid Given" step 2a</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="87">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>30</v>
+      </c>
+      <c r="B14" s="8">
+        <v>20</v>
+      </c>
+      <c r="C14" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating When</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid When" to "Renamed Valid When"</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="87">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>30</v>
+      </c>
+      <c r="B15" s="8">
+        <v>21</v>
+      </c>
+      <c r="C15" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating When</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid When" to "Renamed Valid When" step 2a</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="87">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>30</v>
+      </c>
+      <c r="B16" s="8">
+        <v>24</v>
+      </c>
+      <c r="C16" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Then" to "Renamed Valid Then"</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="87">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>25</v>
+      </c>
+      <c r="C17" s="63" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Then" to "Renamed Valid Then" step 2a</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="87">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="G14" r:id="rId1" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/67" xr:uid="{DA07DA0C-FBDB-4C62-B4E8-45D331DDBB9D}"/>
+    <hyperlink ref="G15:G17" r:id="rId2" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/67" xr:uid="{DAAA10DB-777C-475C-8437-74C66DDB5645}"/>
+    <hyperlink ref="G13" r:id="rId3" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/67" xr:uid="{EA2539A2-B43C-46A3-8D4F-3F532C9F4B83}"/>
+    <hyperlink ref="G12" r:id="rId4" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/67" xr:uid="{333247E3-88E4-4B24-B856-768568BF28BA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
-  <dimension ref="A1:K392"/>
+  <dimension ref="A1:K433"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F211" sqref="F210:F211"/>
+      <selection activeCell="I207" sqref="I207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -4507,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K20" s="38">
         <v>27</v>
@@ -4643,7 +5260,7 @@
       <c r="D25" s="39"/>
       <c r="E25" s="10"/>
       <c r="F25" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G25" s="37"/>
       <c r="H25" s="42"/>
@@ -4679,7 +5296,7 @@
         <v>8</v>
       </c>
       <c r="J26" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K26" s="38">
         <v>27</v>
@@ -4731,7 +5348,7 @@
         <v>29</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I28" s="12">
         <v>8</v>
@@ -4759,7 +5376,7 @@
         <v>30</v>
       </c>
       <c r="H29" s="41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I29" s="12">
         <v>8</v>
@@ -4789,7 +5406,7 @@
         <v>31</v>
       </c>
       <c r="H30" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I30" s="12">
         <v>8</v>
@@ -4813,7 +5430,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="10"/>
       <c r="F31" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G31" s="37"/>
       <c r="H31" s="43"/>
@@ -4849,7 +5466,7 @@
         <v>64</v>
       </c>
       <c r="J32" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K32" s="38">
         <v>27</v>
@@ -4901,7 +5518,7 @@
         <v>29</v>
       </c>
       <c r="H34" s="43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I34" s="12">
         <v>64</v>
@@ -4929,7 +5546,7 @@
         <v>30</v>
       </c>
       <c r="H35" s="43" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I35" s="12">
         <v>64</v>
@@ -4959,7 +5576,7 @@
         <v>31</v>
       </c>
       <c r="H36" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I36" s="12">
         <v>64</v>
@@ -4985,7 +5602,7 @@
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G37" s="37"/>
       <c r="H37" s="43"/>
@@ -5023,7 +5640,7 @@
         <v>66</v>
       </c>
       <c r="J38" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K38" s="38">
         <v>27</v>
@@ -5079,7 +5696,7 @@
         <v>29</v>
       </c>
       <c r="H40" s="43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I40" s="12">
         <v>66</v>
@@ -5109,7 +5726,7 @@
         <v>29</v>
       </c>
       <c r="H41" s="43" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I41" s="12">
         <v>66</v>
@@ -5139,7 +5756,7 @@
         <v>30</v>
       </c>
       <c r="H42" s="43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I42" s="12">
         <v>66</v>
@@ -5171,13 +5788,13 @@
         <v>31</v>
       </c>
       <c r="H43" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I43" s="12">
         <v>66</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K43" s="38">
         <v>27</v>
@@ -5233,7 +5850,7 @@
         <v>10</v>
       </c>
       <c r="J45" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K45" s="38">
         <v>27</v>
@@ -5405,7 +6022,7 @@
         <v>12</v>
       </c>
       <c r="J51" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K51" s="38">
         <v>27</v>
@@ -5577,7 +6194,7 @@
         <v>14</v>
       </c>
       <c r="J57" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K57" s="38">
         <v>27</v>
@@ -5775,7 +6392,7 @@
         <v>61</v>
       </c>
       <c r="J64" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K64" s="38">
         <v>27</v>
@@ -5997,7 +6614,7 @@
         <v>4</v>
       </c>
       <c r="J72" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K72" s="38">
         <v>27</v>
@@ -6354,7 +6971,7 @@
         <v>6</v>
       </c>
       <c r="J84" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K84" s="38">
         <v>27</v>
@@ -6490,7 +7107,7 @@
       <c r="D89" s="39"/>
       <c r="E89" s="10"/>
       <c r="F89" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G89" s="37"/>
       <c r="H89" s="42"/>
@@ -6526,7 +7143,7 @@
         <v>9</v>
       </c>
       <c r="J90" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K90" s="38">
         <v>27</v>
@@ -6578,7 +7195,7 @@
         <v>29</v>
       </c>
       <c r="H92" s="42" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I92" s="12">
         <v>9</v>
@@ -6606,7 +7223,7 @@
         <v>30</v>
       </c>
       <c r="H93" s="41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I93" s="12">
         <v>9</v>
@@ -6636,7 +7253,7 @@
         <v>31</v>
       </c>
       <c r="H94" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I94" s="12">
         <v>9</v>
@@ -6660,7 +7277,7 @@
       <c r="D95" s="39"/>
       <c r="E95" s="10"/>
       <c r="F95" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G95" s="37"/>
       <c r="H95" s="43"/>
@@ -6696,7 +7313,7 @@
         <v>65</v>
       </c>
       <c r="J96" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K96" s="38">
         <v>27</v>
@@ -6748,7 +7365,7 @@
         <v>29</v>
       </c>
       <c r="H98" s="43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I98" s="12">
         <v>65</v>
@@ -6776,7 +7393,7 @@
         <v>30</v>
       </c>
       <c r="H99" s="43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I99" s="12">
         <v>65</v>
@@ -6806,7 +7423,7 @@
         <v>31</v>
       </c>
       <c r="H100" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I100" s="12">
         <v>65</v>
@@ -6832,7 +7449,7 @@
       </c>
       <c r="E101" s="10"/>
       <c r="F101" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G101" s="37"/>
       <c r="H101" s="43"/>
@@ -6870,7 +7487,7 @@
         <v>67</v>
       </c>
       <c r="J102" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K102" s="38">
         <v>27</v>
@@ -6926,7 +7543,7 @@
         <v>29</v>
       </c>
       <c r="H104" s="43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I104" s="12">
         <v>67</v>
@@ -6956,7 +7573,7 @@
         <v>29</v>
       </c>
       <c r="H105" s="43" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I105" s="12">
         <v>67</v>
@@ -6986,7 +7603,7 @@
         <v>30</v>
       </c>
       <c r="H106" s="43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I106" s="12">
         <v>67</v>
@@ -7018,13 +7635,13 @@
         <v>31</v>
       </c>
       <c r="H107" s="43" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I107" s="12">
         <v>67</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K107" s="38">
         <v>27</v>
@@ -7080,7 +7697,7 @@
         <v>11</v>
       </c>
       <c r="J109" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K109" s="38">
         <v>27</v>
@@ -7250,7 +7867,7 @@
         <v>13</v>
       </c>
       <c r="J115" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K115" s="38">
         <v>27</v>
@@ -7422,7 +8039,7 @@
         <v>15</v>
       </c>
       <c r="J121" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K121" s="38">
         <v>27</v>
@@ -7862,7 +8479,7 @@
         <v>16</v>
       </c>
       <c r="J137" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K137" s="38">
         <v>30</v>
@@ -8569,7 +9186,7 @@
         <v>44</v>
       </c>
       <c r="J161" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K161" s="38">
         <v>30</v>
@@ -8859,7 +9476,7 @@
         <v>51</v>
       </c>
       <c r="J171" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K171" s="38">
         <v>30</v>
@@ -9201,7 +9818,7 @@
         <v>20</v>
       </c>
       <c r="J183" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K183" s="51">
         <v>30</v>
@@ -9932,7 +10549,7 @@
         <v>24</v>
       </c>
       <c r="J208" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K208" s="51">
         <v>30</v>
@@ -10307,7 +10924,7 @@
         <v>25</v>
       </c>
       <c r="F221" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G221" s="31"/>
       <c r="H221" s="41"/>
@@ -10426,7 +11043,7 @@
         <v>26</v>
       </c>
       <c r="F225" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G225" s="31"/>
       <c r="H225" s="41"/>
@@ -11255,7 +11872,7 @@
         <v>28</v>
       </c>
       <c r="J254" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K254" s="51">
         <v>28</v>
@@ -11965,7 +12582,7 @@
         <v>38</v>
       </c>
       <c r="J278" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K278" s="51">
         <v>28</v>
@@ -12191,7 +12808,7 @@
         <v>40</v>
       </c>
       <c r="J286" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K286" s="51">
         <v>28</v>
@@ -12445,7 +13062,7 @@
         <v>41</v>
       </c>
       <c r="J295" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K295" s="51">
         <v>28</v>
@@ -12639,7 +13256,7 @@
         <v>33</v>
       </c>
       <c r="J302" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K302" s="51">
         <v>28</v>
@@ -13571,7 +14188,7 @@
         <v>42</v>
       </c>
       <c r="J334" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K334" s="51">
         <v>28</v>
@@ -13797,7 +14414,7 @@
         <v>43</v>
       </c>
       <c r="J342" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K342" s="51">
         <v>28</v>
@@ -14044,7 +14661,7 @@
         <v>55</v>
       </c>
       <c r="J351" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K351" s="72">
         <v>38</v>
@@ -14269,7 +14886,7 @@
         <v>56</v>
       </c>
       <c r="J359" s="43" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K359" s="66">
         <v>39</v>
@@ -14802,7 +15419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="378" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A378" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -14833,7 +15450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="379" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A379" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -14863,7 +15480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="380" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A380" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -14893,7 +15510,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="381" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A381" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -14923,7 +15540,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="382" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A382" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -14956,7 +15573,7 @@
     <row r="383" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A383" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B383" s="65" t="s">
         <v>240</v>
@@ -14967,21 +15584,21 @@
       <c r="D383" s="67"/>
       <c r="E383" s="68"/>
       <c r="F383" s="69" t="s">
-        <v>296</v>
+        <v>333</v>
       </c>
       <c r="H383" s="41"/>
       <c r="I383" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J383" s="71"/>
       <c r="K383" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="384" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A384" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B384" s="65" t="s">
         <v>240</v>
@@ -14996,22 +15613,22 @@
         <v>29</v>
       </c>
       <c r="H384" s="41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I384" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J384" s="71" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K384" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="385" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A385" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B385" s="65" t="s">
         <v>240</v>
@@ -15026,20 +15643,20 @@
         <v>29</v>
       </c>
       <c r="H385" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I385" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J385" s="71"/>
       <c r="K385" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="386" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A386" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B386" s="65" t="s">
         <v>240</v>
@@ -15057,17 +15674,17 @@
         <v>241</v>
       </c>
       <c r="I386" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J386" s="71"/>
       <c r="K386" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="387" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A387" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B387" s="65" t="s">
         <v>240</v>
@@ -15085,17 +15702,17 @@
         <v>133</v>
       </c>
       <c r="I387" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J387" s="71"/>
       <c r="K387" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="388" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A388" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B388" s="65" t="s">
         <v>240</v>
@@ -15113,17 +15730,17 @@
         <v>244</v>
       </c>
       <c r="I388" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J388" s="71"/>
       <c r="K388" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="389" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A389" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B389" s="65" t="s">
         <v>240</v>
@@ -15141,17 +15758,17 @@
         <v>247</v>
       </c>
       <c r="I389" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J389" s="71"/>
       <c r="K389" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="390" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A390" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B390" s="65" t="s">
         <v>240</v>
@@ -15166,20 +15783,20 @@
         <v>31</v>
       </c>
       <c r="H390" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I390" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J390" s="71"/>
       <c r="K390" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="391" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A391" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B391" s="65" t="s">
         <v>240</v>
@@ -15194,29 +15811,1157 @@
         <v>31</v>
       </c>
       <c r="H391" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I391" s="70">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J391" s="71"/>
       <c r="K391" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="392" spans="1:11" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A392" s="61"/>
-      <c r="B392" s="1" t="s">
+    <row r="392" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A392" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B392" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C392" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D392" s="67"/>
+      <c r="E392" s="68"/>
+      <c r="F392" s="69" t="s">
+        <v>321</v>
+      </c>
+      <c r="H392" s="41"/>
+      <c r="I392" s="70">
+        <v>69</v>
+      </c>
+      <c r="J392" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="K392" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A393" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B393" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C393" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D393" s="67"/>
+      <c r="E393" s="68"/>
+      <c r="F393" s="69"/>
+      <c r="G393" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H393" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="I393" s="70">
+        <v>69</v>
+      </c>
+      <c r="J393" s="71"/>
+      <c r="K393" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A394" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B394" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C394" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D394" s="67"/>
+      <c r="E394" s="68"/>
+      <c r="F394" s="69"/>
+      <c r="G394" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H394" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I394" s="70">
+        <v>69</v>
+      </c>
+      <c r="J394" s="71"/>
+      <c r="K394" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A395" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B395" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C395" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D395" s="67"/>
+      <c r="E395" s="68"/>
+      <c r="F395" s="69"/>
+      <c r="G395" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H395" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="I395" s="70">
+        <v>69</v>
+      </c>
+      <c r="J395" s="71"/>
+      <c r="K395" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A396" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B396" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C396" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D396" s="67"/>
+      <c r="E396" s="68"/>
+      <c r="F396" s="69"/>
+      <c r="G396" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H396" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I396" s="70">
+        <v>69</v>
+      </c>
+      <c r="J396" s="71"/>
+      <c r="K396" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A397" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B397" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C397" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D397" s="67"/>
+      <c r="E397" s="68"/>
+      <c r="F397" s="69"/>
+      <c r="G397" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H397" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I397" s="70">
+        <v>69</v>
+      </c>
+      <c r="J397" s="71"/>
+      <c r="K397" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A398" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B398" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C398" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D398" s="67"/>
+      <c r="E398" s="68"/>
+      <c r="F398" s="69"/>
+      <c r="G398" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="H398" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="I398" s="70">
+        <v>69</v>
+      </c>
+      <c r="J398" s="71"/>
+      <c r="K398" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A399" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B399" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C399" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D399" s="67"/>
+      <c r="E399" s="68"/>
+      <c r="F399" s="69"/>
+      <c r="G399" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H399" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I399" s="70">
+        <v>69</v>
+      </c>
+      <c r="J399" s="71"/>
+      <c r="K399" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A400" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B400" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C400" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D400" s="67"/>
+      <c r="E400" s="68"/>
+      <c r="F400" s="69"/>
+      <c r="G400" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H400" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="I400" s="70">
+        <v>69</v>
+      </c>
+      <c r="J400" s="71"/>
+      <c r="K400" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A401" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B401" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C401" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D401" s="67"/>
+      <c r="E401" s="68"/>
+      <c r="F401" s="69"/>
+      <c r="G401" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H401" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="I401" s="70">
+        <v>69</v>
+      </c>
+      <c r="J401" s="71"/>
+      <c r="K401" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A402" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>69</v>
+      </c>
+      <c r="B402" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C402" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D402" s="67"/>
+      <c r="E402" s="68"/>
+      <c r="F402" s="69"/>
+      <c r="G402" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H402" s="41" t="s">
+        <v>324</v>
+      </c>
+      <c r="I402" s="70">
+        <v>69</v>
+      </c>
+      <c r="J402" s="71"/>
+      <c r="K402" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A403" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B403" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C403" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D403" s="67"/>
+      <c r="E403" s="68"/>
+      <c r="F403" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="H403" s="41"/>
+      <c r="I403" s="70">
+        <v>70</v>
+      </c>
+      <c r="J403" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="K403" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A404" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B404" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C404" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D404" s="67"/>
+      <c r="E404" s="68"/>
+      <c r="F404" s="69"/>
+      <c r="G404" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H404" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="I404" s="70">
+        <v>70</v>
+      </c>
+      <c r="J404" s="71"/>
+      <c r="K404" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A405" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B405" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C405" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D405" s="67"/>
+      <c r="E405" s="68"/>
+      <c r="F405" s="69"/>
+      <c r="G405" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H405" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I405" s="70">
+        <v>70</v>
+      </c>
+      <c r="J405" s="71"/>
+      <c r="K405" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A406" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B406" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C406" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D406" s="67"/>
+      <c r="E406" s="68"/>
+      <c r="F406" s="69"/>
+      <c r="G406" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H406" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="I406" s="70">
+        <v>70</v>
+      </c>
+      <c r="J406" s="71"/>
+      <c r="K406" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A407" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B407" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C407" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D407" s="67"/>
+      <c r="E407" s="68"/>
+      <c r="F407" s="69"/>
+      <c r="G407" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H407" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I407" s="70">
+        <v>70</v>
+      </c>
+      <c r="J407" s="71"/>
+      <c r="K407" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A408" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B408" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C408" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D408" s="67"/>
+      <c r="E408" s="68"/>
+      <c r="F408" s="69"/>
+      <c r="G408" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H408" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I408" s="70">
+        <v>70</v>
+      </c>
+      <c r="J408" s="71"/>
+      <c r="K408" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A409" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B409" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C409" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D409" s="67"/>
+      <c r="E409" s="68"/>
+      <c r="F409" s="69"/>
+      <c r="G409" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="H409" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="I409" s="70">
+        <v>70</v>
+      </c>
+      <c r="J409" s="71"/>
+      <c r="K409" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A410" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B410" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C410" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D410" s="67"/>
+      <c r="E410" s="68"/>
+      <c r="F410" s="69"/>
+      <c r="G410" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H410" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I410" s="70">
+        <v>70</v>
+      </c>
+      <c r="J410" s="71"/>
+      <c r="K410" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A411" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B411" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C411" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D411" s="67"/>
+      <c r="E411" s="68"/>
+      <c r="F411" s="69"/>
+      <c r="G411" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H411" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="I411" s="70">
+        <v>70</v>
+      </c>
+      <c r="J411" s="71"/>
+      <c r="K411" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A412" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B412" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C412" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D412" s="67"/>
+      <c r="E412" s="68"/>
+      <c r="F412" s="69"/>
+      <c r="G412" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H412" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="I412" s="70">
+        <v>70</v>
+      </c>
+      <c r="J412" s="71"/>
+      <c r="K412" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A413" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>70</v>
+      </c>
+      <c r="B413" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C413" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D413" s="67"/>
+      <c r="E413" s="68"/>
+      <c r="F413" s="69"/>
+      <c r="G413" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H413" s="41" t="s">
+        <v>327</v>
+      </c>
+      <c r="I413" s="70">
+        <v>70</v>
+      </c>
+      <c r="J413" s="71"/>
+      <c r="K413" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A414" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B414" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C414" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D414" s="67"/>
+      <c r="E414" s="68"/>
+      <c r="F414" s="69" t="s">
+        <v>328</v>
+      </c>
+      <c r="H414" s="41"/>
+      <c r="I414" s="70">
+        <v>71</v>
+      </c>
+      <c r="J414" s="71" t="s">
+        <v>298</v>
+      </c>
+      <c r="K414" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A415" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B415" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C415" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D415" s="67"/>
+      <c r="E415" s="68"/>
+      <c r="F415" s="69"/>
+      <c r="G415" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H415" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="I415" s="70">
+        <v>71</v>
+      </c>
+      <c r="J415" s="71"/>
+      <c r="K415" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A416" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B416" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C416" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D416" s="67"/>
+      <c r="E416" s="68"/>
+      <c r="F416" s="69"/>
+      <c r="G416" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H416" s="41" t="s">
+        <v>329</v>
+      </c>
+      <c r="I416" s="70">
+        <v>71</v>
+      </c>
+      <c r="J416" s="71"/>
+      <c r="K416" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A417" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B417" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C417" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D417" s="67"/>
+      <c r="E417" s="68"/>
+      <c r="F417" s="69"/>
+      <c r="G417" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H417" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I417" s="70">
+        <v>71</v>
+      </c>
+      <c r="J417" s="71"/>
+      <c r="K417" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A418" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B418" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C418" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D418" s="67"/>
+      <c r="E418" s="68"/>
+      <c r="F418" s="69"/>
+      <c r="G418" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H418" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="I418" s="70">
+        <v>71</v>
+      </c>
+      <c r="J418" s="71"/>
+      <c r="K418" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A419" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B419" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C419" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D419" s="67"/>
+      <c r="E419" s="68"/>
+      <c r="F419" s="69"/>
+      <c r="G419" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H419" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I419" s="70">
+        <v>71</v>
+      </c>
+      <c r="J419" s="71"/>
+      <c r="K419" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A420" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B420" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C420" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D420" s="67"/>
+      <c r="E420" s="68"/>
+      <c r="F420" s="69"/>
+      <c r="G420" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H420" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I420" s="70">
+        <v>71</v>
+      </c>
+      <c r="J420" s="71"/>
+      <c r="K420" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A421" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B421" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C421" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D421" s="67"/>
+      <c r="E421" s="68"/>
+      <c r="F421" s="69"/>
+      <c r="G421" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H421" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="I421" s="70">
+        <v>71</v>
+      </c>
+      <c r="J421" s="71"/>
+      <c r="K421" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A422" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>71</v>
+      </c>
+      <c r="B422" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C422" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D422" s="67"/>
+      <c r="E422" s="68"/>
+      <c r="F422" s="69"/>
+      <c r="G422" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H422" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="I422" s="70">
+        <v>71</v>
+      </c>
+      <c r="J422" s="71"/>
+      <c r="K422" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A423" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B423" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C423" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D423" s="67"/>
+      <c r="E423" s="68"/>
+      <c r="F423" s="69" t="s">
+        <v>330</v>
+      </c>
+      <c r="H423" s="41"/>
+      <c r="I423" s="70">
+        <v>72</v>
+      </c>
+      <c r="J423" s="71"/>
+      <c r="K423" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A424" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B424" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C424" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D424" s="67"/>
+      <c r="E424" s="68"/>
+      <c r="F424" s="69"/>
+      <c r="G424" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H424" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="I424" s="70">
+        <v>72</v>
+      </c>
+      <c r="J424" s="71"/>
+      <c r="K424" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A425" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B425" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C425" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D425" s="67"/>
+      <c r="E425" s="68"/>
+      <c r="F425" s="69"/>
+      <c r="G425" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H425" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="I425" s="70">
+        <v>72</v>
+      </c>
+      <c r="J425" s="71"/>
+      <c r="K425" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A426" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B426" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C426" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D426" s="67"/>
+      <c r="E426" s="68"/>
+      <c r="F426" s="69"/>
+      <c r="G426" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H426" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="I426" s="70">
+        <v>72</v>
+      </c>
+      <c r="J426" s="71"/>
+      <c r="K426" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A427" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B427" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C427" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D427" s="67"/>
+      <c r="E427" s="68"/>
+      <c r="F427" s="69"/>
+      <c r="G427" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="H427" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="I427" s="70">
+        <v>72</v>
+      </c>
+      <c r="J427" s="71"/>
+      <c r="K427" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A428" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B428" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C428" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D428" s="67"/>
+      <c r="E428" s="68"/>
+      <c r="F428" s="69"/>
+      <c r="G428" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H428" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I428" s="70">
+        <v>72</v>
+      </c>
+      <c r="J428" s="71"/>
+      <c r="K428" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A429" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B429" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C429" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D429" s="67"/>
+      <c r="E429" s="68"/>
+      <c r="F429" s="69"/>
+      <c r="G429" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H429" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="I429" s="70">
+        <v>72</v>
+      </c>
+      <c r="J429" s="71"/>
+      <c r="K429" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A430" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B430" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C430" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D430" s="67"/>
+      <c r="E430" s="68"/>
+      <c r="F430" s="69"/>
+      <c r="G430" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H430" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="I430" s="70">
+        <v>72</v>
+      </c>
+      <c r="J430" s="71"/>
+      <c r="K430" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A431" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B431" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="C431" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D431" s="67"/>
+      <c r="E431" s="68"/>
+      <c r="F431" s="69"/>
+      <c r="G431" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H431" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="I431" s="70">
+        <v>72</v>
+      </c>
+      <c r="J431" s="71"/>
+      <c r="K431" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A432" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>0</v>
+      </c>
+      <c r="C432" s="66"/>
+      <c r="D432" s="67"/>
+      <c r="E432" s="68"/>
+      <c r="F432" s="69"/>
+      <c r="H432" s="41"/>
+      <c r="I432" s="70"/>
+      <c r="J432" s="71"/>
+      <c r="K432" s="66"/>
+    </row>
+    <row r="433" spans="1:9" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A433" s="61"/>
+      <c r="B433" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C392" s="3"/>
-      <c r="E392" s="10">
+      <c r="C433" s="3"/>
+      <c r="E433" s="10">
         <f>Table14[[#Totals],[Scenario '#]]</f>
         <v>63</v>
       </c>
-      <c r="F392" s="6"/>
-      <c r="H392" s="2"/>
-      <c r="I392" s="12">
+      <c r="F433" s="6"/>
+      <c r="H433" s="2"/>
+      <c r="I433" s="12">
         <f>SUBTOTAL(104,Table14[Scenario '#])</f>
         <v>63</v>
       </c>
@@ -15266,7 +17011,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G386:G1048576 G1:G384">
+  <conditionalFormatting sqref="G1:G384 G386:G1048576">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -15296,7 +17041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB16863-C9D6-47DE-82AF-06BDE2CF5BC1}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -15940,13 +17685,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17290,13 +19035,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17422,13 +19167,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17640,13 +19385,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17683,7 +19428,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17859,13 +19604,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18026,13 +19771,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18053,7 +19798,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18185,7 +19930,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G6" s="87">
         <v>52</v>
@@ -18210,7 +19955,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G7" s="87">
         <v>52</v>
@@ -18218,13 +19963,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18257,7 +20002,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18316,7 +20061,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G2" s="87">
         <v>67</v>
@@ -18341,7 +20086,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G3" s="87">
         <v>67</v>
@@ -18366,7 +20111,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G4" s="87">
         <v>67</v>
@@ -18391,7 +20136,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G5" s="87">
         <v>67</v>
@@ -18416,7 +20161,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G6" s="87">
         <v>67</v>
@@ -18441,7 +20186,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G7" s="87">
         <v>67</v>
@@ -18466,7 +20211,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G8" s="87">
         <v>67</v>
@@ -18530,7 +20275,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G11" s="87">
         <v>67</v>
@@ -18555,7 +20300,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G12" s="87">
         <v>67</v>
@@ -18580,7 +20325,7 @@
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G13" s="87">
         <v>67</v>
@@ -18605,7 +20350,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G14" s="87">
         <v>67</v>
@@ -18630,7 +20375,7 @@
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G15" s="87">
         <v>67</v>
@@ -18655,7 +20400,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G16" s="87">
         <v>67</v>
@@ -18680,7 +20425,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G17" s="87">
         <v>67</v>
@@ -18705,7 +20450,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G18" s="87">
         <v>67</v>
@@ -18730,7 +20475,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G19" s="87">
         <v>67</v>
@@ -18755,7 +20500,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G20" s="87">
         <v>67</v>
@@ -18780,7 +20525,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G21" s="87">
         <v>67</v>
@@ -18805,7 +20550,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G22" s="87">
         <v>67</v>
@@ -18830,7 +20575,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="G23" s="87">
         <v>68</v>
@@ -18855,7 +20600,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="G24" s="87">
         <v>68</v>
@@ -18875,13 +20620,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated test for #60
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31105CD2-F970-458F-B7DF-158F5D105EC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348FCDE-8A8A-4B11-BA2B-244B989CE2DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="24510" windowHeight="15990" tabRatio="693" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="24510" windowHeight="15990" tabRatio="693" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200811" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="371">
   <si>
     <t>Scenario</t>
   </si>
@@ -1414,9 +1414,6 @@
     <t>Duplicate Then control disappears from ATDD.TestScriptor page</t>
   </si>
   <si>
-    <t>ValidTestFunction ([FEATURE] First test object) in codeunit 50100 TestObjectFLX</t>
-  </si>
-  <si>
     <t>Nothing is renamed</t>
   </si>
   <si>
@@ -1594,6 +1591,88 @@
       </rPr>
       <t>reverted</t>
     </r>
+  </si>
+  <si>
+    <t>FirstTestFunctionWithValidGivenWhenThenstructure ([FEATURE] First test object) in codeunit 50100 TestObjectFLX</t>
+  </si>
+  <si>
+    <t>SecondTestFunctionWithValidGivenWhenThenStructure  ([FEATURE] Duplicate test object) in codeunit 50101 DuplicateTestObjectFLX</t>
+  </si>
+  <si>
+    <t>ThirdTestFunctionWithValidGivenWhenThenStructure  ([FEATURE] Duplicate test object) in codeunit 50101 DuplicateTestObjectFLX</t>
+  </si>
+  <si>
+    <t>Rename "Second test function with valid Given-When-Then structure" to "Third test function with valid Given-When-Then structure" and confirm</t>
+  </si>
+  <si>
+    <t>Rename to already existing scenario name</t>
+  </si>
+  <si>
+    <t>Message "Scenario already exists. Please update your scenario definition so it is unique" appears</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test function  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SecondTestFunctionWithValidGivenWhenThenStructurewith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> valid Given-When-Then structure</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Other test function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ThirdTestFunctionWithValidGivenWhenThenStructure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with valid Given-When-Then structure</t>
+    </r>
+  </si>
+  <si>
+    <t>Rename to unique name</t>
+  </si>
+  <si>
+    <t>Change "Third test function with valid Given-When-Then structure" to "Another test function with valid Given-When-Then structure" to and confirm</t>
+  </si>
+  <si>
+    <t>Comment line "[SCENARIO 0002] Second test function with valid Given-When-Then structure" is updated to "[SCENARIO 0002] Valid Given-When-Then structure"</t>
+  </si>
+  <si>
+    <t>Second test function (scenario) is renamed</t>
   </si>
 </sst>
 </file>
@@ -2255,7 +2334,7 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="199">
+  <dxfs count="208">
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2364,6 +2443,69 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -3104,36 +3246,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3179,6 +3291,36 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3495,88 +3637,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="198" dataDxfId="197">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="207" dataDxfId="206">
   <autoFilter ref="A1:F19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="196"/>
-    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="195"/>
-    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="194">
+    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="205"/>
+    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="204"/>
+    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="203">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="193">
+    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="202">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="192"/>
-    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="191"/>
+    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="201"/>
+    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="200"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="A1:H17" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="123">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="112">
+    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="122"/>
+    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="121">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="111">
+    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="120">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="110"/>
-    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="119"/>
+    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{53B13E5C-5441-4B69-91E3-36B14A182343}" name="Table15691314" displayName="Table15691314" ref="A1:G73" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
-  <autoFilter ref="A1:G73" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{53B13E5C-5441-4B69-91E3-36B14A182343}" name="Table15691314" displayName="Table15691314" ref="A1:G75" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
+  <autoFilter ref="A1:G75" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF78A628-9C38-4564-9808-3B26AF234F77}" name="GitHub Issue" dataDxfId="95">
+    <tableColumn id="1" xr3:uid="{AF78A628-9C38-4564-9808-3B26AF234F77}" name="GitHub Issue" dataDxfId="113">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2CAB733F-F4E3-4B07-84CB-D00849F9BD6C}" name="#" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{0F5DE106-934C-4581-BEC9-F2BED1604D9A}" name="Feature" dataDxfId="93">
+    <tableColumn id="10" xr3:uid="{2CAB733F-F4E3-4B07-84CB-D00849F9BD6C}" name="#" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{0F5DE106-934C-4581-BEC9-F2BED1604D9A}" name="Feature" dataDxfId="111">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{211378E0-438E-4FA5-A4AE-A66A0C3D748F}" name="Scenario" dataDxfId="92">
+    <tableColumn id="3" xr3:uid="{211378E0-438E-4FA5-A4AE-A66A0C3D748F}" name="Scenario" dataDxfId="110">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{932BD0E7-22E6-4F2C-8057-85843CDDFC76}" name="Result" dataDxfId="91"/>
-    <tableColumn id="9" xr3:uid="{E6B98784-DB78-486D-B5E1-8E879B6CB05A}" name="Notes" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{EF5B5B9D-C80C-4F4B-B547-BA970D46AED2}" name="Issue" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{932BD0E7-22E6-4F2C-8057-85843CDDFC76}" name="Result" dataDxfId="109"/>
+    <tableColumn id="9" xr3:uid="{E6B98784-DB78-486D-B5E1-8E879B6CB05A}" name="Notes" dataDxfId="108"/>
+    <tableColumn id="4" xr3:uid="{EF5B5B9D-C80C-4F4B-B547-BA970D46AED2}" name="Issue" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K468" totalsRowCount="1" headerRowDxfId="106" dataDxfId="105">
-  <autoFilter ref="A1:K467" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K470" totalsRowCount="1" headerRowDxfId="106" dataDxfId="105">
+  <autoFilter ref="A1:K469" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="88" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="97" totalsRowDxfId="10">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="86" totalsRowDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="85" totalsRowDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="84" totalsRowDxfId="6">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="96" totalsRowDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="95" totalsRowDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="94" totalsRowDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="6">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="83" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="82" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="81" totalsRowDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="80" totalsRowDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="79" totalsRowDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="78" totalsRowDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="92" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="91" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="90" totalsRowDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="89" totalsRowDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="88" totalsRowDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="87" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3598,165 +3740,165 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="190" dataDxfId="189">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198">
   <autoFilter ref="A1:F21" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="188"/>
-    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="187"/>
-    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="186">
+    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="197"/>
+    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="196"/>
+    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="195">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="185">
+    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="194">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="184"/>
-    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="183"/>
+    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="193"/>
+    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="192"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H56" totalsRowShown="0" headerRowDxfId="182" dataDxfId="181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H56" totalsRowShown="0" headerRowDxfId="191" dataDxfId="190">
   <autoFilter ref="A1:H56" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="180"/>
-    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="179"/>
-    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="178">
+    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="189"/>
+    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="188"/>
+    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="187">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="177">
+    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="186">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="176"/>
-    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="175"/>
-    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="174"/>
-    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="173"/>
+    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="185"/>
+    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="184"/>
+    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="182"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="172" dataDxfId="171">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="181" dataDxfId="180">
   <autoFilter ref="A1:F3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="170"/>
-    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="169"/>
-    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="168">
+    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="179"/>
+    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="178"/>
+    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="177">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="167">
+    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="176">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="166"/>
-    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="165"/>
+    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="175"/>
+    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="174"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="173" dataDxfId="172">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="162"/>
-    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="161"/>
-    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="160">
+    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="171"/>
+    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="170"/>
+    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="169">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="159">
+    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="168">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="158"/>
-    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="157"/>
-    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="156"/>
+    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="167"/>
+    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="166"/>
+    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="165"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163">
   <autoFilter ref="A1:H7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="153"/>
-    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="151">
+    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="162"/>
+    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="161"/>
+    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="160">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="150">
+    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="159">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="149"/>
-    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="147"/>
-    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="146"/>
+    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="158"/>
+    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="156"/>
+    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="155"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H3" totalsRowShown="0" headerRowDxfId="145" dataDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H3" totalsRowShown="0" headerRowDxfId="154" dataDxfId="153">
   <autoFilter ref="A1:H3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="143"/>
-    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="142"/>
-    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="141">
+    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="152"/>
+    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="151"/>
+    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="150">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="140">
+    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="149">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="139"/>
-    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="137"/>
-    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="148"/>
+    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="147"/>
+    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="146"/>
+    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="145"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
     <sortCondition ref="B1:B7"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="133"/>
-    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="132"/>
-    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="131">
+    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="142"/>
+    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="140">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="130">
+    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="139">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="129"/>
-    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="138"/>
+    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="137"/>
+    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H20" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H20" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
   <autoFilter ref="A1:H20" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="124"/>
-    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="122">
+    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="133"/>
+    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="132"/>
+    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="131">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="121">
+    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="130">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="120"/>
-    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="117"/>
+    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="129"/>
+    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="128"/>
+    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4436,24 +4578,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E20:E1048576 E1:E17">
-    <cfRule type="cellIs" dxfId="77" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4890,13 +5032,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="47" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4916,10 +5058,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AAAF6E-78DD-431A-8469-F0039B6C8AAD}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5906,7 +6048,7 @@
         <v>11</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G46" s="87">
         <v>79</v>
@@ -5932,7 +6074,7 @@
         <v>11</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G47" s="87">
         <v>79</v>
@@ -5958,7 +6100,7 @@
         <v>11</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G48" s="87">
         <v>79</v>
@@ -5984,7 +6126,7 @@
         <v>11</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G49" s="87">
         <v>79</v>
@@ -6099,7 +6241,7 @@
         <v>11</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G54" s="87">
         <v>79</v>
@@ -6146,7 +6288,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G56" s="87">
         <v>79</v>
@@ -6298,7 +6440,7 @@
         <v>11</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G63" s="87">
         <v>80</v>
@@ -6325,7 +6467,7 @@
       </c>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>39</v>
@@ -6346,7 +6488,7 @@
       </c>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>39</v>
@@ -6367,7 +6509,7 @@
       </c>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>39</v>
@@ -6388,7 +6530,7 @@
       </c>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>39</v>
@@ -6409,7 +6551,7 @@
       </c>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>39</v>
@@ -6430,7 +6572,7 @@
       </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>39</v>
@@ -6451,7 +6593,7 @@
       </c>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>60</v>
@@ -6472,7 +6614,7 @@
       </c>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>60</v>
@@ -6493,7 +6635,7 @@
       </c>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>60</v>
@@ -6513,7 +6655,54 @@
         <v>11</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>359</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="B74" s="8">
+        <v>83</v>
+      </c>
+      <c r="C74" s="63" t="str">
+        <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Scenario</v>
+      </c>
+      <c r="D74" s="63" t="str">
+        <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename to already existing scenario name</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="B75" s="8">
+        <v>84</v>
+      </c>
+      <c r="C75" s="63" t="str">
+        <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Scenario</v>
+      </c>
+      <c r="D75" s="63" t="str">
+        <f>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename to unique name</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="G75" s="87">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -6530,13 +6719,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="8" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="10" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6549,21 +6738,22 @@
     <hyperlink ref="G48" r:id="rId6" display="79" xr:uid="{C3DC6227-8481-40BC-813C-08D2DCF92080}"/>
     <hyperlink ref="G49" r:id="rId7" display="79" xr:uid="{2BE836F4-1F2F-4143-966B-B1B9339DD4E9}"/>
     <hyperlink ref="G63" r:id="rId8" display="80" xr:uid="{CD0C66B0-2546-4B51-B47C-A3C0BDF29DEF}"/>
+    <hyperlink ref="G75" r:id="rId9" display="81" xr:uid="{D8B964F8-E918-4135-8DBE-60EA9E0D6823}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
-  <dimension ref="A1:K468"/>
+  <dimension ref="A1:K470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B241" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H384" sqref="H384"/>
+    <sheetView topLeftCell="B382" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H392" sqref="H392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -6787,7 +6977,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="41" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K8" s="38">
         <v>27</v>
@@ -6907,7 +7097,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7094,7 +7284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7144,7 +7334,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K20" s="38">
         <v>27</v>
@@ -7266,7 +7456,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7316,7 +7506,7 @@
         <v>8</v>
       </c>
       <c r="J26" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K26" s="38">
         <v>27</v>
@@ -7436,7 +7626,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7486,7 +7676,7 @@
         <v>64</v>
       </c>
       <c r="J32" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K32" s="38">
         <v>27</v>
@@ -7606,7 +7796,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -7660,7 +7850,7 @@
         <v>66</v>
       </c>
       <c r="J38" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K38" s="38">
         <v>27</v>
@@ -7820,7 +8010,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -7870,7 +8060,7 @@
         <v>10</v>
       </c>
       <c r="J45" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K45" s="38">
         <v>27</v>
@@ -7992,7 +8182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8042,7 +8232,7 @@
         <v>12</v>
       </c>
       <c r="J51" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K51" s="38">
         <v>27</v>
@@ -8164,7 +8354,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8214,7 +8404,7 @@
         <v>14</v>
       </c>
       <c r="J57" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K57" s="38">
         <v>27</v>
@@ -8362,7 +8552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8412,7 +8602,7 @@
         <v>61</v>
       </c>
       <c r="J64" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K64" s="38">
         <v>27</v>
@@ -8634,7 +8824,7 @@
         <v>4</v>
       </c>
       <c r="J72" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K72" s="38">
         <v>27</v>
@@ -8754,7 +8944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>5</v>
@@ -8941,7 +9131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>6</v>
@@ -8991,7 +9181,7 @@
         <v>6</v>
       </c>
       <c r="J84" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K84" s="38">
         <v>27</v>
@@ -9113,7 +9303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>9</v>
@@ -9163,7 +9353,7 @@
         <v>9</v>
       </c>
       <c r="J90" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K90" s="38">
         <v>27</v>
@@ -9283,7 +9473,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>65</v>
@@ -9333,7 +9523,7 @@
         <v>65</v>
       </c>
       <c r="J96" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K96" s="38">
         <v>27</v>
@@ -9453,7 +9643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>67</v>
@@ -9507,7 +9697,7 @@
         <v>67</v>
       </c>
       <c r="J102" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K102" s="38">
         <v>27</v>
@@ -9667,7 +9857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>11</v>
@@ -9717,7 +9907,7 @@
         <v>11</v>
       </c>
       <c r="J109" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K109" s="38">
         <v>27</v>
@@ -9837,7 +10027,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>13</v>
@@ -9887,7 +10077,7 @@
         <v>13</v>
       </c>
       <c r="J115" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K115" s="38">
         <v>27</v>
@@ -10009,7 +10199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>15</v>
@@ -10059,7 +10249,7 @@
         <v>15</v>
       </c>
       <c r="J121" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K121" s="38">
         <v>27</v>
@@ -10207,7 +10397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A127" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>62</v>
@@ -10449,7 +10639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="16.5" outlineLevel="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" ht="16.5" hidden="1" outlineLevel="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>16</v>
@@ -10475,7 +10665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="30.75" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" ht="30.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A137" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>16</v>
@@ -10499,13 +10689,13 @@
         <v>16</v>
       </c>
       <c r="J137" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K137" s="38">
         <v>30</v>
       </c>
     </row>
-    <row r="138" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A138" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>16</v>
@@ -10533,7 +10723,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A139" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>16</v>
@@ -10561,7 +10751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="140" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A140" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>17</v>
@@ -10589,7 +10779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="141" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A141" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>17</v>
@@ -10620,7 +10810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="142" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>17</v>
@@ -10650,7 +10840,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>17</v>
@@ -10680,7 +10870,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A144" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>17</v>
@@ -10710,7 +10900,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A145" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>17</v>
@@ -10740,7 +10930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="146" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A146" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>46</v>
@@ -10768,7 +10958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A147" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>46</v>
@@ -10798,7 +10988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="148" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A148" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>46</v>
@@ -10828,7 +11018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="149" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A149" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>46</v>
@@ -10848,7 +11038,7 @@
         <v>31</v>
       </c>
       <c r="H149" s="41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I149" s="12">
         <v>46</v>
@@ -10858,7 +11048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="150" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>46</v>
@@ -10878,7 +11068,7 @@
         <v>31</v>
       </c>
       <c r="H150" s="41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I150" s="12">
         <v>46</v>
@@ -10888,7 +11078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="151" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A151" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>18</v>
@@ -11007,7 +11197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="155" spans="1:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A155" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>19</v>
@@ -11186,7 +11376,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="161" spans="1:11" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A161" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11212,7 +11402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A162" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11236,13 +11426,13 @@
         <v>44</v>
       </c>
       <c r="J162" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K162" s="38">
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A163" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11270,7 +11460,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A164" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11288,19 +11478,19 @@
         <v>29</v>
       </c>
       <c r="H164" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I164" s="12">
         <v>44</v>
       </c>
       <c r="J164" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K164" s="38">
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A165" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11328,7 +11518,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A166" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11356,7 +11546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A167" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>44</v>
@@ -11384,7 +11574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A168" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11410,7 +11600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A169" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11434,13 +11624,13 @@
         <v>51</v>
       </c>
       <c r="J169" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K169" s="38">
         <v>30</v>
       </c>
     </row>
-    <row r="170" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A170" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11458,7 +11648,7 @@
         <v>29</v>
       </c>
       <c r="H170" s="41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I170" s="12">
         <v>51</v>
@@ -11468,7 +11658,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A171" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11486,19 +11676,19 @@
         <v>29</v>
       </c>
       <c r="H171" s="41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I171" s="12">
         <v>51</v>
       </c>
       <c r="J171" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K171" s="38">
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A172" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11526,7 +11716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A173" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11554,7 +11744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A174" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11582,7 +11772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="30.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>51</v>
@@ -11610,7 +11800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>0</v>
@@ -11684,7 +11874,7 @@
         <v>20</v>
       </c>
       <c r="J178" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K178" s="51">
         <v>30</v>
@@ -11746,7 +11936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:11" s="16" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" s="16" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A181" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>21</v>
@@ -11925,7 +12115,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:11" s="16" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" s="16" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A187" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>47</v>
@@ -11973,7 +12163,7 @@
         <v>29</v>
       </c>
       <c r="H188" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I188" s="18">
         <v>47</v>
@@ -12043,7 +12233,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:11" s="16" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" s="16" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>22</v>
@@ -12122,7 +12312,7 @@
         <v>30</v>
       </c>
       <c r="H193" s="41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I193" s="18">
         <v>22</v>
@@ -12415,7 +12605,7 @@
         <v>24</v>
       </c>
       <c r="J203" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K203" s="51">
         <v>30</v>
@@ -12477,7 +12667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12656,7 +12846,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>48</v>
@@ -12774,7 +12964,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>26</v>
@@ -12853,7 +13043,7 @@
         <v>30</v>
       </c>
       <c r="H218" s="41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I218" s="18">
         <v>26</v>
@@ -12893,7 +13083,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13072,7 +13262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13172,13 +13362,13 @@
         <v>29</v>
       </c>
       <c r="H229" s="41" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I229" s="18">
         <v>49</v>
       </c>
       <c r="J229" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K229" s="51">
         <v>30</v>
@@ -13268,7 +13458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13340,7 +13530,7 @@
         <v>29</v>
       </c>
       <c r="H235" s="41" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I235" s="18">
         <v>53</v>
@@ -13368,13 +13558,13 @@
         <v>29</v>
       </c>
       <c r="H236" s="41" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I236" s="18">
         <v>53</v>
       </c>
       <c r="J236" s="41" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K236" s="51">
         <v>30</v>
@@ -13426,7 +13616,7 @@
         <v>31</v>
       </c>
       <c r="H238" s="41" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I238" s="18">
         <v>53</v>
@@ -13566,7 +13756,7 @@
         <v>28</v>
       </c>
       <c r="J243" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K243" s="51">
         <v>28</v>
@@ -13630,7 +13820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A246" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>29</v>
@@ -14226,7 +14416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A266" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>38</v>
@@ -14276,7 +14466,7 @@
         <v>38</v>
       </c>
       <c r="J267" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K267" s="51">
         <v>28</v>
@@ -14502,7 +14692,7 @@
         <v>40</v>
       </c>
       <c r="J275" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K275" s="51">
         <v>28</v>
@@ -14706,7 +14896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="283" spans="1:11" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A283" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>41</v>
@@ -14756,7 +14946,7 @@
         <v>41</v>
       </c>
       <c r="J284" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K284" s="51">
         <v>28</v>
@@ -14950,7 +15140,7 @@
         <v>33</v>
       </c>
       <c r="J291" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K291" s="51">
         <v>28</v>
@@ -15882,7 +16072,7 @@
         <v>42</v>
       </c>
       <c r="J323" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K323" s="51">
         <v>28</v>
@@ -16086,7 +16276,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="331" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A331" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>43</v>
@@ -16108,7 +16298,7 @@
         <v>43</v>
       </c>
       <c r="J331" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K331" s="51">
         <v>28</v>
@@ -16355,7 +16545,7 @@
         <v>55</v>
       </c>
       <c r="J340" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K340" s="72">
         <v>38</v>
@@ -16437,7 +16627,7 @@
         <v>31</v>
       </c>
       <c r="H343" s="41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I343" s="70">
         <v>55</v>
@@ -16467,7 +16657,7 @@
         <v>31</v>
       </c>
       <c r="H344" s="41" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I344" s="70">
         <v>55</v>
@@ -16501,7 +16691,7 @@
         <v>55</v>
       </c>
       <c r="J345" s="71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K345" s="66">
         <v>38</v>
@@ -16523,7 +16713,7 @@
         <v>55</v>
       </c>
       <c r="F346" s="69" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H346" s="41"/>
       <c r="I346" s="70">
@@ -16647,7 +16837,7 @@
         <v>31</v>
       </c>
       <c r="H350" s="41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I350" s="70">
         <v>73</v>
@@ -16679,7 +16869,7 @@
         <v>31</v>
       </c>
       <c r="H351" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I351" s="70">
         <v>73</v>
@@ -16709,7 +16899,7 @@
         <v>31</v>
       </c>
       <c r="H352" s="41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I352" s="70">
         <v>73</v>
@@ -16733,7 +16923,7 @@
       <c r="D353" s="67"/>
       <c r="E353" s="68"/>
       <c r="F353" s="69" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H353" s="41"/>
       <c r="I353" s="70">
@@ -16818,13 +17008,13 @@
         <v>29</v>
       </c>
       <c r="H356" s="41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I356" s="70">
         <v>78</v>
       </c>
       <c r="J356" s="41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K356" s="66">
         <v>38</v>
@@ -16848,13 +17038,13 @@
         <v>30</v>
       </c>
       <c r="H357" s="41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I357" s="70">
         <v>78</v>
       </c>
       <c r="J357" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K357" s="66"/>
     </row>
@@ -16876,13 +17066,13 @@
         <v>31</v>
       </c>
       <c r="H358" s="41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I358" s="70">
         <v>78</v>
       </c>
       <c r="J358" s="71" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K358" s="66">
         <v>38</v>
@@ -16906,13 +17096,13 @@
         <v>31</v>
       </c>
       <c r="H359" s="41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I359" s="70">
         <v>78</v>
       </c>
       <c r="J359" s="71" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K359" s="66">
         <v>38</v>
@@ -16936,13 +17126,13 @@
         <v>31</v>
       </c>
       <c r="H360" s="41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I360" s="70">
         <v>78</v>
       </c>
       <c r="J360" s="71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K360" s="66">
         <v>38</v>
@@ -16964,7 +17154,7 @@
         <v>78</v>
       </c>
       <c r="F361" s="69" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H361" s="41"/>
       <c r="I361" s="70">
@@ -17056,7 +17246,7 @@
         <v>29</v>
       </c>
       <c r="H364" s="41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I364" s="70">
         <v>79</v>
@@ -17086,13 +17276,13 @@
         <v>30</v>
       </c>
       <c r="H365" s="41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I365" s="70">
         <v>79</v>
       </c>
       <c r="J365" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K365" s="66">
         <v>38</v>
@@ -17118,13 +17308,13 @@
         <v>31</v>
       </c>
       <c r="H366" s="41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I366" s="70">
         <v>79</v>
       </c>
       <c r="J366" s="71" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K366" s="66">
         <v>38</v>
@@ -17150,13 +17340,13 @@
         <v>31</v>
       </c>
       <c r="H367" s="41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I367" s="70">
         <v>79</v>
       </c>
       <c r="J367" s="71" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K367" s="66">
         <v>38</v>
@@ -17182,13 +17372,13 @@
         <v>31</v>
       </c>
       <c r="H368" s="41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I368" s="70">
         <v>79</v>
       </c>
       <c r="J368" s="71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K368" s="66">
         <v>38</v>
@@ -17200,7 +17390,7 @@
         <v>0</v>
       </c>
       <c r="B369" s="80" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C369" s="81"/>
       <c r="D369" s="82"/>
@@ -17223,7 +17413,7 @@
         <v>80</v>
       </c>
       <c r="B370" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C370" s="66" t="s">
         <v>57</v>
@@ -17249,7 +17439,7 @@
         <v>80</v>
       </c>
       <c r="B371" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C371" s="66" t="s">
         <v>57</v>
@@ -17267,7 +17457,7 @@
         <v>80</v>
       </c>
       <c r="J371" s="43" t="s">
-        <v>319</v>
+        <v>359</v>
       </c>
       <c r="K371" s="66">
         <v>60</v>
@@ -17279,7 +17469,7 @@
         <v>80</v>
       </c>
       <c r="B372" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C372" s="66" t="s">
         <v>57</v>
@@ -17291,7 +17481,7 @@
         <v>30</v>
       </c>
       <c r="H372" s="41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I372" s="70">
         <v>80</v>
@@ -17307,7 +17497,7 @@
         <v>80</v>
       </c>
       <c r="B373" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C373" s="66" t="s">
         <v>57</v>
@@ -17335,7 +17525,7 @@
         <v>81</v>
       </c>
       <c r="B374" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C374" s="66" t="s">
         <v>57</v>
@@ -17363,7 +17553,7 @@
         <v>81</v>
       </c>
       <c r="B375" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C375" s="66" t="s">
         <v>57</v>
@@ -17394,7 +17584,7 @@
         <v>81</v>
       </c>
       <c r="B376" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C376" s="66" t="s">
         <v>57</v>
@@ -17424,7 +17614,7 @@
         <v>81</v>
       </c>
       <c r="B377" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C377" s="66" t="s">
         <v>57</v>
@@ -17438,7 +17628,7 @@
         <v>31</v>
       </c>
       <c r="H377" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I377" s="70">
         <v>81</v>
@@ -17454,7 +17644,7 @@
         <v>81</v>
       </c>
       <c r="B378" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C378" s="66" t="s">
         <v>57</v>
@@ -17468,7 +17658,7 @@
         <v>31</v>
       </c>
       <c r="H378" s="41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I378" s="70">
         <v>81</v>
@@ -17484,7 +17674,7 @@
         <v>82</v>
       </c>
       <c r="B379" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C379" s="66" t="s">
         <v>57</v>
@@ -17512,7 +17702,7 @@
         <v>82</v>
       </c>
       <c r="B380" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C380" s="66" t="s">
         <v>57</v>
@@ -17543,7 +17733,7 @@
         <v>82</v>
       </c>
       <c r="B381" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C381" s="66" t="s">
         <v>57</v>
@@ -17557,7 +17747,7 @@
         <v>30</v>
       </c>
       <c r="H381" s="41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I381" s="70">
         <v>82</v>
@@ -17573,7 +17763,7 @@
         <v>82</v>
       </c>
       <c r="B382" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C382" s="66" t="s">
         <v>57</v>
@@ -17587,7 +17777,7 @@
         <v>31</v>
       </c>
       <c r="H382" s="41" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I382" s="70">
         <v>82</v>
@@ -17603,7 +17793,7 @@
         <v>82</v>
       </c>
       <c r="B383" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C383" s="66" t="s">
         <v>57</v>
@@ -17617,7 +17807,7 @@
         <v>31</v>
       </c>
       <c r="H383" s="41" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I383" s="70">
         <v>82</v>
@@ -17633,88 +17823,114 @@
         <v>83</v>
       </c>
       <c r="B384" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C384" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="D384" s="67"/>
+      <c r="D384" s="67" t="s">
+        <v>57</v>
+      </c>
       <c r="E384" s="68"/>
-      <c r="F384" s="6"/>
+      <c r="F384" s="6" t="s">
+        <v>363</v>
+      </c>
       <c r="G384" s="37"/>
       <c r="H384" s="41"/>
       <c r="I384" s="70">
         <v>83</v>
       </c>
-      <c r="J384" s="71"/>
+      <c r="J384" s="43"/>
       <c r="K384" s="66">
         <v>60</v>
       </c>
     </row>
-    <row r="385" spans="1:11" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:11" s="114" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A385" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>83</v>
       </c>
       <c r="B385" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C385" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="D385" s="67"/>
+      <c r="D385" s="67" t="s">
+        <v>57</v>
+      </c>
       <c r="E385" s="68"/>
       <c r="F385" s="6"/>
-      <c r="G385" s="37"/>
-      <c r="H385" s="41"/>
+      <c r="G385" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H385" s="41" t="s">
+        <v>365</v>
+      </c>
       <c r="I385" s="70">
         <v>83</v>
       </c>
-      <c r="J385" s="71"/>
+      <c r="J385" s="43" t="s">
+        <v>360</v>
+      </c>
       <c r="K385" s="66">
         <v>60</v>
       </c>
     </row>
-    <row r="386" spans="1:11" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:11" s="114" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>83</v>
       </c>
       <c r="B386" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C386" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="D386" s="67"/>
+      <c r="D386" s="67" t="s">
+        <v>57</v>
+      </c>
       <c r="E386" s="68"/>
       <c r="F386" s="6"/>
-      <c r="G386" s="37"/>
-      <c r="H386" s="41"/>
+      <c r="G386" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H386" s="41" t="s">
+        <v>366</v>
+      </c>
       <c r="I386" s="70">
         <v>83</v>
       </c>
-      <c r="J386" s="71"/>
+      <c r="J386" s="43" t="s">
+        <v>361</v>
+      </c>
       <c r="K386" s="66">
         <v>60</v>
       </c>
     </row>
-    <row r="387" spans="1:11" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:11" s="114" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A387" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>83</v>
       </c>
       <c r="B387" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C387" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="D387" s="67"/>
+      <c r="D387" s="67" t="s">
+        <v>57</v>
+      </c>
       <c r="E387" s="68"/>
       <c r="F387" s="6"/>
-      <c r="G387" s="37"/>
-      <c r="H387" s="41"/>
+      <c r="G387" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H387" s="41" t="s">
+        <v>362</v>
+      </c>
       <c r="I387" s="70">
         <v>83</v>
       </c>
@@ -17723,22 +17939,28 @@
         <v>60</v>
       </c>
     </row>
-    <row r="388" spans="1:11" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:11" s="114" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A388" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>83</v>
       </c>
       <c r="B388" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C388" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="D388" s="67"/>
+      <c r="D388" s="67" t="s">
+        <v>57</v>
+      </c>
       <c r="E388" s="68"/>
       <c r="F388" s="6"/>
-      <c r="G388" s="37"/>
-      <c r="H388" s="41"/>
+      <c r="G388" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H388" s="41" t="s">
+        <v>364</v>
+      </c>
       <c r="I388" s="70">
         <v>83</v>
       </c>
@@ -17750,21 +17972,25 @@
     <row r="389" spans="1:11" s="114" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>84</v>
+      </c>
+      <c r="B389" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="C389" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D389" s="67"/>
+      <c r="E389" s="68">
         <v>83</v>
       </c>
-      <c r="B389" s="65" t="s">
-        <v>352</v>
-      </c>
-      <c r="C389" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="D389" s="67"/>
-      <c r="E389" s="68"/>
-      <c r="F389" s="6"/>
+      <c r="F389" s="6" t="s">
+        <v>367</v>
+      </c>
       <c r="G389" s="37"/>
       <c r="H389" s="41"/>
       <c r="I389" s="70">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J389" s="71"/>
       <c r="K389" s="66">
@@ -17774,131 +18000,149 @@
     <row r="390" spans="1:11" s="114" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>84</v>
+      </c>
+      <c r="B390" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="C390" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D390" s="67"/>
+      <c r="E390" s="68">
         <v>83</v>
       </c>
-      <c r="B390" s="65" t="s">
-        <v>352</v>
-      </c>
-      <c r="C390" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="D390" s="67"/>
-      <c r="E390" s="68"/>
       <c r="F390" s="6"/>
-      <c r="G390" s="37"/>
-      <c r="H390" s="41"/>
+      <c r="G390" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H390" s="41" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",I385)</f>
+        <v>Result from scenario 83</v>
+      </c>
       <c r="I390" s="70">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J390" s="71"/>
       <c r="K390" s="66">
         <v>60</v>
       </c>
     </row>
-    <row r="391" spans="1:11" s="114" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:11" s="114" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>84</v>
+      </c>
+      <c r="B391" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="C391" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D391" s="67"/>
+      <c r="E391" s="68">
         <v>83</v>
       </c>
-      <c r="B391" s="65" t="s">
-        <v>352</v>
-      </c>
-      <c r="C391" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="D391" s="67"/>
-      <c r="E391" s="68"/>
       <c r="F391" s="6"/>
-      <c r="G391" s="37"/>
-      <c r="H391" s="41"/>
+      <c r="G391" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H391" s="41" t="s">
+        <v>368</v>
+      </c>
       <c r="I391" s="70">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J391" s="71"/>
       <c r="K391" s="66">
         <v>60</v>
       </c>
     </row>
-    <row r="392" spans="1:11" s="65" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A392" s="105">
-        <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>0</v>
-      </c>
-      <c r="B392" s="106" t="s">
-        <v>231</v>
-      </c>
-      <c r="C392" s="107"/>
-      <c r="D392" s="108"/>
-      <c r="E392" s="109"/>
-      <c r="F392" s="110"/>
-      <c r="G392" s="106"/>
-      <c r="H392" s="79" t="s">
-        <v>42</v>
-      </c>
-      <c r="I392" s="111"/>
-      <c r="J392" s="112" t="s">
-        <v>2</v>
-      </c>
-      <c r="K392" s="107">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="393" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:11" s="114" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A392" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>84</v>
+      </c>
+      <c r="B392" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="C392" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D392" s="67"/>
+      <c r="E392" s="68">
+        <v>83</v>
+      </c>
+      <c r="F392" s="6"/>
+      <c r="G392" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H392" s="41" t="s">
+        <v>369</v>
+      </c>
+      <c r="I392" s="70">
+        <v>84</v>
+      </c>
+      <c r="J392" s="71"/>
+      <c r="K392" s="66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" s="114" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A393" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B393" s="65" t="s">
-        <v>231</v>
+        <v>351</v>
       </c>
       <c r="C393" s="66" t="s">
         <v>57</v>
       </c>
       <c r="D393" s="67"/>
-      <c r="E393" s="68"/>
-      <c r="F393" s="69" t="s">
-        <v>231</v>
-      </c>
-      <c r="H393" s="41"/>
+      <c r="E393" s="68">
+        <v>83</v>
+      </c>
+      <c r="F393" s="6"/>
+      <c r="G393" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H393" s="41" t="s">
+        <v>354</v>
+      </c>
       <c r="I393" s="70">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="J393" s="71"/>
       <c r="K393" s="66">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="394" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A394" s="64">
-        <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>56</v>
-      </c>
-      <c r="B394" s="65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" s="65" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A394" s="105">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>0</v>
+      </c>
+      <c r="B394" s="106" t="s">
         <v>231</v>
       </c>
-      <c r="C394" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="D394" s="67"/>
-      <c r="E394" s="68"/>
-      <c r="F394" s="69"/>
-      <c r="G394" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H394" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="I394" s="70">
-        <v>56</v>
-      </c>
-      <c r="J394" s="43" t="s">
-        <v>319</v>
+      <c r="C394" s="107"/>
+      <c r="D394" s="108"/>
+      <c r="E394" s="109"/>
+      <c r="F394" s="110"/>
+      <c r="G394" s="106"/>
+      <c r="H394" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="I394" s="111"/>
+      <c r="J394" s="112" t="s">
+        <v>2</v>
       </c>
       <c r="K394" s="66">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="395" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A395" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -17911,13 +18155,10 @@
       </c>
       <c r="D395" s="67"/>
       <c r="E395" s="68"/>
-      <c r="F395" s="69"/>
-      <c r="G395" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H395" s="41" t="s">
-        <v>227</v>
-      </c>
+      <c r="F395" s="69" t="s">
+        <v>231</v>
+      </c>
+      <c r="H395" s="41"/>
       <c r="I395" s="70">
         <v>56</v>
       </c>
@@ -17926,7 +18167,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="396" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A396" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -17941,22 +18182,22 @@
       <c r="E396" s="68"/>
       <c r="F396" s="69"/>
       <c r="G396" s="65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H396" s="41" t="s">
-        <v>232</v>
+        <v>55</v>
       </c>
       <c r="I396" s="70">
         <v>56</v>
       </c>
-      <c r="J396" s="71" t="s">
-        <v>233</v>
+      <c r="J396" s="43" t="s">
+        <v>359</v>
       </c>
       <c r="K396" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="397" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A397" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>56</v>
@@ -17971,10 +18212,10 @@
       <c r="E397" s="68"/>
       <c r="F397" s="69"/>
       <c r="G397" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H397" s="41" t="s">
-        <v>131</v>
+        <v>227</v>
       </c>
       <c r="I397" s="70">
         <v>56</v>
@@ -17987,7 +18228,7 @@
     <row r="398" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A398" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B398" s="65" t="s">
         <v>231</v>
@@ -17996,25 +18237,28 @@
         <v>57</v>
       </c>
       <c r="D398" s="67"/>
-      <c r="E398" s="68">
+      <c r="E398" s="68"/>
+      <c r="F398" s="69"/>
+      <c r="G398" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H398" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="I398" s="70">
         <v>56</v>
       </c>
-      <c r="F398" s="69" t="s">
-        <v>240</v>
-      </c>
-      <c r="H398" s="41"/>
-      <c r="I398" s="70">
-        <v>57</v>
-      </c>
-      <c r="J398" s="71"/>
+      <c r="J398" s="71" t="s">
+        <v>233</v>
+      </c>
       <c r="K398" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="399" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A399" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B399" s="65" t="s">
         <v>231</v>
@@ -18023,19 +18267,16 @@
         <v>57</v>
       </c>
       <c r="D399" s="67"/>
-      <c r="E399" s="68">
-        <v>56</v>
-      </c>
+      <c r="E399" s="68"/>
       <c r="F399" s="69"/>
       <c r="G399" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H399" s="41" t="str">
-        <f>_xlfn.CONCAT("Result from scenario ",I394)</f>
-        <v>Result from scenario 56</v>
+        <v>31</v>
+      </c>
+      <c r="H399" s="41" t="s">
+        <v>131</v>
       </c>
       <c r="I399" s="70">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J399" s="71"/>
       <c r="K399" s="66">
@@ -18057,13 +18298,10 @@
       <c r="E400" s="68">
         <v>56</v>
       </c>
-      <c r="F400" s="69"/>
-      <c r="G400" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="H400" s="41" t="s">
-        <v>133</v>
-      </c>
+      <c r="F400" s="69" t="s">
+        <v>240</v>
+      </c>
+      <c r="H400" s="41"/>
       <c r="I400" s="70">
         <v>57</v>
       </c>
@@ -18072,7 +18310,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="401" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A401" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>57</v>
@@ -18089,10 +18327,11 @@
       </c>
       <c r="F401" s="69"/>
       <c r="G401" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H401" s="41" t="s">
-        <v>234</v>
+        <v>29</v>
+      </c>
+      <c r="H401" s="41" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",I396)</f>
+        <v>Result from scenario 56</v>
       </c>
       <c r="I401" s="70">
         <v>57</v>
@@ -18105,7 +18344,7 @@
     <row r="402" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A402" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B402" s="65" t="s">
         <v>231</v>
@@ -18115,24 +18354,27 @@
       </c>
       <c r="D402" s="67"/>
       <c r="E402" s="68">
-        <v>57</v>
-      </c>
-      <c r="F402" s="69" t="s">
-        <v>239</v>
-      </c>
-      <c r="H402" s="41"/>
+        <v>56</v>
+      </c>
+      <c r="F402" s="69"/>
+      <c r="G402" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="H402" s="41" t="s">
+        <v>133</v>
+      </c>
       <c r="I402" s="70">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J402" s="71"/>
       <c r="K402" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="403" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A403" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B403" s="65" t="s">
         <v>231</v>
@@ -18142,18 +18384,17 @@
       </c>
       <c r="D403" s="67"/>
       <c r="E403" s="68">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F403" s="69"/>
       <c r="G403" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H403" s="41" t="str">
-        <f>_xlfn.CONCAT("Result from scenario ",I398)</f>
-        <v>Result from scenario 57</v>
+        <v>31</v>
+      </c>
+      <c r="H403" s="41" t="s">
+        <v>234</v>
       </c>
       <c r="I403" s="70">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J403" s="71"/>
       <c r="K403" s="66">
@@ -18175,13 +18416,10 @@
       <c r="E404" s="68">
         <v>57</v>
       </c>
-      <c r="F404" s="69"/>
-      <c r="G404" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="H404" s="41" t="s">
-        <v>235</v>
-      </c>
+      <c r="F404" s="69" t="s">
+        <v>239</v>
+      </c>
+      <c r="H404" s="41"/>
       <c r="I404" s="70">
         <v>58</v>
       </c>
@@ -18207,10 +18445,11 @@
       </c>
       <c r="F405" s="69"/>
       <c r="G405" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H405" s="41" t="s">
-        <v>236</v>
+        <v>29</v>
+      </c>
+      <c r="H405" s="41" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",I400)</f>
+        <v>Result from scenario 57</v>
       </c>
       <c r="I405" s="70">
         <v>58</v>
@@ -18237,10 +18476,10 @@
       </c>
       <c r="F406" s="69"/>
       <c r="G406" s="65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H406" s="41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I406" s="70">
         <v>58</v>
@@ -18250,7 +18489,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="407" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A407" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>58</v>
@@ -18270,7 +18509,7 @@
         <v>31</v>
       </c>
       <c r="H407" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I407" s="70">
         <v>58</v>
@@ -18283,7 +18522,7 @@
     <row r="408" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A408" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B408" s="65" t="s">
         <v>231</v>
@@ -18293,24 +18532,27 @@
       </c>
       <c r="D408" s="67"/>
       <c r="E408" s="68">
-        <v>56</v>
-      </c>
-      <c r="F408" s="69" t="s">
-        <v>241</v>
-      </c>
-      <c r="H408" s="41"/>
+        <v>57</v>
+      </c>
+      <c r="F408" s="69"/>
+      <c r="G408" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H408" s="41" t="s">
+        <v>238</v>
+      </c>
       <c r="I408" s="70">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J408" s="71"/>
       <c r="K408" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="409" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A409" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B409" s="65" t="s">
         <v>231</v>
@@ -18320,18 +18562,17 @@
       </c>
       <c r="D409" s="67"/>
       <c r="E409" s="68">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F409" s="69"/>
       <c r="G409" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H409" s="41" t="str">
-        <f>_xlfn.CONCAT("Result from scenario ",I393)</f>
-        <v>Result from scenario 56</v>
+        <v>31</v>
+      </c>
+      <c r="H409" s="41" t="s">
+        <v>237</v>
       </c>
       <c r="I409" s="70">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J409" s="71"/>
       <c r="K409" s="66">
@@ -18353,13 +18594,10 @@
       <c r="E410" s="68">
         <v>56</v>
       </c>
-      <c r="F410" s="69"/>
-      <c r="G410" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="H410" s="41" t="s">
-        <v>144</v>
-      </c>
+      <c r="F410" s="69" t="s">
+        <v>241</v>
+      </c>
+      <c r="H410" s="41"/>
       <c r="I410" s="70">
         <v>59</v>
       </c>
@@ -18368,7 +18606,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="411" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A411" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>59</v>
@@ -18385,10 +18623,11 @@
       </c>
       <c r="F411" s="69"/>
       <c r="G411" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H411" s="41" t="s">
-        <v>186</v>
+        <v>29</v>
+      </c>
+      <c r="H411" s="41" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",I395)</f>
+        <v>Result from scenario 56</v>
       </c>
       <c r="I411" s="70">
         <v>59</v>
@@ -18401,34 +18640,37 @@
     <row r="412" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A412" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B412" s="65" t="s">
         <v>231</v>
       </c>
       <c r="C412" s="66" t="s">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="D412" s="67"/>
       <c r="E412" s="68">
-        <v>57</v>
-      </c>
-      <c r="F412" s="69" t="s">
-        <v>245</v>
-      </c>
-      <c r="H412" s="41"/>
+        <v>56</v>
+      </c>
+      <c r="F412" s="69"/>
+      <c r="G412" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="H412" s="41" t="s">
+        <v>144</v>
+      </c>
       <c r="I412" s="70">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J412" s="71"/>
       <c r="K412" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="413" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A413" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B413" s="65" t="s">
         <v>231</v>
@@ -18438,25 +18680,24 @@
       </c>
       <c r="D413" s="67"/>
       <c r="E413" s="68">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F413" s="69"/>
       <c r="G413" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H413" s="41" t="str">
-        <f>_xlfn.CONCAT("Result from scenario ",I398)</f>
-        <v>Result from scenario 57</v>
+        <v>31</v>
+      </c>
+      <c r="H413" s="41" t="s">
+        <v>186</v>
       </c>
       <c r="I413" s="70">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J413" s="71"/>
       <c r="K413" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="414" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A414" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -18465,19 +18706,16 @@
         <v>231</v>
       </c>
       <c r="C414" s="66" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
       <c r="D414" s="67"/>
       <c r="E414" s="68">
         <v>57</v>
       </c>
-      <c r="F414" s="69"/>
-      <c r="G414" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="H414" s="41" t="s">
-        <v>243</v>
-      </c>
+      <c r="F414" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="H414" s="41"/>
       <c r="I414" s="70">
         <v>60</v>
       </c>
@@ -18503,10 +18741,11 @@
       </c>
       <c r="F415" s="69"/>
       <c r="G415" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="H415" s="41" t="s">
-        <v>236</v>
+        <v>29</v>
+      </c>
+      <c r="H415" s="41" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",I400)</f>
+        <v>Result from scenario 57</v>
       </c>
       <c r="I415" s="70">
         <v>60</v>
@@ -18516,7 +18755,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="416" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A416" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -18533,10 +18772,10 @@
       </c>
       <c r="F416" s="69"/>
       <c r="G416" s="65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H416" s="41" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="I416" s="70">
         <v>60</v>
@@ -18546,7 +18785,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="417" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A417" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>60</v>
@@ -18566,7 +18805,7 @@
         <v>31</v>
       </c>
       <c r="H417" s="41" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="I417" s="70">
         <v>60</v>
@@ -18579,7 +18818,7 @@
     <row r="418" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A418" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B418" s="65" t="s">
         <v>231</v>
@@ -18588,23 +18827,28 @@
         <v>57</v>
       </c>
       <c r="D418" s="67"/>
-      <c r="E418" s="68"/>
-      <c r="F418" s="69" t="s">
-        <v>317</v>
-      </c>
-      <c r="H418" s="41"/>
+      <c r="E418" s="68">
+        <v>57</v>
+      </c>
+      <c r="F418" s="69"/>
+      <c r="G418" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H418" s="41" t="s">
+        <v>238</v>
+      </c>
       <c r="I418" s="70">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="J418" s="71"/>
       <c r="K418" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="419" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A419" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B419" s="65" t="s">
         <v>231</v>
@@ -18613,25 +18857,25 @@
         <v>57</v>
       </c>
       <c r="D419" s="67"/>
-      <c r="E419" s="68"/>
+      <c r="E419" s="68">
+        <v>57</v>
+      </c>
       <c r="F419" s="69"/>
       <c r="G419" s="65" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H419" s="41" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="I419" s="70">
-        <v>68</v>
-      </c>
-      <c r="J419" s="71" t="s">
-        <v>283</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="J419" s="71"/>
       <c r="K419" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="420" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A420" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>68</v>
@@ -18644,13 +18888,10 @@
       </c>
       <c r="D420" s="67"/>
       <c r="E420" s="68"/>
-      <c r="F420" s="69"/>
-      <c r="G420" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H420" s="41" t="s">
-        <v>282</v>
-      </c>
+      <c r="F420" s="69" t="s">
+        <v>317</v>
+      </c>
+      <c r="H420" s="41"/>
       <c r="I420" s="70">
         <v>68</v>
       </c>
@@ -18659,7 +18900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="421" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A421" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>68</v>
@@ -18677,17 +18918,19 @@
         <v>29</v>
       </c>
       <c r="H421" s="41" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="I421" s="70">
         <v>68</v>
       </c>
-      <c r="J421" s="71"/>
+      <c r="J421" s="71" t="s">
+        <v>283</v>
+      </c>
       <c r="K421" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="422" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A422" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>68</v>
@@ -18705,7 +18948,7 @@
         <v>29</v>
       </c>
       <c r="H422" s="41" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="I422" s="70">
         <v>68</v>
@@ -18730,10 +18973,10 @@
       <c r="E423" s="68"/>
       <c r="F423" s="69"/>
       <c r="G423" s="65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H423" s="41" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I423" s="70">
         <v>68</v>
@@ -18758,10 +19001,10 @@
       <c r="E424" s="68"/>
       <c r="F424" s="69"/>
       <c r="G424" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H424" s="41" t="s">
-        <v>238</v>
+        <v>133</v>
       </c>
       <c r="I424" s="70">
         <v>68</v>
@@ -18771,7 +19014,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="425" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A425" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>68</v>
@@ -18786,10 +19029,10 @@
       <c r="E425" s="68"/>
       <c r="F425" s="69"/>
       <c r="G425" s="65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H425" s="41" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
       <c r="I425" s="70">
         <v>68</v>
@@ -18799,7 +19042,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="426" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A426" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>68</v>
@@ -18817,7 +19060,7 @@
         <v>31</v>
       </c>
       <c r="H426" s="41" t="s">
-        <v>285</v>
+        <v>238</v>
       </c>
       <c r="I426" s="70">
         <v>68</v>
@@ -18827,10 +19070,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="427" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A427" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B427" s="65" t="s">
         <v>231</v>
@@ -18840,24 +19083,25 @@
       </c>
       <c r="D427" s="67"/>
       <c r="E427" s="68"/>
-      <c r="F427" s="69" t="s">
-        <v>305</v>
-      </c>
-      <c r="H427" s="41"/>
+      <c r="F427" s="69"/>
+      <c r="G427" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H427" s="41" t="s">
+        <v>284</v>
+      </c>
       <c r="I427" s="70">
-        <v>69</v>
-      </c>
-      <c r="J427" s="71" t="s">
-        <v>304</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="J427" s="71"/>
       <c r="K427" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="428" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A428" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B428" s="65" t="s">
         <v>231</v>
@@ -18869,20 +19113,20 @@
       <c r="E428" s="68"/>
       <c r="F428" s="69"/>
       <c r="G428" s="65" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H428" s="41" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="I428" s="70">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J428" s="71"/>
       <c r="K428" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="429" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A429" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>69</v>
@@ -18895,22 +19139,21 @@
       </c>
       <c r="D429" s="67"/>
       <c r="E429" s="68"/>
-      <c r="F429" s="69"/>
-      <c r="G429" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H429" s="41" t="s">
-        <v>282</v>
-      </c>
+      <c r="F429" s="69" t="s">
+        <v>305</v>
+      </c>
+      <c r="H429" s="41"/>
       <c r="I429" s="70">
         <v>69</v>
       </c>
-      <c r="J429" s="71"/>
+      <c r="J429" s="71" t="s">
+        <v>304</v>
+      </c>
       <c r="K429" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="430" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A430" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>69</v>
@@ -18928,7 +19171,7 @@
         <v>29</v>
       </c>
       <c r="H430" s="41" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="I430" s="70">
         <v>69</v>
@@ -18938,7 +19181,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="431" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A431" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>69</v>
@@ -18956,7 +19199,7 @@
         <v>29</v>
       </c>
       <c r="H431" s="41" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="I431" s="70">
         <v>69</v>
@@ -18984,7 +19227,7 @@
         <v>29</v>
       </c>
       <c r="H432" s="41" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I432" s="70">
         <v>69</v>
@@ -19009,10 +19252,10 @@
       <c r="E433" s="68"/>
       <c r="F433" s="69"/>
       <c r="G433" s="65" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="H433" s="41" t="s">
-        <v>307</v>
+        <v>133</v>
       </c>
       <c r="I433" s="70">
         <v>69</v>
@@ -19037,10 +19280,10 @@
       <c r="E434" s="68"/>
       <c r="F434" s="69"/>
       <c r="G434" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H434" s="41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I434" s="70">
         <v>69</v>
@@ -19050,7 +19293,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="435" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A435" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>69</v>
@@ -19065,10 +19308,10 @@
       <c r="E435" s="68"/>
       <c r="F435" s="69"/>
       <c r="G435" s="65" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H435" s="41" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="I435" s="70">
         <v>69</v>
@@ -19096,7 +19339,7 @@
         <v>31</v>
       </c>
       <c r="H436" s="41" t="s">
-        <v>303</v>
+        <v>238</v>
       </c>
       <c r="I436" s="70">
         <v>69</v>
@@ -19106,7 +19349,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="437" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A437" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>69</v>
@@ -19124,7 +19367,7 @@
         <v>31</v>
       </c>
       <c r="H437" s="41" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="I437" s="70">
         <v>69</v>
@@ -19137,7 +19380,7 @@
     <row r="438" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A438" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B438" s="65" t="s">
         <v>231</v>
@@ -19147,24 +19390,25 @@
       </c>
       <c r="D438" s="67"/>
       <c r="E438" s="68"/>
-      <c r="F438" s="69" t="s">
-        <v>309</v>
-      </c>
-      <c r="H438" s="41"/>
+      <c r="F438" s="69"/>
+      <c r="G438" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H438" s="41" t="s">
+        <v>303</v>
+      </c>
       <c r="I438" s="70">
-        <v>70</v>
-      </c>
-      <c r="J438" s="71" t="s">
-        <v>304</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J438" s="71"/>
       <c r="K438" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="439" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A439" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B439" s="65" t="s">
         <v>231</v>
@@ -19176,20 +19420,20 @@
       <c r="E439" s="68"/>
       <c r="F439" s="69"/>
       <c r="G439" s="65" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H439" s="41" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="I439" s="70">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J439" s="71"/>
       <c r="K439" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="440" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A440" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>70</v>
@@ -19202,22 +19446,21 @@
       </c>
       <c r="D440" s="67"/>
       <c r="E440" s="68"/>
-      <c r="F440" s="69"/>
-      <c r="G440" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H440" s="41" t="s">
-        <v>282</v>
-      </c>
+      <c r="F440" s="69" t="s">
+        <v>309</v>
+      </c>
+      <c r="H440" s="41"/>
       <c r="I440" s="70">
         <v>70</v>
       </c>
-      <c r="J440" s="71"/>
+      <c r="J440" s="71" t="s">
+        <v>304</v>
+      </c>
       <c r="K440" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="441" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A441" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>70</v>
@@ -19235,7 +19478,7 @@
         <v>29</v>
       </c>
       <c r="H441" s="41" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="I441" s="70">
         <v>70</v>
@@ -19245,7 +19488,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="442" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A442" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>70</v>
@@ -19263,7 +19506,7 @@
         <v>29</v>
       </c>
       <c r="H442" s="41" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="I442" s="70">
         <v>70</v>
@@ -19291,7 +19534,7 @@
         <v>29</v>
       </c>
       <c r="H443" s="41" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I443" s="70">
         <v>70</v>
@@ -19316,10 +19559,10 @@
       <c r="E444" s="68"/>
       <c r="F444" s="69"/>
       <c r="G444" s="65" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="H444" s="41" t="s">
-        <v>310</v>
+        <v>133</v>
       </c>
       <c r="I444" s="70">
         <v>70</v>
@@ -19344,10 +19587,10 @@
       <c r="E445" s="68"/>
       <c r="F445" s="69"/>
       <c r="G445" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H445" s="41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I445" s="70">
         <v>70</v>
@@ -19357,7 +19600,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="446" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A446" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>70</v>
@@ -19372,10 +19615,10 @@
       <c r="E446" s="68"/>
       <c r="F446" s="69"/>
       <c r="G446" s="65" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H446" s="41" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="I446" s="70">
         <v>70</v>
@@ -19403,7 +19646,7 @@
         <v>31</v>
       </c>
       <c r="H447" s="41" t="s">
-        <v>303</v>
+        <v>238</v>
       </c>
       <c r="I447" s="70">
         <v>70</v>
@@ -19413,7 +19656,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="448" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A448" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>70</v>
@@ -19431,7 +19674,7 @@
         <v>31</v>
       </c>
       <c r="H448" s="41" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="I448" s="70">
         <v>70</v>
@@ -19444,7 +19687,7 @@
     <row r="449" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A449" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B449" s="65" t="s">
         <v>231</v>
@@ -19454,24 +19697,25 @@
       </c>
       <c r="D449" s="67"/>
       <c r="E449" s="68"/>
-      <c r="F449" s="69" t="s">
-        <v>312</v>
-      </c>
-      <c r="H449" s="41"/>
+      <c r="F449" s="69"/>
+      <c r="G449" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H449" s="41" t="s">
+        <v>303</v>
+      </c>
       <c r="I449" s="70">
-        <v>71</v>
-      </c>
-      <c r="J449" s="71" t="s">
-        <v>283</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="J449" s="71"/>
       <c r="K449" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="450" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A450" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B450" s="65" t="s">
         <v>231</v>
@@ -19483,20 +19727,20 @@
       <c r="E450" s="68"/>
       <c r="F450" s="69"/>
       <c r="G450" s="65" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H450" s="41" t="s">
-        <v>281</v>
+        <v>311</v>
       </c>
       <c r="I450" s="70">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J450" s="71"/>
       <c r="K450" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="451" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A451" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>71</v>
@@ -19509,17 +19753,16 @@
       </c>
       <c r="D451" s="67"/>
       <c r="E451" s="68"/>
-      <c r="F451" s="69"/>
-      <c r="G451" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H451" s="41" t="s">
-        <v>313</v>
-      </c>
+      <c r="F451" s="69" t="s">
+        <v>312</v>
+      </c>
+      <c r="H451" s="41"/>
       <c r="I451" s="70">
         <v>71</v>
       </c>
-      <c r="J451" s="71"/>
+      <c r="J451" s="71" t="s">
+        <v>283</v>
+      </c>
       <c r="K451" s="66">
         <v>39</v>
       </c>
@@ -19542,7 +19785,7 @@
         <v>29</v>
       </c>
       <c r="H452" s="41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I452" s="70">
         <v>71</v>
@@ -19552,7 +19795,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="453" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A453" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>71</v>
@@ -19570,7 +19813,7 @@
         <v>29</v>
       </c>
       <c r="H453" s="41" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
       <c r="I453" s="70">
         <v>71</v>
@@ -19580,7 +19823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="454" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A454" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>71</v>
@@ -19595,10 +19838,10 @@
       <c r="E454" s="68"/>
       <c r="F454" s="69"/>
       <c r="G454" s="65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H454" s="41" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="I454" s="70">
         <v>71</v>
@@ -19623,10 +19866,10 @@
       <c r="E455" s="68"/>
       <c r="F455" s="69"/>
       <c r="G455" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H455" s="41" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I455" s="70">
         <v>71</v>
@@ -19636,7 +19879,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="456" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A456" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>71</v>
@@ -19651,10 +19894,10 @@
       <c r="E456" s="68"/>
       <c r="F456" s="69"/>
       <c r="G456" s="65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H456" s="41" t="s">
-        <v>284</v>
+        <v>133</v>
       </c>
       <c r="I456" s="70">
         <v>71</v>
@@ -19664,7 +19907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="457" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A457" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>71</v>
@@ -19682,7 +19925,7 @@
         <v>31</v>
       </c>
       <c r="H457" s="41" t="s">
-        <v>285</v>
+        <v>238</v>
       </c>
       <c r="I457" s="70">
         <v>71</v>
@@ -19692,10 +19935,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="458" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A458" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B458" s="65" t="s">
         <v>231</v>
@@ -19705,22 +19948,25 @@
       </c>
       <c r="D458" s="67"/>
       <c r="E458" s="68"/>
-      <c r="F458" s="69" t="s">
-        <v>314</v>
-      </c>
-      <c r="H458" s="41"/>
+      <c r="F458" s="69"/>
+      <c r="G458" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H458" s="41" t="s">
+        <v>284</v>
+      </c>
       <c r="I458" s="70">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J458" s="71"/>
       <c r="K458" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="459" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A459" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B459" s="65" t="s">
         <v>231</v>
@@ -19732,20 +19978,20 @@
       <c r="E459" s="68"/>
       <c r="F459" s="69"/>
       <c r="G459" s="65" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H459" s="41" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I459" s="70">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J459" s="71"/>
       <c r="K459" s="66">
         <v>39</v>
       </c>
     </row>
-    <row r="460" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A460" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>72</v>
@@ -19758,13 +20004,10 @@
       </c>
       <c r="D460" s="67"/>
       <c r="E460" s="68"/>
-      <c r="F460" s="69"/>
-      <c r="G460" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="H460" s="41" t="s">
-        <v>315</v>
-      </c>
+      <c r="F460" s="69" t="s">
+        <v>314</v>
+      </c>
+      <c r="H460" s="41"/>
       <c r="I460" s="70">
         <v>72</v>
       </c>
@@ -19791,7 +20034,7 @@
         <v>29</v>
       </c>
       <c r="H461" s="41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I461" s="70">
         <v>72</v>
@@ -19801,7 +20044,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="462" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A462" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>72</v>
@@ -19819,7 +20062,7 @@
         <v>29</v>
       </c>
       <c r="H462" s="41" t="s">
-        <v>232</v>
+        <v>315</v>
       </c>
       <c r="I462" s="70">
         <v>72</v>
@@ -19829,7 +20072,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="463" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A463" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>72</v>
@@ -19844,10 +20087,10 @@
       <c r="E463" s="68"/>
       <c r="F463" s="69"/>
       <c r="G463" s="65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H463" s="41" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="I463" s="70">
         <v>72</v>
@@ -19872,10 +20115,10 @@
       <c r="E464" s="68"/>
       <c r="F464" s="69"/>
       <c r="G464" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H464" s="41" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I464" s="70">
         <v>72</v>
@@ -19885,7 +20128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="465" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A465" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>72</v>
@@ -19900,10 +20143,10 @@
       <c r="E465" s="68"/>
       <c r="F465" s="69"/>
       <c r="G465" s="65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H465" s="41" t="s">
-        <v>316</v>
+        <v>133</v>
       </c>
       <c r="I465" s="70">
         <v>72</v>
@@ -19931,7 +20174,7 @@
         <v>31</v>
       </c>
       <c r="H466" s="41" t="s">
-        <v>285</v>
+        <v>238</v>
       </c>
       <c r="I466" s="70">
         <v>72</v>
@@ -19941,42 +20184,98 @@
         <v>39</v>
       </c>
     </row>
-    <row r="467" spans="1:11" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:11" s="65" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A467" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
-        <v>0</v>
-      </c>
-      <c r="B467" s="65"/>
-      <c r="C467" s="66"/>
+        <v>72</v>
+      </c>
+      <c r="B467" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="C467" s="66" t="s">
+        <v>57</v>
+      </c>
       <c r="D467" s="67"/>
       <c r="E467" s="68"/>
       <c r="F467" s="69"/>
-      <c r="G467" s="65"/>
-      <c r="H467" s="41"/>
-      <c r="I467" s="70"/>
+      <c r="G467" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H467" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="I467" s="70">
+        <v>72</v>
+      </c>
       <c r="J467" s="71"/>
-      <c r="K467" s="66"/>
-    </row>
-    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A468" s="61"/>
-      <c r="B468" s="1" t="s">
+      <c r="K467" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="468" spans="1:11" s="65" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A468" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>72</v>
+      </c>
+      <c r="B468" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="C468" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D468" s="67"/>
+      <c r="E468" s="68"/>
+      <c r="F468" s="69"/>
+      <c r="G468" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="H468" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="I468" s="70">
+        <v>72</v>
+      </c>
+      <c r="J468" s="71"/>
+      <c r="K468" s="66">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="469" spans="1:11" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A469" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>0</v>
+      </c>
+      <c r="B469" s="65"/>
+      <c r="C469" s="66"/>
+      <c r="D469" s="67"/>
+      <c r="E469" s="68"/>
+      <c r="F469" s="69"/>
+      <c r="G469" s="65"/>
+      <c r="H469" s="41"/>
+      <c r="I469" s="70"/>
+      <c r="J469" s="71"/>
+      <c r="K469" s="66"/>
+    </row>
+    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A470" s="61"/>
+      <c r="B470" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C468" s="3"/>
-      <c r="E468" s="10">
+      <c r="C470" s="3"/>
+      <c r="E470" s="10">
         <f>Table14[[#Totals],[Scenario '#]]</f>
-        <v>83</v>
-      </c>
-      <c r="F468" s="6"/>
-      <c r="H468" s="2"/>
-      <c r="I468" s="12">
+        <v>84</v>
+      </c>
+      <c r="F470" s="6"/>
+      <c r="H470" s="2"/>
+      <c r="I470" s="12">
         <f>SUBTOTAL(104,Table14[Scenario '#])</f>
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -19986,17 +20285,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="43" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="40" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -20008,7 +20307,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="colorScale" priority="102">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -20019,7 +20318,40 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G421:G1048576 G1:G345 G369 G392:G419">
+  <conditionalFormatting sqref="G423:G1048576 G1:G345 G369 G394:G421">
+    <cfRule type="cellIs" dxfId="48" priority="34" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="35" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="36" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G422">
+    <cfRule type="cellIs" dxfId="45" priority="31" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="32" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G346:G352">
+    <cfRule type="cellIs" dxfId="42" priority="28" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G353:G360">
     <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20030,7 +20362,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G420">
+  <conditionalFormatting sqref="G361:G363">
     <cfRule type="cellIs" dxfId="36" priority="22" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20041,7 +20373,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G346:G352">
+  <conditionalFormatting sqref="G364:G368">
     <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20052,7 +20384,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G353:G360">
+  <conditionalFormatting sqref="G370:G373">
     <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20063,7 +20395,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G361:G363">
+  <conditionalFormatting sqref="G374:G378">
     <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20074,7 +20406,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G364:G368">
+  <conditionalFormatting sqref="G379:G384 G388:G392">
     <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20085,7 +20417,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G370:G373">
+  <conditionalFormatting sqref="G385:G386">
     <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20096,7 +20428,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G374:G378">
+  <conditionalFormatting sqref="G387">
     <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20107,7 +20439,7 @@
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G379:G391">
+  <conditionalFormatting sqref="G393">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
@@ -20770,13 +21102,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="71" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22040,13 +22372,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="68" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22172,13 +22504,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22390,13 +22722,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22609,13 +22941,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22736,13 +23068,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22928,13 +23260,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23490,13 +23822,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Retested #79 and #80
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvanv\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4842B603-0A8F-4B80-9201-95A056D85C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAC4142-538B-47A6-849C-F95E6105B47D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="24510" windowHeight="15990" tabRatio="693" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="24510" windowHeight="15990" tabRatio="693" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200811" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,9 @@
     <sheet name="20201027" sheetId="11" r:id="rId9"/>
     <sheet name="20201028" sheetId="12" r:id="rId10"/>
     <sheet name="20201121" sheetId="13" r:id="rId11"/>
-    <sheet name="ATDD Scenarios" sheetId="3" r:id="rId12"/>
-    <sheet name="Questions" sheetId="2" r:id="rId13"/>
+    <sheet name="20201122" sheetId="14" r:id="rId12"/>
+    <sheet name="ATDD Scenarios" sheetId="3" r:id="rId13"/>
+    <sheet name="Questions" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="378">
   <si>
     <t>Scenario</t>
   </si>
@@ -1688,6 +1689,12 @@
   </si>
   <si>
     <t>Enter "New Feature"in empty control</t>
+  </si>
+  <si>
+    <t>To "Valid Then" belongs helper function CreateValidThen, this should be renamed to CreateRenamedValidThen, instead a call to MakeRenamedValidThen is created (with no comment and no helper function</t>
+  </si>
+  <si>
+    <t>cannot reproduce</t>
   </si>
 </sst>
 </file>
@@ -2382,7 +2389,78 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="211">
+  <dxfs count="229">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2474,6 +2552,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color rgb="FFC00000"/>
@@ -2492,26 +2590,6 @@
         <i val="0"/>
         <color rgb="FF0070C0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3147,6 +3225,92 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3310,43 +3474,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3706,268 +3833,290 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="210" dataDxfId="209">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="228" dataDxfId="227">
   <autoFilter ref="A1:F19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="208"/>
-    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="207"/>
-    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="206">
+    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="226"/>
+    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="225"/>
+    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="224">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="205">
+    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="223">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="204"/>
-    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="203"/>
+    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="222"/>
+    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="221"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145">
   <autoFilter ref="A1:H17" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="126">
+    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="144">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="124">
+    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="143"/>
+    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="142">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="123">
+    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="141">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="122"/>
-    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="120"/>
-    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="140"/>
+    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="138"/>
+    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="137"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{53B13E5C-5441-4B69-91E3-36B14A182343}" name="Table15691314" displayName="Table15691314" ref="A1:G75" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{53B13E5C-5441-4B69-91E3-36B14A182343}" name="Table15691314" displayName="Table15691314" ref="A1:G75" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
   <autoFilter ref="A1:G75" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF78A628-9C38-4564-9808-3B26AF234F77}" name="GitHub Issue" dataDxfId="116">
+    <tableColumn id="1" xr3:uid="{AF78A628-9C38-4564-9808-3B26AF234F77}" name="GitHub Issue" dataDxfId="134">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2CAB733F-F4E3-4B07-84CB-D00849F9BD6C}" name="#" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{0F5DE106-934C-4581-BEC9-F2BED1604D9A}" name="Feature" dataDxfId="114">
+    <tableColumn id="10" xr3:uid="{2CAB733F-F4E3-4B07-84CB-D00849F9BD6C}" name="#" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{0F5DE106-934C-4581-BEC9-F2BED1604D9A}" name="Feature" dataDxfId="132">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{211378E0-438E-4FA5-A4AE-A66A0C3D748F}" name="Scenario" dataDxfId="113">
+    <tableColumn id="3" xr3:uid="{211378E0-438E-4FA5-A4AE-A66A0C3D748F}" name="Scenario" dataDxfId="131">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{932BD0E7-22E6-4F2C-8057-85843CDDFC76}" name="Result" dataDxfId="112"/>
-    <tableColumn id="9" xr3:uid="{E6B98784-DB78-486D-B5E1-8E879B6CB05A}" name="Notes" dataDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{EF5B5B9D-C80C-4F4B-B547-BA970D46AED2}" name="Issue" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{932BD0E7-22E6-4F2C-8057-85843CDDFC76}" name="Result" dataDxfId="130"/>
+    <tableColumn id="9" xr3:uid="{E6B98784-DB78-486D-B5E1-8E879B6CB05A}" name="Notes" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{EF5B5B9D-C80C-4F4B-B547-BA970D46AED2}" name="Issue" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K478" totalsRowCount="1" headerRowDxfId="109" dataDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6AAF2E7-A1F3-4605-8BF9-A1BF72A0A475}" name="Table1569131415" displayName="Table1569131415" ref="A1:G11" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+  <autoFilter ref="A1:G11" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F2860C1F-2CAC-4F48-9D21-EE749371FC24}" name="GitHub Issue" dataDxfId="2">
+      <calculatedColumnFormula>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{C5E95249-B8EB-486E-8767-21D8F0A0A62C}" name="#" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{3D03DEE9-A69F-4186-9544-A9E1591B8341}" name="Feature" dataDxfId="1">
+      <calculatedColumnFormula>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{EBAA9733-8EE7-4AB7-AA6E-AD5B463DCCDB}" name="Scenario" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{B8D9077E-097D-43F7-AB61-3DC50B07F8DB}" name="Result" dataDxfId="104"/>
+    <tableColumn id="9" xr3:uid="{D33A8DD7-138F-48EF-8A7B-F7CF762853E4}" name="Notes" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{5957F9B4-6CFA-4A46-96FE-FA6B5AD2F680}" name="Issue" dataDxfId="102"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K478" totalsRowCount="1" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="A1:K477" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="100" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="125" totalsRowDxfId="19">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="99" totalsRowDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="98" totalsRowDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="97" totalsRowDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="96" totalsRowDxfId="6">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="124" totalsRowDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="123" totalsRowDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="122" totalsRowDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="121" totalsRowDxfId="15">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="95" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="94" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="93" totalsRowDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="92" totalsRowDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="91" totalsRowDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="90" totalsRowDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="120" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="119" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="118" totalsRowDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="117" totalsRowDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="116" totalsRowDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="115" totalsRowDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="107">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="114">
   <autoFilter ref="A1:F7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="202" dataDxfId="201">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="220" dataDxfId="219">
   <autoFilter ref="A1:F21" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="200"/>
-    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="199"/>
-    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="198">
+    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="218"/>
+    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="217"/>
+    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="216">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="197">
+    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="215">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="196"/>
-    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="195"/>
+    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="214"/>
+    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="213"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H56" totalsRowShown="0" headerRowDxfId="194" dataDxfId="193">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H56" totalsRowShown="0" headerRowDxfId="212" dataDxfId="211">
   <autoFilter ref="A1:H56" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="192"/>
-    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="191"/>
-    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="190">
+    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="210"/>
+    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="209"/>
+    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="208">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="189">
+    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="207">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="188"/>
-    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="187"/>
-    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="186"/>
-    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="185"/>
+    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="206"/>
+    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="205"/>
+    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="204"/>
+    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="203"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="184" dataDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="202" dataDxfId="201">
   <autoFilter ref="A1:F3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="182"/>
-    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="181"/>
-    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="180">
+    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="200"/>
+    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="199"/>
+    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="198">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="179">
+    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="197">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="178"/>
-    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="177"/>
+    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="196"/>
+    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="195"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="194" dataDxfId="193">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="174"/>
-    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="173"/>
-    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="172">
+    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="192"/>
+    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="191"/>
+    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="190">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="171">
+    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="189">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="170"/>
-    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="169"/>
-    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="168"/>
+    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="188"/>
+    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="187"/>
+    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="186"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
   <autoFilter ref="A1:H7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="165"/>
-    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="164"/>
-    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="163">
+    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="183"/>
+    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="182"/>
+    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="181">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="162">
+    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="180">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="161"/>
-    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="158"/>
+    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="179"/>
+    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="178"/>
+    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="177"/>
+    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="176"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H3" totalsRowShown="0" headerRowDxfId="157" dataDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H3" totalsRowShown="0" headerRowDxfId="175" dataDxfId="174">
   <autoFilter ref="A1:H3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="155"/>
-    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="154"/>
-    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="153">
+    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="173"/>
+    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="171">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="152">
+    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="170">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="151"/>
-    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="169"/>
+    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="168"/>
+    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="167"/>
+    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="165" dataDxfId="164">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
     <sortCondition ref="B1:B7"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="145"/>
-    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="144"/>
-    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="143">
+    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="163"/>
+    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="161">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="142">
+    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="160">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="140"/>
-    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="139"/>
+    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="159"/>
+    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="158"/>
+    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="157"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H20" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H20" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155">
   <autoFilter ref="A1:H20" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="136"/>
-    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="134">
+    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="154"/>
+    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="152">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="133">
+    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="151">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="132"/>
-    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="131"/>
-    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="130"/>
-    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="129"/>
+    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="150"/>
+    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="149"/>
+    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="148"/>
+    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="147"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4647,24 +4796,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E20:E1048576 E1:E17">
-    <cfRule type="cellIs" dxfId="89" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="86" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5101,13 +5250,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="59" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5129,8 +5278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AAAF6E-78DD-431A-8469-F0039B6C8AAD}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6788,13 +6937,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="9" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6818,11 +6967,349 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3776AF98-0090-4511-ADEE-DA882ECBACE1}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="90.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B2" s="8">
+        <v>24</v>
+      </c>
+      <c r="C2" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D2" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Then" to "Renamed Valid Then"</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="87">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B3" s="8">
+        <v>25</v>
+      </c>
+      <c r="C3" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D3" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Then" to "Renamed Valid Then" step 2a</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="87">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B4" s="8">
+        <v>26</v>
+      </c>
+      <c r="C4" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D4" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Revert Rename of Then</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="87">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B5" s="8">
+        <v>27</v>
+      </c>
+      <c r="C5" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D5" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Revert Rename of Then step 2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="87">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B6" s="8">
+        <v>48</v>
+      </c>
+      <c r="C6" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D6" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename "Valid Then" to "Renamed Valid Then" step 2b</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B7" s="8">
+        <v>49</v>
+      </c>
+      <c r="C7" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D7" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename prefix</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G7" s="87">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="B8" s="8">
+        <v>53</v>
+      </c>
+      <c r="C8" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Updating Then</v>
+      </c>
+      <c r="D8" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Rename duplicate Then</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="87"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="B9" s="8">
+        <v>56</v>
+      </c>
+      <c r="C9" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D9" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="B10" s="8">
+        <v>57</v>
+      </c>
+      <c r="C10" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D10" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario step 2a</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="B11" s="8">
+        <v>58</v>
+      </c>
+      <c r="C11" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Scenario</v>
+      </c>
+      <c r="D11" s="63" t="str">
+        <f>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Removing Scenario step 3a</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G11" s="87">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="7" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="8" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E11">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"N/A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="79" xr:uid="{9AF6A301-427B-4D65-AE20-92BC89FB3E04}"/>
+    <hyperlink ref="G3" r:id="rId2" display="79" xr:uid="{42D87E32-837E-4065-B25D-828BED3C65C7}"/>
+    <hyperlink ref="G4" r:id="rId3" display="79" xr:uid="{CD8164CF-83C5-4EF6-B598-93F03B26844F}"/>
+    <hyperlink ref="G5" r:id="rId4" display="79" xr:uid="{45CF0FFD-1899-4854-9441-05942DB1C911}"/>
+    <hyperlink ref="G7" r:id="rId5" display="51" xr:uid="{7A961CC3-5617-4A50-B6D7-CDBC57077F35}"/>
+    <hyperlink ref="G11" r:id="rId6" display="80" xr:uid="{E58F64F3-AB36-4760-94CC-34B583AB9D41}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <tableParts count="1">
+    <tablePart r:id="rId8"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
   <dimension ref="A1:K478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I476" sqref="I476"/>
+    <sheetView topLeftCell="B216" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H215" sqref="H215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -6996,7 +7483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5" outlineLevel="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="16.5" hidden="1" outlineLevel="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>1</v>
@@ -7022,7 +7509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30.75" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30.75" hidden="1" outlineLevel="2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>1</v>
@@ -7052,7 +7539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>1</v>
@@ -7082,7 +7569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>1</v>
@@ -7110,7 +7597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>1</v>
@@ -7138,7 +7625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>1</v>
@@ -7166,7 +7653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7195,7 +7682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A14" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7227,7 +7714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7260,7 +7747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A16" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7291,7 +7778,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A17" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7322,7 +7809,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>2</v>
@@ -7353,7 +7840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7379,7 +7866,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7409,7 +7896,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7439,7 +7926,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7467,7 +7954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7495,7 +7982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>3</v>
@@ -7525,7 +8012,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7551,7 +8038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7581,7 +8068,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7609,7 +8096,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7637,7 +8124,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7667,7 +8154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>8</v>
@@ -7695,7 +8182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7721,7 +8208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7751,7 +8238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7779,7 +8266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7807,7 +8294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7837,7 +8324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>64</v>
@@ -7865,7 +8352,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -7893,7 +8380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A38" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -7925,7 +8412,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -7955,7 +8442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -7985,7 +8472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A41" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -8015,7 +8502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A42" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -8047,7 +8534,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A43" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>66</v>
@@ -8079,7 +8566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -8105,7 +8592,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A45" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -8135,7 +8622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -8165,7 +8652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A47" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -8193,7 +8680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A48" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -8223,7 +8710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A49" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>10</v>
@@ -8251,7 +8738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8277,7 +8764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8307,7 +8794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8337,7 +8824,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8365,7 +8852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8393,7 +8880,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>12</v>
@@ -8423,7 +8910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8449,7 +8936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8479,7 +8966,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8507,7 +8994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8537,7 +9024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8565,7 +9052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8593,7 +9080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A62" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>14</v>
@@ -8621,7 +9108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8647,7 +9134,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8677,7 +9164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8705,7 +9192,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8735,7 +9222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8763,7 +9250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8791,7 +9278,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>61</v>
@@ -8819,7 +9306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A70" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>0</v>
@@ -12626,7 +13113,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="15.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A202" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>24</v>
@@ -12652,7 +13139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A203" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>24</v>
@@ -12682,7 +13169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A204" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>24</v>
@@ -12710,7 +13197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A205" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>24</v>
@@ -12738,7 +13225,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A206" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12766,7 +13253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A207" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12797,7 +13284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A208" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12827,7 +13314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A209" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12857,7 +13344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:11" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A210" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12887,7 +13374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A211" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>25</v>
@@ -12917,7 +13404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>48</v>
@@ -12945,7 +13432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A213" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>48</v>
@@ -12976,7 +13463,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A214" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>48</v>
@@ -12996,7 +13483,7 @@
         <v>30</v>
       </c>
       <c r="H214" s="41" t="s">
-        <v>198</v>
+        <v>353</v>
       </c>
       <c r="I214" s="18">
         <v>48</v>
@@ -13006,7 +13493,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A215" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>48</v>
@@ -13036,7 +13523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>26</v>
@@ -13064,7 +13551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A217" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>26</v>
@@ -13095,7 +13582,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A218" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>26</v>
@@ -13125,7 +13612,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="219" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A219" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>26</v>
@@ -13155,7 +13642,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A220" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13183,7 +13670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="221" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A221" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13214,7 +13701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A222" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13244,7 +13731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="223" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A223" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13274,7 +13761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A224" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13304,7 +13791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A225" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>27</v>
@@ -13334,7 +13821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A226" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13360,7 +13847,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A227" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13388,7 +13875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A228" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13416,7 +13903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A229" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13446,7 +13933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A230" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13474,7 +13961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A231" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13502,7 +13989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="45" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A232" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>49</v>
@@ -13530,7 +14017,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A233" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13556,7 +14043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="234" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A234" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13584,7 +14071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A235" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13612,7 +14099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A236" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13642,7 +14129,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="237" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A237" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13670,7 +14157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A238" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13698,7 +14185,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="239" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A239" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13726,7 +14213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="240" spans="1:11" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:11" ht="30.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>53</v>
@@ -13754,7 +14241,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="50">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>0</v>
@@ -20592,12 +21079,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="53" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="49" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="52" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="48" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20626,145 +21113,145 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G345 G369 G394:G421 G423:G474 G476:G1048576">
-    <cfRule type="cellIs" dxfId="51" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="40" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="41" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="42" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G422">
-    <cfRule type="cellIs" dxfId="48" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="37" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="38" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="39" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G346:G352">
-    <cfRule type="cellIs" dxfId="45" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="34" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="35" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="36" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G353:G360">
-    <cfRule type="cellIs" dxfId="42" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="31" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="32" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="33" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G361:G363">
-    <cfRule type="cellIs" dxfId="39" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="28" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="29" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="30" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G364:G368">
-    <cfRule type="cellIs" dxfId="36" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="25" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="26" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="27" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G370:G373">
-    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="23" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G374:G378">
-    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="21" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G379:G384 G388:G392">
-    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="16" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="18" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G385:G386">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G387">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="12" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G393">
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20776,7 +21263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB16863-C9D6-47DE-82AF-06BDE2CF5BC1}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -20924,10 +21411,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"Solved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21420,13 +21907,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22690,13 +23177,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22822,13 +23309,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23040,13 +23527,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23259,13 +23746,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="71" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23386,13 +23873,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="68" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23578,13 +24065,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="65" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24140,13 +24627,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="62" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added test for #62. Tested and not OK.
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE52D6F-615D-4279-8E75-83207DFED34A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9012FC-BE0D-4CED-BB3D-B26323E4951E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="255" windowWidth="25440" windowHeight="15990" tabRatio="888" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,6 @@
     <sheet name="20200811" sheetId="1" r:id="rId16"/>
     <sheet name="Questions" sheetId="2" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId18"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="438">
   <si>
     <t>Scenario</t>
   </si>
@@ -1635,9 +1632,6 @@
     <t>Rename "Second Test function in existing test codeunit with valid Given-When-Then structure" to "Third Test function in existing test codeunit with valid Given-When-Then structure" and confirm</t>
   </si>
   <si>
-    <t>User selects first scenario line of existing test codeunit in ATDD.TestScriptor page</t>
-  </si>
-  <si>
     <t>Added scenario "New Scenario (2)"</t>
   </si>
   <si>
@@ -1660,9 +1654,6 @@
   </si>
   <si>
     <t>User confirms removal of helper function(s)</t>
-  </si>
-  <si>
-    <t>Scenario is removed from ATDD.TestScriptor page</t>
   </si>
   <si>
     <t>Scenario is removed from test codeunit</t>
@@ -1726,9 +1717,6 @@
     <t>Test codeunit with one Test function in existing test codeunit with valid Given-When-Then structure and call to Initialize</t>
   </si>
   <si>
-    <t>User selects this scenario line in ATDD.TestScriptor page</t>
-  </si>
-  <si>
     <t>All Given/When/Then helper functions related to scenario are removed from test codeunit</t>
   </si>
   <si>
@@ -1863,9 +1851,6 @@
     <t>User adds Feature "New Feature"</t>
   </si>
   <si>
-    <t>New line appears on ATDD.TestScriptor page with FEATURE/SCENARIO "New Feature"/"New Test Procedure"</t>
-  </si>
-  <si>
     <t>Scenario change is reverted</t>
   </si>
   <si>
@@ -1887,16 +1872,58 @@
     <t>Enter "New Feature !@#$%^&amp;*()" in empty control</t>
   </si>
   <si>
-    <t>New line appears on ATDD.TestScriptor page with FEATURE/SCENARIO "New Feature !@#$%^&amp;*()"/"New Test Procedure"</t>
-  </si>
-  <si>
-    <t>Add Given "new feature all lowercase"</t>
-  </si>
-  <si>
-    <t>New line appears on ATDD.TestScriptor page with FEATURE/SCENARIO "new feature all lowercase)"/"New Test Procedure"</t>
-  </si>
-  <si>
     <t>New test codeunit was created with name "NewFeatureAllLowercase", test function NewTestProcedure with call to Intitialize helper and Initialize helper function</t>
+  </si>
+  <si>
+    <t>Enter "new feature all lowercase" in empty control</t>
+  </si>
+  <si>
+    <t>Removing Feature</t>
+  </si>
+  <si>
+    <t>[FEATURE] "First test object" in codeunit 50100 TestObjectFLX</t>
+  </si>
+  <si>
+    <t>Remove "First test object" by clicking on garbage can icon</t>
+  </si>
+  <si>
+    <t>Remove Feature</t>
+  </si>
+  <si>
+    <t>Remove Feature step 2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "First test object" is removed from Features pane in ATTD.TestScriptor page</t>
+  </si>
+  <si>
+    <t>User selects green Features control on TestScriptor to open Features pane</t>
+  </si>
+  <si>
+    <t>User selects first scenario line of existing test codeunit in TestScriptor</t>
+  </si>
+  <si>
+    <t>Scenario is removed from TestScriptor</t>
+  </si>
+  <si>
+    <t>User selects this scenario line in TestScriptor</t>
+  </si>
+  <si>
+    <t>New line appears on TestScriptor with FEATURE/SCENARIO "New Feature"/"New Test Procedure"</t>
+  </si>
+  <si>
+    <t>New line appears on TestScriptor with FEATURE/SCENARIO "New Feature !@#$%^&amp;*()"/"New Test Procedure"</t>
+  </si>
+  <si>
+    <t>New line appears on TestScriptor with FEATURE/SCENARIO "new feature all lowercase)"/"New Test Procedure"</t>
+  </si>
+  <si>
+    <t>All lines with FEATURE "First test object" are removed from TestScriptor</t>
+  </si>
+  <si>
+    <t>then</t>
+  </si>
+  <si>
+    <t>Codeunit file containing FEATURE "First test object" is removed</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2086,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2122,6 +2149,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2216,7 +2249,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2576,124 +2609,37 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="272">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="250">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3247,26 +3193,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color rgb="FF0070C0"/>
@@ -3307,25 +3233,26 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3349,42 +3276,100 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
+        <color rgb="FF9C5700"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFC00000"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF00B050"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3479,278 +3464,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4248,6 +3961,172 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4266,408 +4145,363 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ATDD Scenarios"/>
-      <sheetName val="20210130"/>
-      <sheetName val="20210121"/>
-      <sheetName val="20201128"/>
-      <sheetName val="20201122"/>
-      <sheetName val="20201121"/>
-      <sheetName val="20201028"/>
-      <sheetName val="20201027"/>
-      <sheetName val="20201014"/>
-      <sheetName val="20201013"/>
-      <sheetName val="20201005"/>
-      <sheetName val="20200930"/>
-      <sheetName val="20200925"/>
-      <sheetName val="20200924"/>
-      <sheetName val="20200817"/>
-      <sheetName val="20200811"/>
-      <sheetName val="Questions"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K558" totalsRowCount="1" headerRowDxfId="271" dataDxfId="270">
-  <autoFilter ref="A1:K557" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:K570" totalsRowCount="1" headerRowDxfId="249" dataDxfId="248">
+  <autoFilter ref="A1:K569" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="125" totalsRowDxfId="17">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="247" totalsRowDxfId="81">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="124" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="123" totalsRowDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="122" totalsRowDxfId="14"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="121" totalsRowDxfId="13">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="246" totalsRowDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="245" totalsRowDxfId="79"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="244" totalsRowDxfId="78"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="243" totalsRowDxfId="77">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="120" totalsRowDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="119" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="118" totalsRowDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="117" totalsRowDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="116" totalsRowDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="115" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="242" totalsRowDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="241" totalsRowDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="240" totalsRowDxfId="74"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="239" totalsRowDxfId="73"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="238" totalsRowDxfId="72"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="237" totalsRowDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H3" totalsRowShown="0" headerRowDxfId="195" dataDxfId="194">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0878DA4D-3CB5-4619-9A0A-599FABB7DC57}" name="Table15610" displayName="Table15610" ref="A1:H3" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
   <autoFilter ref="A1:H3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="193"/>
-    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="192"/>
-    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="191">
+    <tableColumn id="1" xr3:uid="{C6EFDEDE-76B4-4209-B4EC-DA1A18EB1E97}" name="GitHub Issue" dataDxfId="160"/>
+    <tableColumn id="10" xr3:uid="{098AFD04-1402-4D76-99F4-42E88291CD78}" name="#" dataDxfId="159"/>
+    <tableColumn id="2" xr3:uid="{A22ED63C-C67C-4B00-9624-32C3F944037E}" name="Feature" dataDxfId="158">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="190">
+    <tableColumn id="3" xr3:uid="{0FA99C46-646D-4E8F-B0BF-1140AA37D40A}" name="Scenario" dataDxfId="157">
       <calculatedColumnFormula>VLOOKUP(Table15610[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="189"/>
-    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="188"/>
-    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="187"/>
-    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="186"/>
+    <tableColumn id="7" xr3:uid="{5BC9D45B-40F1-46DC-B2C7-78D14AACF783}" name="Result" dataDxfId="156"/>
+    <tableColumn id="9" xr3:uid="{A9EC8C02-2838-4482-9A0B-CA631C93AC74}" name="Notes" dataDxfId="155"/>
+    <tableColumn id="4" xr3:uid="{E96BEF3B-15D4-4559-8F93-2C643E06E8D1}" name="Issue" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{97AE6093-DFB3-42D0-B2E6-8E88C3C12FA7}" name="Issue 2" dataDxfId="153"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84A32EDF-0443-4988-8345-B50349BD0E2C}" name="Table1569" displayName="Table1569" ref="A1:H7" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
   <autoFilter ref="A1:H7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="183"/>
-    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="181">
+    <tableColumn id="1" xr3:uid="{248814DF-5555-48D1-9D24-25C77E412F33}" name="GitHub Issue" dataDxfId="150"/>
+    <tableColumn id="10" xr3:uid="{DAC0FF69-4A7B-44B9-8A64-DFAA331BA6B1}" name="#" dataDxfId="149"/>
+    <tableColumn id="2" xr3:uid="{C47ECF80-F072-49CE-92EE-000858F57C33}" name="Feature" dataDxfId="148">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="180">
+    <tableColumn id="3" xr3:uid="{FCE57A87-2CF1-4AE6-AFB5-A6F87E64A8A7}" name="Scenario" dataDxfId="147">
       <calculatedColumnFormula>VLOOKUP(Table1569[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="179"/>
-    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="176"/>
+    <tableColumn id="7" xr3:uid="{6DD95B02-B080-42ED-B11F-42AF08CA790D}" name="Result" dataDxfId="146"/>
+    <tableColumn id="9" xr3:uid="{BA282B2B-17BD-4261-9760-F2A925429F7A}" name="Notes" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{0183AB17-AE90-4F38-BCEF-5EDD0F7F69C4}" name="Issue" dataDxfId="144"/>
+    <tableColumn id="5" xr3:uid="{6F37CA82-D4F1-4817-A998-D7062FF308E8}" name="Issue 2" dataDxfId="143"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="175" dataDxfId="174">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8B897917-DF76-417A-9052-CAD936FCC4FA}" name="Table1568" displayName="Table1568" ref="A1:G7" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="173"/>
-    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="172"/>
-    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="171">
+    <tableColumn id="1" xr3:uid="{DFA97F91-F25D-410C-A738-818C1315CE90}" name="GitHub Issue" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{8A423300-CF45-42DD-9AF6-E565A7CBEE15}" name="#" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{A58FE8A3-D520-4C85-914A-401B76F604A6}" name="Feature" dataDxfId="138">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="170">
+    <tableColumn id="3" xr3:uid="{8FD6A196-893D-483F-BF09-DF7AE9ACEE4A}" name="Scenario" dataDxfId="137">
       <calculatedColumnFormula>VLOOKUP(Table1568[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="169"/>
-    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="168"/>
-    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="167"/>
+    <tableColumn id="7" xr3:uid="{7BE5BF66-1736-41B3-815E-22C1DAA5E223}" name="Result" dataDxfId="136"/>
+    <tableColumn id="9" xr3:uid="{99539950-BFFA-452F-AA77-25B9B87A9CBF}" name="Notes" dataDxfId="135"/>
+    <tableColumn id="4" xr3:uid="{775459C3-4D9D-4D39-8F6A-F5DCF4903870}" name="Issue" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{780C6028-726C-4E93-B91B-EA6388173E09}" name="Table1567" displayName="Table1567" ref="A1:F3" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132">
   <autoFilter ref="A1:F3" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="164"/>
-    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="163"/>
-    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="162">
+    <tableColumn id="1" xr3:uid="{94C77221-7074-4F1C-A74C-5E453E4BFC90}" name="GitHub Issue" dataDxfId="131"/>
+    <tableColumn id="10" xr3:uid="{13D7D9D4-76B1-4C39-BB48-F4BE5FCA510E}" name="#" dataDxfId="130"/>
+    <tableColumn id="2" xr3:uid="{F0CE7E7A-B26F-463D-BFEC-A7D26F66E924}" name="Feature" dataDxfId="129">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="161">
+    <tableColumn id="3" xr3:uid="{EC4230E9-2E23-4E05-8AC2-BBCD98169A66}" name="Scenario" dataDxfId="128">
       <calculatedColumnFormula>VLOOKUP(Table1567[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="160"/>
-    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="159"/>
+    <tableColumn id="7" xr3:uid="{9B22461A-D8F9-4348-BA40-9D96FF1E5CAE}" name="Result" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{E1ED6C50-B858-4476-B39D-6499153902DD}" name="Notes" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H56" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9AAA7B7D-0F02-47E8-8021-590D6C529FA2}" name="Table156" displayName="Table156" ref="A1:H56" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="A1:H56" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="156"/>
-    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="155"/>
-    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="154">
+    <tableColumn id="1" xr3:uid="{62FA5252-C97E-479F-BD0E-51EB8F86927E}" name="GitHub Issue" dataDxfId="123"/>
+    <tableColumn id="10" xr3:uid="{88279534-B9B2-45EF-85ED-48B0CB30B0FC}" name="#" dataDxfId="122"/>
+    <tableColumn id="2" xr3:uid="{65C1E46E-678E-4257-B598-65E6C48B5518}" name="Feature" dataDxfId="121">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="153">
+    <tableColumn id="3" xr3:uid="{9BDB295D-43E6-4149-9BDB-0C68EF5BEA4F}" name="Scenario" dataDxfId="120">
       <calculatedColumnFormula>VLOOKUP(Table156[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="152"/>
-    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="150"/>
-    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="149"/>
+    <tableColumn id="7" xr3:uid="{3D6CA3EE-871F-49D7-AEA4-105F31214D8D}" name="Result" dataDxfId="119"/>
+    <tableColumn id="9" xr3:uid="{08CE583F-3E90-4BB7-9FD0-B61300756B3F}" name="Notes" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{ED4FF26B-7742-450D-A2C7-E28622E770A8}" name="Issue" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{8C2A13FB-6FA9-473F-8411-E2953BA508DA}" name="Issue 2" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{244B00F4-A283-4C03-A548-5D414192658A}" name="Table15" displayName="Table15" ref="A1:F21" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
   <autoFilter ref="A1:F21" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="146"/>
-    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="145"/>
-    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="144">
+    <tableColumn id="1" xr3:uid="{C88BBA8B-13D1-4F8C-8228-1F627ECA93F3}" name="GitHub Issue" dataDxfId="113"/>
+    <tableColumn id="10" xr3:uid="{C17894F7-82C1-41F9-A109-9D2BE65F4A6B}" name="#" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{B20FB9C3-EBA7-4961-B8F0-A6492DB4ECA8}" name="Feature" dataDxfId="111">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="143">
+    <tableColumn id="3" xr3:uid="{DB9C27DA-5910-400F-AEF3-F7CB64F76112}" name="Scenario" dataDxfId="110">
       <calculatedColumnFormula>VLOOKUP(Table15[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="142"/>
-    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="141"/>
+    <tableColumn id="7" xr3:uid="{EE5D19B8-A5A9-46A0-9116-C9340A380AE6}" name="Result" dataDxfId="109"/>
+    <tableColumn id="9" xr3:uid="{EE39F3A9-2DC0-4B72-8030-6BA6C4137552}" name="Notes" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{549C6A2B-5218-4DC2-B34E-4FA680434377}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:F19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="138"/>
-    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="137"/>
-    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="136">
+    <tableColumn id="1" xr3:uid="{87974612-E18C-48A1-9664-C54B638536B0}" name="GitHub Issue" dataDxfId="105"/>
+    <tableColumn id="10" xr3:uid="{F6A07010-F1E9-4910-AF3B-6F8DF5829579}" name="#" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{02982BB0-7410-4185-8CF1-D0B4FA55AF99}" name="Feature" dataDxfId="103">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="135">
+    <tableColumn id="3" xr3:uid="{DEA89800-56FD-4648-9748-AFB5CE1C3B9D}" name="Scenario" dataDxfId="102">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="134"/>
-    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="133"/>
+    <tableColumn id="7" xr3:uid="{777A3026-0C2D-4E8E-87BB-6E1E61B95CE5}" name="Result" dataDxfId="101"/>
+    <tableColumn id="9" xr3:uid="{A29A313E-BA52-41CC-802A-A04F1DB6E8D8}" name="Notes" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="99">
   <autoFilter ref="A1:F7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="130"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="129"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="128"/>
-    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="127"/>
-    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{0CA1625E-B949-475F-AD44-FA7F1E12DD0E}" name="Table156913141718" displayName="Table156913141718" ref="A1:G89" totalsRowCount="1" headerRowDxfId="269" dataDxfId="268">
-  <autoFilter ref="A1:G88" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{0CA1625E-B949-475F-AD44-FA7F1E12DD0E}" name="Table156913141718" displayName="Table156913141718" ref="A1:G91" totalsRowCount="1" headerRowDxfId="236" dataDxfId="235">
+  <autoFilter ref="A1:G90" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}">
     <filterColumn colId="0">
       <filters>
-        <filter val="61"/>
+        <filter val="62"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1A8599FD-1C61-41AF-A7FB-6EDD5FDE3FEB}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="267" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{1A8599FD-1C61-41AF-A7FB-6EDD5FDE3FEB}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="234" totalsRowDxfId="67">
       <calculatedColumnFormula>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1377C3C6-C300-4847-B79A-1D0F6C2AE0CC}" name="#" totalsRowFunction="max" dataDxfId="266" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{39AAC1D7-9EAD-4B4E-BA0A-8AB521EE839B}" name="Feature" totalsRowFunction="count" dataDxfId="265" totalsRowDxfId="4">
+    <tableColumn id="10" xr3:uid="{1377C3C6-C300-4847-B79A-1D0F6C2AE0CC}" name="#" totalsRowFunction="max" dataDxfId="233" totalsRowDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{39AAC1D7-9EAD-4B4E-BA0A-8AB521EE839B}" name="Feature" totalsRowFunction="count" dataDxfId="232" totalsRowDxfId="65">
       <calculatedColumnFormula>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F0AB1435-8452-4B63-9569-71273D4BAC2D}" name="Scenario" dataDxfId="264" totalsRowDxfId="3">
+    <tableColumn id="3" xr3:uid="{F0AB1435-8452-4B63-9569-71273D4BAC2D}" name="Scenario" dataDxfId="231" totalsRowDxfId="64">
       <calculatedColumnFormula>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DAB7B1B6-F4C7-4D28-9FF3-B53BE65BB3B2}" name="Result" totalsRowFunction="count" dataDxfId="263" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{EDAE2678-FD2D-44B6-9DD0-DE034D9542CC}" name="Notes" dataDxfId="262" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{61EA8510-A09F-4B09-9021-5721F13CCBF8}" name="Issue" totalsRowFunction="count" dataDxfId="261" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{DAB7B1B6-F4C7-4D28-9FF3-B53BE65BB3B2}" name="Result" totalsRowFunction="count" dataDxfId="230" totalsRowDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{EDAE2678-FD2D-44B6-9DD0-DE034D9542CC}" name="Notes" dataDxfId="229" totalsRowDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{61EA8510-A09F-4B09-9021-5721F13CCBF8}" name="Issue" totalsRowFunction="count" dataDxfId="228" totalsRowDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CD807E79-84C6-4174-92DA-26DB54E8608E}" name="Table1569131417" displayName="Table1569131417" ref="A1:G2" totalsRowShown="0" headerRowDxfId="260" dataDxfId="259">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CD807E79-84C6-4174-92DA-26DB54E8608E}" name="Table1569131417" displayName="Table1569131417" ref="A1:G2" totalsRowShown="0" headerRowDxfId="227" dataDxfId="226">
   <autoFilter ref="A1:G2" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{673102FE-495C-4F59-87B9-0B59EF49F20F}" name="GitHub Issue" dataDxfId="258">
+    <tableColumn id="1" xr3:uid="{673102FE-495C-4F59-87B9-0B59EF49F20F}" name="GitHub Issue" dataDxfId="225">
       <calculatedColumnFormula>VLOOKUP(Table1569131417[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5979941B-1711-4D7C-8B8E-50A457816369}" name="#" dataDxfId="257"/>
-    <tableColumn id="2" xr3:uid="{A93EBCE7-5EE0-4459-AE49-29CC32041F78}" name="Feature" dataDxfId="256">
+    <tableColumn id="10" xr3:uid="{5979941B-1711-4D7C-8B8E-50A457816369}" name="#" dataDxfId="224"/>
+    <tableColumn id="2" xr3:uid="{A93EBCE7-5EE0-4459-AE49-29CC32041F78}" name="Feature" dataDxfId="223">
       <calculatedColumnFormula>VLOOKUP(Table1569131417[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3E240C7B-3FDF-455F-B3F9-1D16F0FA84E2}" name="Scenario" dataDxfId="255">
+    <tableColumn id="3" xr3:uid="{3E240C7B-3FDF-455F-B3F9-1D16F0FA84E2}" name="Scenario" dataDxfId="222">
       <calculatedColumnFormula>VLOOKUP(Table1569131417[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{73149383-24BF-4083-B896-7E4F67AF994B}" name="Result" dataDxfId="254"/>
-    <tableColumn id="9" xr3:uid="{F7A64097-CB13-478B-B07A-D0A3F3C1AA76}" name="Notes" dataDxfId="253"/>
-    <tableColumn id="4" xr3:uid="{6F45352D-9D31-446D-A797-1ED8F59729D4}" name="Issue" dataDxfId="252"/>
+    <tableColumn id="7" xr3:uid="{73149383-24BF-4083-B896-7E4F67AF994B}" name="Result" dataDxfId="221"/>
+    <tableColumn id="9" xr3:uid="{F7A64097-CB13-478B-B07A-D0A3F3C1AA76}" name="Notes" dataDxfId="220"/>
+    <tableColumn id="4" xr3:uid="{6F45352D-9D31-446D-A797-1ED8F59729D4}" name="Issue" dataDxfId="219"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{D0EFC6B3-167C-4D39-B64D-E3BD46D148CB}" name="Table156913141516" displayName="Table156913141516" ref="A1:G5" totalsRowShown="0" headerRowDxfId="251" dataDxfId="250">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{D0EFC6B3-167C-4D39-B64D-E3BD46D148CB}" name="Table156913141516" displayName="Table156913141516" ref="A1:G5" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217">
   <autoFilter ref="A1:G5" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{841C50AF-62ED-40B6-A5EA-BCC2B893F03A}" name="GitHub Issue" dataDxfId="249">
+    <tableColumn id="1" xr3:uid="{841C50AF-62ED-40B6-A5EA-BCC2B893F03A}" name="GitHub Issue" dataDxfId="216">
       <calculatedColumnFormula>VLOOKUP(Table156913141516[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F503BC1B-7DB8-4002-ABF1-58ABE89E1830}" name="#" dataDxfId="248"/>
-    <tableColumn id="2" xr3:uid="{C571017F-6C16-4BB1-82F5-13611FFB59CF}" name="Feature" dataDxfId="247">
+    <tableColumn id="10" xr3:uid="{F503BC1B-7DB8-4002-ABF1-58ABE89E1830}" name="#" dataDxfId="215"/>
+    <tableColumn id="2" xr3:uid="{C571017F-6C16-4BB1-82F5-13611FFB59CF}" name="Feature" dataDxfId="214">
       <calculatedColumnFormula>VLOOKUP(Table156913141516[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{338C274F-0757-442C-A461-222ACF7CA161}" name="Scenario" dataDxfId="246">
+    <tableColumn id="3" xr3:uid="{338C274F-0757-442C-A461-222ACF7CA161}" name="Scenario" dataDxfId="213">
       <calculatedColumnFormula>VLOOKUP(Table156913141516[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C548F0C1-A750-457C-B904-D1F8B4782288}" name="Result" dataDxfId="245"/>
-    <tableColumn id="9" xr3:uid="{DB18A27F-42A0-4092-ABBD-7337C53F28D0}" name="Notes" dataDxfId="244"/>
-    <tableColumn id="4" xr3:uid="{D578B900-59BC-4A17-B895-07C1F3BA9A78}" name="Issue" dataDxfId="243"/>
+    <tableColumn id="7" xr3:uid="{C548F0C1-A750-457C-B904-D1F8B4782288}" name="Result" dataDxfId="212"/>
+    <tableColumn id="9" xr3:uid="{DB18A27F-42A0-4092-ABBD-7337C53F28D0}" name="Notes" dataDxfId="211"/>
+    <tableColumn id="4" xr3:uid="{D578B900-59BC-4A17-B895-07C1F3BA9A78}" name="Issue" dataDxfId="210"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6AAF2E7-A1F3-4605-8BF9-A1BF72A0A475}" name="Table1569131415" displayName="Table1569131415" ref="A1:G11" totalsRowShown="0" headerRowDxfId="242" dataDxfId="241">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B6AAF2E7-A1F3-4605-8BF9-A1BF72A0A475}" name="Table1569131415" displayName="Table1569131415" ref="A1:G11" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208">
   <autoFilter ref="A1:G11" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F2860C1F-2CAC-4F48-9D21-EE749371FC24}" name="GitHub Issue" dataDxfId="240">
+    <tableColumn id="1" xr3:uid="{F2860C1F-2CAC-4F48-9D21-EE749371FC24}" name="GitHub Issue" dataDxfId="207">
       <calculatedColumnFormula>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C5E95249-B8EB-486E-8767-21D8F0A0A62C}" name="#" dataDxfId="239"/>
-    <tableColumn id="2" xr3:uid="{3D03DEE9-A69F-4186-9544-A9E1591B8341}" name="Feature" dataDxfId="238">
+    <tableColumn id="10" xr3:uid="{C5E95249-B8EB-486E-8767-21D8F0A0A62C}" name="#" dataDxfId="206"/>
+    <tableColumn id="2" xr3:uid="{3D03DEE9-A69F-4186-9544-A9E1591B8341}" name="Feature" dataDxfId="205">
       <calculatedColumnFormula>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EBAA9733-8EE7-4AB7-AA6E-AD5B463DCCDB}" name="Scenario" dataDxfId="237">
+    <tableColumn id="3" xr3:uid="{EBAA9733-8EE7-4AB7-AA6E-AD5B463DCCDB}" name="Scenario" dataDxfId="204">
       <calculatedColumnFormula>VLOOKUP(Table1569131415[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B8D9077E-097D-43F7-AB61-3DC50B07F8DB}" name="Result" dataDxfId="236"/>
-    <tableColumn id="9" xr3:uid="{D33A8DD7-138F-48EF-8A7B-F7CF762853E4}" name="Notes" dataDxfId="235"/>
-    <tableColumn id="4" xr3:uid="{5957F9B4-6CFA-4A46-96FE-FA6B5AD2F680}" name="Issue" dataDxfId="234"/>
+    <tableColumn id="7" xr3:uid="{B8D9077E-097D-43F7-AB61-3DC50B07F8DB}" name="Result" dataDxfId="203"/>
+    <tableColumn id="9" xr3:uid="{D33A8DD7-138F-48EF-8A7B-F7CF762853E4}" name="Notes" dataDxfId="202"/>
+    <tableColumn id="4" xr3:uid="{5957F9B4-6CFA-4A46-96FE-FA6B5AD2F680}" name="Issue" dataDxfId="201"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{53B13E5C-5441-4B69-91E3-36B14A182343}" name="Table15691314" displayName="Table15691314" ref="A1:G75" totalsRowShown="0" headerRowDxfId="233" dataDxfId="232">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{53B13E5C-5441-4B69-91E3-36B14A182343}" name="Table15691314" displayName="Table15691314" ref="A1:G75" totalsRowShown="0" headerRowDxfId="200" dataDxfId="199">
   <autoFilter ref="A1:G75" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF78A628-9C38-4564-9808-3B26AF234F77}" name="GitHub Issue" dataDxfId="231">
+    <tableColumn id="1" xr3:uid="{AF78A628-9C38-4564-9808-3B26AF234F77}" name="GitHub Issue" dataDxfId="198">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2CAB733F-F4E3-4B07-84CB-D00849F9BD6C}" name="#" dataDxfId="230"/>
-    <tableColumn id="2" xr3:uid="{0F5DE106-934C-4581-BEC9-F2BED1604D9A}" name="Feature" dataDxfId="229">
+    <tableColumn id="10" xr3:uid="{2CAB733F-F4E3-4B07-84CB-D00849F9BD6C}" name="#" dataDxfId="197"/>
+    <tableColumn id="2" xr3:uid="{0F5DE106-934C-4581-BEC9-F2BED1604D9A}" name="Feature" dataDxfId="196">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{211378E0-438E-4FA5-A4AE-A66A0C3D748F}" name="Scenario" dataDxfId="228">
+    <tableColumn id="3" xr3:uid="{211378E0-438E-4FA5-A4AE-A66A0C3D748F}" name="Scenario" dataDxfId="195">
       <calculatedColumnFormula>VLOOKUP(Table15691314[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{932BD0E7-22E6-4F2C-8057-85843CDDFC76}" name="Result" dataDxfId="227"/>
-    <tableColumn id="9" xr3:uid="{E6B98784-DB78-486D-B5E1-8E879B6CB05A}" name="Notes" dataDxfId="226"/>
-    <tableColumn id="4" xr3:uid="{EF5B5B9D-C80C-4F4B-B547-BA970D46AED2}" name="Issue" dataDxfId="225"/>
+    <tableColumn id="7" xr3:uid="{932BD0E7-22E6-4F2C-8057-85843CDDFC76}" name="Result" dataDxfId="194"/>
+    <tableColumn id="9" xr3:uid="{E6B98784-DB78-486D-B5E1-8E879B6CB05A}" name="Notes" dataDxfId="193"/>
+    <tableColumn id="4" xr3:uid="{EF5B5B9D-C80C-4F4B-B547-BA970D46AED2}" name="Issue" dataDxfId="192"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="224" dataDxfId="223">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B3F603AC-EDFF-47AE-8B3E-0198F2732BD8}" name="Table156913" displayName="Table156913" ref="A1:H17" totalsRowShown="0" headerRowDxfId="191" dataDxfId="190">
   <autoFilter ref="A1:H17" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="222">
+    <tableColumn id="1" xr3:uid="{F049DD95-CBB6-4CF4-AECD-FFE9EFA9225F}" name="GitHub Issue" dataDxfId="189">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],11,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="221"/>
-    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="220">
+    <tableColumn id="10" xr3:uid="{3F1C7698-2293-4A2C-B7C0-4DBB6CF0E963}" name="#" dataDxfId="188"/>
+    <tableColumn id="2" xr3:uid="{095F1FFC-6CB5-40A3-BA57-56E07ECC5DFF}" name="Feature" dataDxfId="187">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="219">
+    <tableColumn id="3" xr3:uid="{92FC64C8-BA2C-4608-BABF-37803E5F32B7}" name="Scenario" dataDxfId="186">
       <calculatedColumnFormula>VLOOKUP(Table156913[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="218"/>
-    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="217"/>
-    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="216"/>
-    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="215"/>
+    <tableColumn id="7" xr3:uid="{D8859BCF-2778-4731-9B31-282100C936B6}" name="Result" dataDxfId="185"/>
+    <tableColumn id="9" xr3:uid="{1F12BDA7-6B5C-44A5-A019-FB17D08F7B57}" name="Notes" dataDxfId="184"/>
+    <tableColumn id="4" xr3:uid="{693E0BB4-2DC4-437F-9B72-7F30012CBE28}" name="Issue" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{EF7CB576-7161-4A79-9067-E1E6E50DE81A}" name="Issue 2" dataDxfId="182"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H20" totalsRowShown="0" headerRowDxfId="214" dataDxfId="213">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D86B072-B738-45B9-B991-A3DF4F258129}" name="Table1561012" displayName="Table1561012" ref="A1:H20" totalsRowShown="0" headerRowDxfId="181" dataDxfId="180">
   <autoFilter ref="A1:H20" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="212"/>
-    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="211"/>
-    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="210">
+    <tableColumn id="1" xr3:uid="{55E3B8C8-F10F-4605-A66E-73817D42A4AC}" name="GitHub Issue" dataDxfId="179"/>
+    <tableColumn id="10" xr3:uid="{1D01CD7E-CE7A-46E0-9094-E48EC4E812F7}" name="#" dataDxfId="178"/>
+    <tableColumn id="2" xr3:uid="{74EC06EB-7CBA-45ED-ADA4-37F743DBE530}" name="Feature" dataDxfId="177">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="209">
+    <tableColumn id="3" xr3:uid="{EAC8A485-DE32-4AB9-B5F0-48E78CE4B246}" name="Scenario" dataDxfId="176">
       <calculatedColumnFormula>VLOOKUP(Table1561012[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="208"/>
-    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="207"/>
-    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="206"/>
-    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="205"/>
+    <tableColumn id="7" xr3:uid="{BF2B6AC7-09A3-4E65-B760-CB091327A3AE}" name="Result" dataDxfId="175"/>
+    <tableColumn id="9" xr3:uid="{282C4C2A-2464-4CF7-9523-9A0CB7C7EE29}" name="Notes" dataDxfId="174"/>
+    <tableColumn id="4" xr3:uid="{C276B215-15EF-4B27-B0D5-0BE0D0B2907C}" name="Issue" dataDxfId="173"/>
+    <tableColumn id="5" xr3:uid="{529D0B5D-E5CF-4508-B52C-43B6A37D18CE}" name="Issue 2" dataDxfId="172"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="204" dataDxfId="203">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D434FA94-BA04-4027-BE83-B87EF2AF446C}" name="Table111" displayName="Table111" ref="A1:G7" totalsRowShown="0" headerRowDxfId="171" dataDxfId="170">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
     <sortCondition ref="B1:B7"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="202"/>
-    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="201"/>
-    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="200">
+    <tableColumn id="1" xr3:uid="{5DB71EFE-0BD0-4F57-B252-2F07EE896089}" name="GitHub Issue" dataDxfId="169"/>
+    <tableColumn id="10" xr3:uid="{952FB679-3CD2-4BAC-A972-B723C7656EBD}" name="#" dataDxfId="168"/>
+    <tableColumn id="2" xr3:uid="{0493B1AA-97DD-4AF0-884B-769757075C7E}" name="Feature" dataDxfId="167">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="199">
+    <tableColumn id="3" xr3:uid="{AF7D4B28-493E-4662-8260-00BC0726EB68}" name="Scenario" dataDxfId="166">
       <calculatedColumnFormula>VLOOKUP(Table111[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="198"/>
-    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="197"/>
-    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="196"/>
+    <tableColumn id="7" xr3:uid="{4A72ED44-050F-4EF5-876A-55D26D5DAF80}" name="Result" dataDxfId="165"/>
+    <tableColumn id="9" xr3:uid="{D44A7FF0-254A-482D-92E3-36D6B5CF3331}" name="Notes" dataDxfId="164"/>
+    <tableColumn id="4" xr3:uid="{986B8609-766C-4F17-B4FE-EE68B195D1CE}" name="Issue" dataDxfId="163"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4936,10 +4770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
-  <dimension ref="A1:K558"/>
+  <dimension ref="A1:K570"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C547" sqref="A547:XFD551"/>
+      <selection activeCell="F576" sqref="F576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -16510,7 +16344,7 @@
         <v>29</v>
       </c>
       <c r="H402" s="41" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="I402" s="70">
         <v>55</v>
@@ -16716,7 +16550,7 @@
         <v>29</v>
       </c>
       <c r="H409" s="41" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="I409" s="70">
         <v>73</v>
@@ -16921,7 +16755,7 @@
         <v>29</v>
       </c>
       <c r="H416" s="41" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="I416" s="70">
         <v>78</v>
@@ -16949,7 +16783,7 @@
         <v>29</v>
       </c>
       <c r="H417" s="41" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I417" s="70">
         <v>78</v>
@@ -17157,7 +16991,7 @@
         <v>29</v>
       </c>
       <c r="H424" s="41" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="I424" s="70">
         <v>79</v>
@@ -17187,7 +17021,7 @@
         <v>29</v>
       </c>
       <c r="H425" s="41" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I425" s="70">
         <v>79</v>
@@ -17255,7 +17089,7 @@
         <v>79</v>
       </c>
       <c r="J427" s="71" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K427" s="66">
         <v>38</v>
@@ -17287,7 +17121,7 @@
         <v>79</v>
       </c>
       <c r="J428" s="71" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K428" s="66">
         <v>38</v>
@@ -17319,7 +17153,7 @@
         <v>79</v>
       </c>
       <c r="J429" s="71" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K429" s="66">
         <v>38</v>
@@ -17931,7 +17765,7 @@
         <v>31</v>
       </c>
       <c r="H450" s="41" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="I450" s="70">
         <v>83</v>
@@ -18038,7 +17872,7 @@
         <v>29</v>
       </c>
       <c r="H454" s="2" t="s">
-        <v>386</v>
+        <v>429</v>
       </c>
       <c r="I454" s="70">
         <v>56</v>
@@ -18066,7 +17900,7 @@
         <v>30</v>
       </c>
       <c r="H455" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I455" s="70">
         <v>56</v>
@@ -18152,9 +17986,9 @@
       <c r="G458" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="H458" s="2" t="e">
-        <f>_xlfn.CONCAT("Result from scenario ",[1]!Table14[[#This Row],[Dependency]])</f>
-        <v>#REF!</v>
+      <c r="H458" s="2" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",Table14[[#This Row],[Dependency]])</f>
+        <v>Result from scenario 56</v>
       </c>
       <c r="I458" s="70">
         <v>57</v>
@@ -18214,7 +18048,7 @@
         <v>31</v>
       </c>
       <c r="H460" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I460" s="70">
         <v>57</v>
@@ -18270,9 +18104,9 @@
       <c r="G462" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="H462" s="2" t="e">
-        <f>_xlfn.CONCAT("Result from scenario ",[1]!Table14[[#This Row],[Dependency]])</f>
-        <v>#REF!</v>
+      <c r="H462" s="2" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",Table14[[#This Row],[Dependency]])</f>
+        <v>Result from scenario 57</v>
       </c>
       <c r="I462" s="70">
         <v>58</v>
@@ -18302,7 +18136,7 @@
         <v>30</v>
       </c>
       <c r="H463" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I463" s="70">
         <v>58</v>
@@ -18332,7 +18166,7 @@
         <v>31</v>
       </c>
       <c r="H464" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I464" s="70">
         <v>58</v>
@@ -18362,7 +18196,7 @@
         <v>31</v>
       </c>
       <c r="H465" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I465" s="70">
         <v>58</v>
@@ -18392,7 +18226,7 @@
         <v>31</v>
       </c>
       <c r="H466" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I466" s="70">
         <v>58</v>
@@ -18448,9 +18282,9 @@
       <c r="G468" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="H468" s="2" t="e">
-        <f>_xlfn.CONCAT("Result from scenario ",[1]!Table14[[#This Row],[Dependency]])</f>
-        <v>#REF!</v>
+      <c r="H468" s="2" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",Table14[[#This Row],[Dependency]])</f>
+        <v>Result from scenario 56</v>
       </c>
       <c r="I468" s="70">
         <v>59</v>
@@ -18566,9 +18400,9 @@
       <c r="G472" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="H472" s="2" t="e">
-        <f>_xlfn.CONCAT("Result from scenario ",[1]!Table14[[#This Row],[Dependency]])</f>
-        <v>#REF!</v>
+      <c r="H472" s="2" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",Table14[[#This Row],[Dependency]])</f>
+        <v>Result from scenario 57</v>
       </c>
       <c r="I472" s="70">
         <v>60</v>
@@ -18598,7 +18432,7 @@
         <v>30</v>
       </c>
       <c r="H473" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I473" s="70">
         <v>60</v>
@@ -18628,7 +18462,7 @@
         <v>31</v>
       </c>
       <c r="H474" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I474" s="70">
         <v>60</v>
@@ -18658,7 +18492,7 @@
         <v>31</v>
       </c>
       <c r="H475" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I475" s="70">
         <v>60</v>
@@ -18688,7 +18522,7 @@
         <v>31</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I476" s="70">
         <v>60</v>
@@ -18741,7 +18575,7 @@
         <v>29</v>
       </c>
       <c r="H478" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I478" s="70">
         <v>68</v>
@@ -18771,7 +18605,7 @@
         <v>29</v>
       </c>
       <c r="H479" s="2" t="s">
-        <v>401</v>
+        <v>431</v>
       </c>
       <c r="I479" s="70">
         <v>68</v>
@@ -18799,7 +18633,7 @@
         <v>29</v>
       </c>
       <c r="H480" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I480" s="70">
         <v>68</v>
@@ -18855,7 +18689,7 @@
         <v>30</v>
       </c>
       <c r="H482" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I482" s="70">
         <v>68</v>
@@ -18883,7 +18717,7 @@
         <v>31</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I483" s="70">
         <v>68</v>
@@ -18911,7 +18745,7 @@
         <v>31</v>
       </c>
       <c r="H484" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I484" s="70">
         <v>68</v>
@@ -18939,7 +18773,7 @@
         <v>31</v>
       </c>
       <c r="H485" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I485" s="70">
         <v>68</v>
@@ -18967,7 +18801,7 @@
         <v>31</v>
       </c>
       <c r="H486" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I486" s="70">
         <v>68</v>
@@ -19022,7 +18856,7 @@
         <v>29</v>
       </c>
       <c r="H488" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I488" s="70">
         <v>69</v>
@@ -19050,7 +18884,7 @@
         <v>29</v>
       </c>
       <c r="H489" s="2" t="s">
-        <v>401</v>
+        <v>431</v>
       </c>
       <c r="I489" s="70">
         <v>69</v>
@@ -19078,7 +18912,7 @@
         <v>29</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I490" s="70">
         <v>69</v>
@@ -19134,7 +18968,7 @@
         <v>29</v>
       </c>
       <c r="H492" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I492" s="70">
         <v>69</v>
@@ -19162,7 +18996,7 @@
         <v>123</v>
       </c>
       <c r="H493" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I493" s="70">
         <v>69</v>
@@ -19190,7 +19024,7 @@
         <v>31</v>
       </c>
       <c r="H494" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I494" s="70">
         <v>69</v>
@@ -19218,7 +19052,7 @@
         <v>31</v>
       </c>
       <c r="H495" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I495" s="70">
         <v>69</v>
@@ -19246,7 +19080,7 @@
         <v>31</v>
       </c>
       <c r="H496" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I496" s="70">
         <v>69</v>
@@ -19274,7 +19108,7 @@
         <v>31</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I497" s="70">
         <v>69</v>
@@ -19302,7 +19136,7 @@
         <v>31</v>
       </c>
       <c r="H498" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I498" s="70">
         <v>69</v>
@@ -19357,7 +19191,7 @@
         <v>29</v>
       </c>
       <c r="H500" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I500" s="70">
         <v>70</v>
@@ -19385,7 +19219,7 @@
         <v>29</v>
       </c>
       <c r="H501" s="2" t="s">
-        <v>401</v>
+        <v>431</v>
       </c>
       <c r="I501" s="70">
         <v>70</v>
@@ -19413,7 +19247,7 @@
         <v>29</v>
       </c>
       <c r="H502" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I502" s="70">
         <v>70</v>
@@ -19469,7 +19303,7 @@
         <v>29</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I504" s="70">
         <v>70</v>
@@ -19497,7 +19331,7 @@
         <v>123</v>
       </c>
       <c r="H505" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I505" s="70">
         <v>70</v>
@@ -19525,7 +19359,7 @@
         <v>31</v>
       </c>
       <c r="H506" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I506" s="70">
         <v>70</v>
@@ -19553,7 +19387,7 @@
         <v>31</v>
       </c>
       <c r="H507" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I507" s="70">
         <v>70</v>
@@ -19581,7 +19415,7 @@
         <v>31</v>
       </c>
       <c r="H508" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I508" s="70">
         <v>70</v>
@@ -19609,7 +19443,7 @@
         <v>31</v>
       </c>
       <c r="H509" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I509" s="70">
         <v>70</v>
@@ -19637,7 +19471,7 @@
         <v>31</v>
       </c>
       <c r="H510" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I510" s="70">
         <v>70</v>
@@ -19692,7 +19526,7 @@
         <v>29</v>
       </c>
       <c r="H512" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I512" s="70">
         <v>71</v>
@@ -19720,7 +19554,7 @@
         <v>29</v>
       </c>
       <c r="H513" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I513" s="70">
         <v>71</v>
@@ -19748,7 +19582,7 @@
         <v>29</v>
       </c>
       <c r="H514" s="2" t="s">
-        <v>401</v>
+        <v>431</v>
       </c>
       <c r="I514" s="70">
         <v>71</v>
@@ -19776,7 +19610,7 @@
         <v>29</v>
       </c>
       <c r="H515" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I515" s="70">
         <v>71</v>
@@ -19832,7 +19666,7 @@
         <v>31</v>
       </c>
       <c r="H517" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I517" s="70">
         <v>71</v>
@@ -19857,7 +19691,7 @@
       <c r="E518" s="68"/>
       <c r="F518" s="69"/>
       <c r="H518" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I518" s="70">
         <v>71</v>
@@ -19885,7 +19719,7 @@
         <v>31</v>
       </c>
       <c r="H519" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I519" s="70">
         <v>71</v>
@@ -19913,7 +19747,7 @@
         <v>31</v>
       </c>
       <c r="H520" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I520" s="70">
         <v>71</v>
@@ -19966,7 +19800,7 @@
         <v>29</v>
       </c>
       <c r="H522" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I522" s="70">
         <v>72</v>
@@ -19994,7 +19828,7 @@
         <v>29</v>
       </c>
       <c r="H523" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I523" s="70">
         <v>72</v>
@@ -20022,7 +19856,7 @@
         <v>29</v>
       </c>
       <c r="H524" s="2" t="s">
-        <v>401</v>
+        <v>431</v>
       </c>
       <c r="I524" s="70">
         <v>72</v>
@@ -20050,7 +19884,7 @@
         <v>29</v>
       </c>
       <c r="H525" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I525" s="70">
         <v>72</v>
@@ -20106,7 +19940,7 @@
         <v>31</v>
       </c>
       <c r="H527" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I527" s="70">
         <v>72</v>
@@ -20134,7 +19968,7 @@
         <v>31</v>
       </c>
       <c r="H528" s="2" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="I528" s="70">
         <v>72</v>
@@ -20162,7 +19996,7 @@
         <v>31</v>
       </c>
       <c r="H529" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="I529" s="70">
         <v>72</v>
@@ -20190,7 +20024,7 @@
         <v>31</v>
       </c>
       <c r="H530" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I530" s="70">
         <v>72</v>
@@ -20200,7 +20034,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="531" spans="1:11" s="16" customFormat="1" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:11" s="16" customFormat="1" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A531" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>0</v>
@@ -20415,7 +20249,7 @@
         <v>30</v>
       </c>
       <c r="H538" s="41" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I538" s="70">
         <v>86</v>
@@ -20445,7 +20279,7 @@
         <v>31</v>
       </c>
       <c r="H539" s="41" t="s">
-        <v>416</v>
+        <v>432</v>
       </c>
       <c r="I539" s="70">
         <v>86</v>
@@ -20475,7 +20309,7 @@
         <v>31</v>
       </c>
       <c r="H540" s="41" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I540" s="70">
         <v>86</v>
@@ -20501,7 +20335,7 @@
         <v>86</v>
       </c>
       <c r="F541" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G541" s="37"/>
       <c r="H541" s="41"/>
@@ -20564,7 +20398,7 @@
         <v>30</v>
       </c>
       <c r="H543" s="41" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I543" s="70">
         <v>95</v>
@@ -20596,7 +20430,7 @@
         <v>31</v>
       </c>
       <c r="H544" s="41" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="I544" s="70">
         <v>95</v>
@@ -20626,7 +20460,7 @@
         <v>31</v>
       </c>
       <c r="H545" s="41" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="I545" s="70">
         <v>95</v>
@@ -20650,7 +20484,7 @@
       <c r="D546" s="67"/>
       <c r="E546" s="68"/>
       <c r="F546" s="6" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G546" s="37"/>
       <c r="H546" s="41"/>
@@ -20720,7 +20554,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="549" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:11" ht="16.5" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A549" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>96</v>
@@ -20738,7 +20572,7 @@
         <v>30</v>
       </c>
       <c r="H549" s="41" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="I549" s="70">
         <v>96</v>
@@ -20766,7 +20600,7 @@
         <v>31</v>
       </c>
       <c r="H550" s="41" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="I550" s="70">
         <v>96</v>
@@ -20794,7 +20628,7 @@
         <v>31</v>
       </c>
       <c r="H551" s="41" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I551" s="70">
         <v>96</v>
@@ -20820,7 +20654,7 @@
         <v>96</v>
       </c>
       <c r="F552" s="6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G552" s="37"/>
       <c r="H552" s="41"/>
@@ -20874,7 +20708,9 @@
         <v>56</v>
       </c>
       <c r="D554" s="67"/>
-      <c r="E554" s="68"/>
+      <c r="E554" s="68">
+        <v>96</v>
+      </c>
       <c r="F554" s="6"/>
       <c r="G554" s="37" t="s">
         <v>29</v>
@@ -20892,7 +20728,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="555" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:11" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A555" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>97</v>
@@ -20912,7 +20748,7 @@
         <v>30</v>
       </c>
       <c r="H555" s="41" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="I555" s="70">
         <v>97</v>
@@ -20942,7 +20778,7 @@
         <v>31</v>
       </c>
       <c r="H556" s="41" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="I556" s="70">
         <v>97</v>
@@ -20952,7 +20788,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="557" spans="1:11" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:11" ht="60.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A557" s="64">
         <f>Table14[[#This Row],[Scenario '#]]</f>
         <v>97</v>
@@ -20972,7 +20808,7 @@
         <v>31</v>
       </c>
       <c r="H557" s="41" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="I557" s="70">
         <v>97</v>
@@ -20982,36 +20818,379 @@
         <v>61</v>
       </c>
     </row>
-    <row r="558" spans="1:11" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A558" s="61"/>
-      <c r="B558" s="1" t="s">
+    <row r="558" spans="1:11" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A558" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>0</v>
+      </c>
+      <c r="B558" s="121" t="s">
+        <v>422</v>
+      </c>
+      <c r="C558" s="122"/>
+      <c r="D558" s="123"/>
+      <c r="E558" s="124"/>
+      <c r="F558" s="125"/>
+      <c r="G558" s="126"/>
+      <c r="H558" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="I558" s="127"/>
+      <c r="J558" s="128" t="s">
+        <v>2</v>
+      </c>
+      <c r="K558" s="122">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="559" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A559" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>98</v>
+      </c>
+      <c r="B559" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C559" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D559" s="67"/>
+      <c r="E559" s="68"/>
+      <c r="F559" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="G559" s="31"/>
+      <c r="H559" s="41"/>
+      <c r="I559" s="70">
+        <v>98</v>
+      </c>
+      <c r="J559" s="71"/>
+      <c r="K559" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="560" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A560" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>98</v>
+      </c>
+      <c r="B560" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C560" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D560" s="67"/>
+      <c r="E560" s="68"/>
+      <c r="F560" s="17"/>
+      <c r="G560" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H560" s="41" t="s">
+        <v>382</v>
+      </c>
+      <c r="I560" s="70">
+        <v>98</v>
+      </c>
+      <c r="J560" s="43" t="s">
+        <v>423</v>
+      </c>
+      <c r="K560" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="561" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A561" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>98</v>
+      </c>
+      <c r="B561" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C561" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D561" s="67"/>
+      <c r="E561" s="68"/>
+      <c r="F561" s="17"/>
+      <c r="G561" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H561" s="41" t="s">
+        <v>428</v>
+      </c>
+      <c r="I561" s="70">
+        <v>98</v>
+      </c>
+      <c r="J561" s="43"/>
+      <c r="K561" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="562" spans="1:11" ht="30" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A562" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>98</v>
+      </c>
+      <c r="B562" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C562" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D562" s="67"/>
+      <c r="E562" s="68"/>
+      <c r="F562" s="17"/>
+      <c r="G562" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H562" s="41" t="s">
+        <v>424</v>
+      </c>
+      <c r="I562" s="70">
+        <v>98</v>
+      </c>
+      <c r="J562" s="71"/>
+      <c r="K562" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="563" spans="1:11" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A563" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>98</v>
+      </c>
+      <c r="B563" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C563" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D563" s="67"/>
+      <c r="E563" s="68"/>
+      <c r="F563" s="17"/>
+      <c r="G563" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H563" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="I563" s="70">
+        <v>98</v>
+      </c>
+      <c r="J563" s="71"/>
+      <c r="K563" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="564" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A564" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>99</v>
+      </c>
+      <c r="B564" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C564" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D564" s="67"/>
+      <c r="E564" s="68">
+        <v>98</v>
+      </c>
+      <c r="F564" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="G564" s="31"/>
+      <c r="H564" s="41"/>
+      <c r="I564" s="70">
+        <v>99</v>
+      </c>
+      <c r="J564" s="71"/>
+      <c r="K564" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="565" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A565" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>99</v>
+      </c>
+      <c r="B565" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C565" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D565" s="67"/>
+      <c r="E565" s="68">
+        <v>98</v>
+      </c>
+      <c r="F565" s="17"/>
+      <c r="G565" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H565" s="41" t="str">
+        <f>_xlfn.CONCAT("Result from scenario ",Table14[[#This Row],[Dependency]])</f>
+        <v>Result from scenario 98</v>
+      </c>
+      <c r="I565" s="70">
+        <v>99</v>
+      </c>
+      <c r="J565" s="71"/>
+      <c r="K565" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="566" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A566" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>99</v>
+      </c>
+      <c r="B566" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C566" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D566" s="67"/>
+      <c r="E566" s="68">
+        <v>98</v>
+      </c>
+      <c r="F566" s="17"/>
+      <c r="G566" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H566" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="I566" s="70">
+        <v>99</v>
+      </c>
+      <c r="J566" s="71"/>
+      <c r="K566" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="567" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A567" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>99</v>
+      </c>
+      <c r="B567" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C567" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D567" s="67"/>
+      <c r="E567" s="68">
+        <v>98</v>
+      </c>
+      <c r="F567" s="17"/>
+      <c r="G567" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H567" s="41" t="s">
+        <v>427</v>
+      </c>
+      <c r="I567" s="70">
+        <v>99</v>
+      </c>
+      <c r="J567" s="71"/>
+      <c r="K567" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="568" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A568" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>99</v>
+      </c>
+      <c r="B568" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C568" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D568" s="67"/>
+      <c r="E568" s="68">
+        <v>98</v>
+      </c>
+      <c r="F568" s="6"/>
+      <c r="G568" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H568" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="I568" s="70">
+        <v>99</v>
+      </c>
+      <c r="J568" s="71"/>
+      <c r="K568" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="569" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A569" s="64">
+        <f>Table14[[#This Row],[Scenario '#]]</f>
+        <v>99</v>
+      </c>
+      <c r="B569" s="65" t="s">
+        <v>422</v>
+      </c>
+      <c r="C569" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D569" s="67"/>
+      <c r="E569" s="68">
+        <v>98</v>
+      </c>
+      <c r="F569" s="6"/>
+      <c r="G569" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="H569" s="41" t="s">
+        <v>437</v>
+      </c>
+      <c r="I569" s="70">
+        <v>99</v>
+      </c>
+      <c r="J569" s="71"/>
+      <c r="K569" s="66">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="570" spans="1:11" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A570" s="61"/>
+      <c r="B570" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C558" s="3"/>
-      <c r="E558" s="10">
+      <c r="C570" s="3"/>
+      <c r="E570" s="10">
         <f>Table14[[#Totals],[Scenario '#]]</f>
         <v>63</v>
       </c>
-      <c r="F558" s="6"/>
-      <c r="H558" s="2"/>
-      <c r="I558" s="12">
+      <c r="F570" s="6"/>
+      <c r="H570" s="2"/>
+      <c r="I570" s="12">
         <f>SUBTOTAL(104,Table14[Scenario '#])</f>
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="75" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="108" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="74" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="107" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="colorScale" priority="170">
+    <cfRule type="colorScale" priority="176">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -21023,7 +21202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -21035,7 +21214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -21044,14 +21223,25 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="73" priority="9" operator="equal">
+  <conditionalFormatting sqref="G1:G563 G568:G1048576">
+    <cfRule type="cellIs" dxfId="58" priority="4" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G564:G567">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21172,13 +21362,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21375,13 +21565,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21593,13 +21783,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21724,13 +21914,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22994,13 +23184,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23508,13 +23698,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23939,24 +24129,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E20:E1048576 E1:E17">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E19">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24128,10 +24318,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Solved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24151,10 +24341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB6A8DF-4065-42B5-9CAC-CBAA6A687101}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25919,7 +26109,7 @@
       </c>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>61</v>
@@ -25940,7 +26130,7 @@
       </c>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>61</v>
@@ -25961,7 +26151,7 @@
       </c>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>61</v>
@@ -25985,7 +26175,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>61</v>
@@ -26007,7 +26197,7 @@
       <c r="F87" s="2"/>
       <c r="G87" s="87"/>
     </row>
-    <row r="88" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
         <v>61</v>
@@ -26029,30 +26219,78 @@
       <c r="F88" s="2"/>
       <c r="G88" s="87"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="B89" s="8">
+        <v>98</v>
+      </c>
+      <c r="C89" s="63" t="str">
+        <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Feature</v>
+      </c>
+      <c r="D89" s="63" t="str">
+        <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Remove Feature</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="2"/>
+      <c r="G89" s="87">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],11,FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="B90" s="8">
+        <v>99</v>
+      </c>
+      <c r="C90" s="63" t="str">
+        <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],2,FALSE)</f>
+        <v>Removing Feature</v>
+      </c>
+      <c r="D90" s="63" t="str">
+        <f>VLOOKUP(Table156913141718[[#This Row],['#]],Table14[],6,FALSE)</f>
+        <v>Remove Feature step 2a</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="2"/>
+      <c r="G90" s="87">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="8">
+      <c r="B91" s="8">
         <f>SUBTOTAL(104,Table156913141718['#])</f>
-        <v>97</v>
-      </c>
-      <c r="C89" s="1">
+        <v>99</v>
+      </c>
+      <c r="C91" s="1">
         <f>SUBTOTAL(103,Table156913141718[Feature])</f>
-        <v>5</v>
-      </c>
-      <c r="E89" s="1">
+        <v>2</v>
+      </c>
+      <c r="E91" s="1">
         <f>SUBTOTAL(103,Table156913141718[Result])</f>
-        <v>5</v>
-      </c>
-      <c r="F89" s="2"/>
-      <c r="G89" s="1">
+        <v>2</v>
+      </c>
+      <c r="F91" s="2"/>
+      <c r="G91" s="1">
         <f>SUBTOTAL(103,Table156913141718[Issue])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A90:A1048576 A1:A88">
+  <conditionalFormatting sqref="A92:A1048576 A1:A90">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -26064,14 +26302,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E88 E90:E1048576">
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+  <conditionalFormatting sqref="E1:E90 E92:E1048576">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26079,11 +26317,13 @@
     <hyperlink ref="G41" r:id="rId1" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/86" xr:uid="{36B320AC-D209-49F4-A645-3635696FF7B2}"/>
     <hyperlink ref="G44" r:id="rId2" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/86" xr:uid="{B1A1D832-7E06-4C28-8482-2A1E4FB23300}"/>
     <hyperlink ref="G86" r:id="rId3" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/87" xr:uid="{E8C69C73-B6E2-4B01-8FF4-1BB763B71D00}"/>
+    <hyperlink ref="G89" r:id="rId4" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/62" xr:uid="{07BC4F57-D48D-4466-9A5C-4893FCF174E2}"/>
+    <hyperlink ref="G90" r:id="rId5" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/62" xr:uid="{09063BDD-B0A7-4C6E-980E-83435CAD8F47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -26165,13 +26405,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="67" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26330,13 +26570,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="64" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26641,13 +26881,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="61" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26664,13 +26904,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28353,13 +28593,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="55" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28795,13 +29035,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29347,13 +29587,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29543,13 +29783,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#62 last tests passed
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F754C-0C97-4A93-82C5-320090D214FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3598A5-DD93-4D78-A92F-2F23AB712D3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="888" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="888" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="23" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="90" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="444">
   <si>
     <t>Scenario</t>
   </si>
@@ -1862,11 +1862,6 @@
   </si>
   <si>
     <t>Codeunit files containing FEATURE "Same Feature" is removed</t>
-  </si>
-  <si>
-    <t>Notes
-*  "Same Feature" is removed from Features pane in ATTD.TestScriptor page, so this is OK
-* But the related files are not removed and the test scenarios in it are still displayed in the TestScriptor pane</t>
   </si>
 </sst>
 </file>
@@ -2532,297 +2527,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2882,6 +2586,26 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2911,6 +2635,36 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2966,6 +2720,100 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2977,6 +2825,9 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2991,6 +2842,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3021,6 +2892,26 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3033,6 +2924,9 @@
       </font>
       <numFmt numFmtId="164" formatCode="0000"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3049,6 +2943,9 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -3056,6 +2953,25 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -3079,6 +2995,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <i/>
         <strike val="0"/>
         <outline val="0"/>
@@ -3091,6 +3027,9 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3108,6 +3047,9 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -3122,6 +3064,9 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -3134,6 +3079,15 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3172,6 +3126,47 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -13002,7 +12997,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{22E5CA79-C496-4575-8AF4-3B0E850079C1}" name="PivotTable2" cacheId="90" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{22E5CA79-C496-4575-8AF4-3B0E850079C1}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -13121,115 +13116,115 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:L622" totalsRowCount="1" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:L622" totalsRowCount="1" headerRowDxfId="91" dataDxfId="90">
   <autoFilter ref="A1:L621" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="94" totalsRowDxfId="18">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="89" totalsRowDxfId="88">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="93" totalsRowDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="92" totalsRowDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="91" totalsRowDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="90" totalsRowDxfId="14">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="80">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="89" totalsRowDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="88" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="87" totalsRowDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="86" totalsRowDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{7DDD814C-B9C8-4D4A-9C5D-71C8F05A4A7B}" name="Equals Scenario #" dataDxfId="85" totalsRowDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="84" totalsRowDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="83" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{7DDD814C-B9C8-4D4A-9C5D-71C8F05A4A7B}" name="Equals Scenario #" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="67" totalsRowDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73731A94-2591-485D-ADAB-6B0E2755AB81}" name="Table156913141718202" displayName="Table156913141718202" ref="A1:G8" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73731A94-2591-485D-ADAB-6B0E2755AB81}" name="Table156913141718202" displayName="Table156913141718202" ref="A1:G8" totalsRowCount="1" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:G7" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState ref="A2:G3">
     <sortCondition ref="A1:A3"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9CDBCCAA-B4BB-4D15-92EA-2D699DFCCD0A}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{9CDBCCAA-B4BB-4D15-92EA-2D699DFCCD0A}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="60" totalsRowDxfId="6">
       <calculatedColumnFormula>VLOOKUP(Table156913141718202[[#This Row],['#]],Table14[],12,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{29A4A28F-C35B-4074-AB25-9D19C79E081E}" name="#" totalsRowLabel="0101" dataDxfId="40" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{91BC586B-5227-4D70-9FFF-F4416722E348}" name="Feature" totalsRowFunction="count" dataDxfId="39" totalsRowDxfId="4">
+    <tableColumn id="10" xr3:uid="{29A4A28F-C35B-4074-AB25-9D19C79E081E}" name="#" totalsRowLabel="0101" dataDxfId="59" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{91BC586B-5227-4D70-9FFF-F4416722E348}" name="Feature" totalsRowFunction="count" dataDxfId="58" totalsRowDxfId="4">
       <calculatedColumnFormula>VLOOKUP(Table156913141718202[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A3988237-C6D4-4C80-AC26-406D5703BDB6}" name="Scenario" dataDxfId="38" totalsRowDxfId="3">
+    <tableColumn id="3" xr3:uid="{A3988237-C6D4-4C80-AC26-406D5703BDB6}" name="Scenario" dataDxfId="57" totalsRowDxfId="3">
       <calculatedColumnFormula>VLOOKUP(Table156913141718202[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1CD84B03-BCCF-48E0-A1DA-06FFA61642D7}" name="Result" totalsRowFunction="count" dataDxfId="37" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6CEC1C14-1D0C-4594-A34A-80FB746DF386}" name="Notes" dataDxfId="36" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{FB643267-7515-4F8D-A93B-5692DA2D707D}" name="Issue" totalsRowFunction="count" dataDxfId="35" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{1CD84B03-BCCF-48E0-A1DA-06FFA61642D7}" name="Result" totalsRowFunction="count" dataDxfId="56" totalsRowDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6CEC1C14-1D0C-4594-A34A-80FB746DF386}" name="Notes" dataDxfId="55" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FB643267-7515-4F8D-A93B-5692DA2D707D}" name="Issue" totalsRowFunction="count" dataDxfId="54" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{FFB2FDC9-C46F-4D61-B75B-E0C27DCB3F81}" name="Table1569131417181922" displayName="Table1569131417181922" ref="A1:G5" totalsRowCount="1" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{FFB2FDC9-C46F-4D61-B75B-E0C27DCB3F81}" name="Table1569131417181922" displayName="Table1569131417181922" ref="A1:G5" totalsRowCount="1" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:G4" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState ref="A2:G4">
     <sortCondition ref="A1:A4"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{76E8B066-259D-4FD4-890F-30A4D28DDA21}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="80" totalsRowDxfId="79">
+    <tableColumn id="1" xr3:uid="{76E8B066-259D-4FD4-890F-30A4D28DDA21}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="48" totalsRowDxfId="47">
       <calculatedColumnFormula>VLOOKUP(Table1569131417181922[[#This Row],['#]],Table14[],12,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A71FD1BB-EE40-4FC5-9C87-A4C969F58623}" name="#" totalsRowLabel="0101" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{8758245D-5463-4647-9D67-5069622B7403}" name="Feature" totalsRowFunction="count" dataDxfId="76" totalsRowDxfId="75">
+    <tableColumn id="10" xr3:uid="{A71FD1BB-EE40-4FC5-9C87-A4C969F58623}" name="#" totalsRowLabel="0101" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{8758245D-5463-4647-9D67-5069622B7403}" name="Feature" totalsRowFunction="count" dataDxfId="44" totalsRowDxfId="43">
       <calculatedColumnFormula>VLOOKUP(Table1569131417181922[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{96FAE6B8-EACB-44D8-984E-71F58CF30956}" name="Scenario" dataDxfId="74" totalsRowDxfId="73">
+    <tableColumn id="3" xr3:uid="{96FAE6B8-EACB-44D8-984E-71F58CF30956}" name="Scenario" dataDxfId="42" totalsRowDxfId="41">
       <calculatedColumnFormula>VLOOKUP(Table1569131417181922[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{191F6F0B-F0C8-4FE4-A087-32F80D21AE19}" name="Result" totalsRowFunction="count" dataDxfId="72" totalsRowDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{32D9487A-18A4-42F7-980A-E41559E81EF4}" name="Notes" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{8A9CA2C8-EC80-4AAB-B86F-49D461EA9A76}" name="Issue" totalsRowFunction="count" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{191F6F0B-F0C8-4FE4-A087-32F80D21AE19}" name="Result" totalsRowFunction="count" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{32D9487A-18A4-42F7-980A-E41559E81EF4}" name="Notes" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{8A9CA2C8-EC80-4AAB-B86F-49D461EA9A76}" name="Issue" totalsRowFunction="count" dataDxfId="36" totalsRowDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EF97CF47-DA9F-44A0-9086-E7AB4767E05F}" name="Table15691314171820" displayName="Table15691314171820" ref="A1:G20" totalsRowCount="1" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EF97CF47-DA9F-44A0-9086-E7AB4767E05F}" name="Table15691314171820" displayName="Table15691314171820" ref="A1:G20" totalsRowCount="1" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:G19" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <sortState ref="A2:G12">
     <sortCondition ref="A1:A12"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{58C024A2-6E76-44B9-A162-A9CBABA5B93B}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="64" totalsRowDxfId="50">
+    <tableColumn id="1" xr3:uid="{58C024A2-6E76-44B9-A162-A9CBABA5B93B}" name="GitHub Issue" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="13">
       <calculatedColumnFormula>VLOOKUP(Table15691314171820[[#This Row],['#]],Table14[],12,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{20998797-515A-4AA2-B8FB-85833DFF0ED0}" name="#" totalsRowLabel="0101" dataDxfId="63" totalsRowDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{C02F5D4B-8535-441B-A029-18F02F4F23AF}" name="Feature" totalsRowFunction="count" dataDxfId="62" totalsRowDxfId="48">
+    <tableColumn id="10" xr3:uid="{20998797-515A-4AA2-B8FB-85833DFF0ED0}" name="#" totalsRowLabel="0101" dataDxfId="28" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{C02F5D4B-8535-441B-A029-18F02F4F23AF}" name="Feature" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="11">
       <calculatedColumnFormula>VLOOKUP(Table15691314171820[[#This Row],['#]],Table14[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1C5B3407-A686-4B72-B6FD-80560E377E67}" name="Scenario" dataDxfId="61" totalsRowDxfId="47">
+    <tableColumn id="3" xr3:uid="{1C5B3407-A686-4B72-B6FD-80560E377E67}" name="Scenario" dataDxfId="26" totalsRowDxfId="10">
       <calculatedColumnFormula>VLOOKUP(Table15691314171820[[#This Row],['#]],Table14[],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{09DF1135-5480-4E04-BC95-F376428BE24E}" name="Result" totalsRowFunction="count" dataDxfId="60" totalsRowDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{EEA2061E-82D6-4A37-B7A2-CEFD28C8E098}" name="Notes" dataDxfId="59" totalsRowDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{2693F482-249A-461E-A08C-7C43041F6A13}" name="Issue" totalsRowFunction="count" dataDxfId="58" totalsRowDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{09DF1135-5480-4E04-BC95-F376428BE24E}" name="Result" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{EEA2061E-82D6-4A37-B7A2-CEFD28C8E098}" name="Notes" dataDxfId="24" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{2693F482-249A-461E-A08C-7C43041F6A13}" name="Issue" totalsRowFunction="count" dataDxfId="23" totalsRowDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="A1:F7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -32229,12 +32224,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="34" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="33" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="107" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32261,13 +32256,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32284,7 +32279,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32431,7 +32426,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="87"/>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>VLOOKUP(Table156913141718202[[#This Row],['#]],Table14[],12,FALSE)</f>
         <v>62</v>
@@ -32448,14 +32443,10 @@
         <v>Remove Feature (two in two codeunits) step 2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="G7" s="87">
-        <v>62</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="87"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -32475,7 +32466,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="1">
         <f>SUBTOTAL(103,Table156913141718202[Issue])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -32492,23 +32483,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E1048576 E1:E7">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" display="https://github.com/fluxxus-nl/ATDD.TestScriptor.VSCodeExtension/issues/62" xr:uid="{0F6BA178-889A-4DAC-9FF0-C05900E6726D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -32656,13 +32644,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E1048576 E1:E4">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33141,13 +33129,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:E1048576 E1:E19">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33311,10 +33299,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Solved"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated questions status #114
</commit_message>
<xml_diff>
--- a/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
+++ b/test/test-scenarios/atdd-test-scenarios-and-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\ATDD.TestScriptor.VSCodeExtension\test\test-scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3565354-97A9-488C-B8E1-E08D70DD8719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3ED500-B73C-4EBB-B402-8435E2928C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="285" windowWidth="24120" windowHeight="15990" tabRatio="566" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="566" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="23" r:id="rId1"/>
@@ -2588,14 +2588,20 @@
   </cellStyles>
   <dxfs count="52">
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2605,167 +2611,18 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF000000"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2818,41 +2675,37 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2869,6 +2722,9 @@
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2881,6 +2737,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2911,6 +2787,26 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2923,6 +2819,9 @@
       </font>
       <numFmt numFmtId="164" formatCode="0000"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2939,6 +2838,9 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2946,6 +2848,25 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2969,6 +2890,26 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <i/>
         <strike val="0"/>
         <outline val="0"/>
@@ -2981,6 +2922,9 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2998,6 +2942,9 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -3012,6 +2959,9 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -3024,6 +2974,15 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3062,6 +3021,47 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -13052,32 +13052,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:L623" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF4D00C3-E1B1-43AF-B727-CD24E93B89EC}" name="Table14" displayName="Table14" ref="A1:L623" totalsRowCount="1" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:L622" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="49" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{126DDE30-F6FC-4FDE-AF87-9CE1B3F05533}" name="Column1" dataDxfId="44" totalsRowDxfId="43">
       <calculatedColumnFormula>Table14[[#This Row],[Scenario '#]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="48" totalsRowDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="47" totalsRowDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="46" totalsRowDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="7">
+    <tableColumn id="2" xr3:uid="{B104394B-17C0-4DEE-B32E-F93702CD36E1}" name="Feature" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{DBB88613-266C-43B5-8498-BC6FAEA286C9}" name="UI" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{34C6255A-5D6C-4161-875E-2F88A1085F27}" name="Positive-negative" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="15" xr3:uid="{D1D1554E-D467-4545-807F-9757B09275F6}" name="Dependency" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="35">
       <totalsRowFormula>Table14[[#Totals],[Scenario '#]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="44" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="43" totalsRowDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="42" totalsRowDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="41" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7DDD814C-B9C8-4D4A-9C5D-71C8F05A4A7B}" name="Equals Scenario #" dataDxfId="40" totalsRowDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="39" totalsRowDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="38" totalsRowDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{B9AC3CF9-58E6-40C0-9390-315FF89C7419}" name="Scenario" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{88C23544-A804-4166-8DF0-93133B3A67AF}" name="Given-When-Then (Tag)" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{5AC48A9D-3D8E-4B1E-A0F2-F29BD8E1D734}" name="Given-When-Then (Description)" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{74BFFA9E-D38E-4B06-A503-1135EB85A785}" name="Scenario #" totalsRowFunction="max" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{7DDD814C-B9C8-4D4A-9C5D-71C8F05A4A7B}" name="Equals Scenario #" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{3136E83F-8489-460E-A005-8E1B7EEBC026}" name="Notes" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{B206D1D6-F293-4319-BF64-E77AFD6CFF38}" name="GitHub Issue" dataDxfId="22" totalsRowDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A2692945-AD2D-4521-9F79-85E4A11E13DE}" name="Table1" displayName="Table1" ref="A1:G106" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A2692945-AD2D-4521-9F79-85E4A11E13DE}" name="Table1" displayName="Table1" ref="A1:G106" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:G106" xr:uid="{F8344284-47AF-49AF-9E64-E03BD9F00473}">
     <filterColumn colId="0">
       <filters>
@@ -13097,34 +13097,34 @@
     <sortCondition ref="A1:A106"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9DBFC768-5222-479B-9A3E-F76FAF3C9995}" name="GitHub Issue" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{9DBFC768-5222-479B-9A3E-F76FAF3C9995}" name="GitHub Issue" dataDxfId="15">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[#Data],12,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3F962CFD-CBDD-4F5C-BBE0-374FF1D50983}" name="#" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{94075763-A0E0-42CE-9EB1-001FC7BD72E1}" name="Feature" dataDxfId="26">
+    <tableColumn id="10" xr3:uid="{3F962CFD-CBDD-4F5C-BBE0-374FF1D50983}" name="#" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{94075763-A0E0-42CE-9EB1-001FC7BD72E1}" name="Feature" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[#Data],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8C78C923-35FB-41BC-A270-42E426593B5F}" name="Scenario" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{8C78C923-35FB-41BC-A270-42E426593B5F}" name="Scenario" dataDxfId="12">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],['#]],Table14[#Data],6,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EB3314D7-BA03-43B1-A101-31FDDAD83F09}" name="Result" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{FFD54D52-F546-4C7F-A7A9-BB65F0C53FFA}" name="Notes" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{EC2E4889-B5C7-4301-8505-C161E283A66B}" name="Issue" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{EB3314D7-BA03-43B1-A101-31FDDAD83F09}" name="Result" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{FFD54D52-F546-4C7F-A7A9-BB65F0C53FFA}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{EC2E4889-B5C7-4301-8505-C161E283A66B}" name="Issue" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9A9E1B84-D3AD-4457-93D0-E02565E417A9}" name="Table2" displayName="Table2" ref="A1:F7" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F7" xr:uid="{EB128BE2-39AB-4779-BE48-2D3090EF510B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{809A052F-4CCE-4265-8EE0-6469B69CF4E9}" name="#" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{393EFC23-0E09-457A-8852-347692957937}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8B34BA27-BE68-42A9-BE23-4517F07BA6FB}" name="Question" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{C8D65C97-0725-439B-8696-77108772192A}" name="Answer" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{74BF07AF-988A-4911-BCBB-A2660AF07C56}" name="GitHub Issue" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B6E42313-0DE8-4118-818A-72DE4F7F4231}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13554,7 +13554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834A1FB-B3FD-4E72-A531-171E1058A77F}">
   <dimension ref="A1:L623"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B430" sqref="B430"/>
     </sheetView>
   </sheetViews>
@@ -32155,12 +32155,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="21" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="108" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="20" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="107" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32187,13 +32187,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34389,13 +34389,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34419,8 +34419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB16863-C9D6-47DE-82AF-06BDE2CF5BC1}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34520,7 +34520,7 @@
         <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -34563,10 +34563,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Solved"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>